<commit_message>
Dragon Egg - my best attempt at matching the previous publication.  50 frames slow after exiting the shop
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -1940,6 +1940,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1961,29 +1964,29 @@
     <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2019,20 +2022,34 @@
     <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2041,23 +2058,6 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2377,7 +2377,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2393,16 +2393,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="155" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="154"/>
+      <c r="C1" s="156" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="157"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
@@ -2480,10 +2480,10 @@
       <c r="B5" s="147" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2499,10 +2499,10 @@
       <c r="B6" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="153" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="153"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2520,7 +2520,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="158" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2540,7 +2540,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="150"/>
+      <c r="A9" s="151"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="150"/>
+      <c r="A10" s="151"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
+      <c r="A11" s="151"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
+      <c r="A12" s="151"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2605,7 +2605,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2616,7 +2616,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2627,7 +2627,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="148" t="s">
         <v>186</v>
       </c>
@@ -2644,7 +2644,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="150"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="152" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2707,7 +2707,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="150"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
@@ -2724,7 +2724,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="148" t="s">
         <v>218</v>
       </c>
@@ -2741,19 +2741,19 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
+      <c r="A22" s="151"/>
       <c r="B22" s="148" t="s">
         <v>219</v>
       </c>
       <c r="C22" s="101">
-        <v>1438</v>
+        <v>1466</v>
       </c>
       <c r="D22" s="101">
         <v>1418</v>
       </c>
       <c r="E22" s="123">
         <f t="shared" si="1"/>
-        <v>-20</v>
+        <v>-48</v>
       </c>
       <c r="F22" s="105"/>
       <c r="H22" t="s">
@@ -2764,19 +2764,19 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="213" t="s">
+      <c r="A23" s="151"/>
+      <c r="B23" s="149" t="s">
         <v>226</v>
       </c>
       <c r="C23" s="101">
-        <v>1574</v>
+        <v>1605</v>
       </c>
       <c r="D23" s="101">
         <v>1555</v>
       </c>
       <c r="E23" s="123">
         <f t="shared" si="1"/>
-        <v>-19</v>
+        <v>-50</v>
       </c>
       <c r="F23" s="105"/>
       <c r="J23" t="s">
@@ -2784,7 +2784,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
+      <c r="A24" s="151"/>
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
+      <c r="A25" s="151"/>
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="150"/>
+      <c r="A26" s="151"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2832,7 +2832,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="150"/>
+      <c r="A27" s="151"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2843,7 +2843,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="150"/>
+      <c r="A28" s="151"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2854,7 +2854,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="150"/>
+      <c r="A29" s="151"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2865,7 +2865,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="150"/>
+      <c r="A30" s="151"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2876,7 +2876,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
+      <c r="A31" s="151"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2887,7 +2887,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150"/>
+      <c r="A32" s="151"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2898,7 +2898,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
       </c>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="149" t="s">
+      <c r="A36" s="150" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="150"/>
+      <c r="A37" s="151"/>
       <c r="B37" s="98" t="s">
         <v>184</v>
       </c>
@@ -2970,7 +2970,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
+      <c r="A38" s="151"/>
       <c r="B38" s="100"/>
       <c r="C38" s="101"/>
       <c r="D38" s="101"/>
@@ -2981,7 +2981,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150"/>
+      <c r="A39" s="151"/>
       <c r="B39" s="100"/>
       <c r="C39" s="101"/>
       <c r="D39" s="101"/>
@@ -2992,7 +2992,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
+      <c r="A40" s="151"/>
       <c r="B40" s="100"/>
       <c r="C40" s="101"/>
       <c r="D40" s="101"/>
@@ -3003,7 +3003,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="150"/>
+      <c r="A41" s="151"/>
       <c r="B41" s="100"/>
       <c r="C41" s="101"/>
       <c r="D41" s="101"/>
@@ -3014,7 +3014,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150"/>
+      <c r="A42" s="151"/>
       <c r="B42" s="100"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -3025,7 +3025,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="150"/>
+      <c r="A43" s="151"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3036,7 +3036,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
+      <c r="A44" s="151"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3047,7 +3047,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="150"/>
+      <c r="A45" s="151"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3058,7 +3058,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="150"/>
+      <c r="A46" s="151"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3069,7 +3069,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="150"/>
+      <c r="A47" s="151"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3080,7 +3080,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="150"/>
+      <c r="A48" s="151"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3091,7 +3091,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="150"/>
+      <c r="A49" s="151"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3102,7 +3102,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="150"/>
+      <c r="A50" s="151"/>
       <c r="B50" s="98" t="s">
         <v>187</v>
       </c>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="151" t="s">
+      <c r="A53" s="152" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="150"/>
+      <c r="A54" s="151"/>
       <c r="B54" s="98" t="s">
         <v>184</v>
       </c>
@@ -3174,7 +3174,7 @@
       <c r="F54" s="104"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="150"/>
+      <c r="A55" s="151"/>
       <c r="B55" s="100"/>
       <c r="C55" s="101"/>
       <c r="D55" s="101"/>
@@ -3185,7 +3185,7 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="150"/>
+      <c r="A56" s="151"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3196,7 +3196,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="150"/>
+      <c r="A57" s="151"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3207,7 +3207,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="150"/>
+      <c r="A58" s="151"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3218,7 +3218,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="150"/>
+      <c r="A59" s="151"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3229,7 +3229,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="150"/>
+      <c r="A60" s="151"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3240,7 +3240,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="150"/>
+      <c r="A61" s="151"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3251,7 +3251,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="150"/>
+      <c r="A62" s="151"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3262,7 +3262,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="150"/>
+      <c r="A63" s="151"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3273,7 +3273,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="150"/>
+      <c r="A64" s="151"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3284,7 +3284,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="150"/>
+      <c r="A65" s="151"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3295,7 +3295,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="150"/>
+      <c r="A66" s="151"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3306,7 +3306,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="150"/>
+      <c r="A67" s="151"/>
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="149" t="s">
+      <c r="A70" s="150" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3365,7 +3365,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="150"/>
+      <c r="A71" s="151"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="150"/>
+      <c r="A72" s="151"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3389,7 +3389,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="150"/>
+      <c r="A73" s="151"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3400,7 +3400,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="150"/>
+      <c r="A74" s="151"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3411,7 +3411,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="150"/>
+      <c r="A75" s="151"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3422,7 +3422,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="150"/>
+      <c r="A76" s="151"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3433,7 +3433,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="150"/>
+      <c r="A77" s="151"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3444,7 +3444,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="150"/>
+      <c r="A78" s="151"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3455,7 +3455,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="150"/>
+      <c r="A79" s="151"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3466,7 +3466,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="150"/>
+      <c r="A80" s="151"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3477,7 +3477,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="150"/>
+      <c r="A81" s="151"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3488,7 +3488,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="150"/>
+      <c r="A82" s="151"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3499,7 +3499,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="150"/>
+      <c r="A83" s="151"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3510,7 +3510,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="150"/>
+      <c r="A84" s="151"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
@@ -3548,7 +3548,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="151" t="s">
+      <c r="A87" s="152" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3568,7 +3568,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="150"/>
+      <c r="A88" s="151"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="150"/>
+      <c r="A89" s="151"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3592,7 +3592,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="150"/>
+      <c r="A90" s="151"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3603,7 +3603,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="150"/>
+      <c r="A91" s="151"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3614,7 +3614,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="150"/>
+      <c r="A92" s="151"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3625,7 +3625,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="150"/>
+      <c r="A93" s="151"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3636,7 +3636,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="150"/>
+      <c r="A94" s="151"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3647,7 +3647,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="150"/>
+      <c r="A95" s="151"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3658,7 +3658,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="150"/>
+      <c r="A96" s="151"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3669,7 +3669,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="150"/>
+      <c r="A97" s="151"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3680,7 +3680,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="150"/>
+      <c r="A98" s="151"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3691,7 +3691,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="150"/>
+      <c r="A99" s="151"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3702,7 +3702,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="150"/>
+      <c r="A100" s="151"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3713,7 +3713,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="150"/>
+      <c r="A101" s="151"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
       </c>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="149" t="s">
+      <c r="A103" s="150" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="113" t="s">
@@ -3747,7 +3747,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="150"/>
+      <c r="A104" s="151"/>
       <c r="B104" s="98" t="s">
         <v>184</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="F104" s="104"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="150"/>
+      <c r="A105" s="151"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3771,7 +3771,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="150"/>
+      <c r="A106" s="151"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3782,7 +3782,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="150"/>
+      <c r="A107" s="151"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3793,7 +3793,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="150"/>
+      <c r="A108" s="151"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3804,7 +3804,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="150"/>
+      <c r="A109" s="151"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3815,7 +3815,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="150"/>
+      <c r="A110" s="151"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3826,7 +3826,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="150"/>
+      <c r="A111" s="151"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3837,7 +3837,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="150"/>
+      <c r="A112" s="151"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3848,7 +3848,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="150"/>
+      <c r="A113" s="151"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3859,7 +3859,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="150"/>
+      <c r="A114" s="151"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3870,7 +3870,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="150"/>
+      <c r="A115" s="151"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3881,7 +3881,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="150"/>
+      <c r="A116" s="151"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3892,7 +3892,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="150"/>
+      <c r="A117" s="151"/>
       <c r="B117" s="98" t="s">
         <v>187</v>
       </c>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="118" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="119" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="151" t="s">
+      <c r="A119" s="152" t="s">
         <v>175</v>
       </c>
       <c r="B119" s="109" t="s">
@@ -3926,7 +3926,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="150"/>
+      <c r="A120" s="151"/>
       <c r="B120" s="98" t="s">
         <v>184</v>
       </c>
@@ -3939,7 +3939,7 @@
       <c r="F120" s="104"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="150"/>
+      <c r="A121" s="151"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -3950,7 +3950,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="150"/>
+      <c r="A122" s="151"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -3961,7 +3961,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="150"/>
+      <c r="A123" s="151"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -3972,7 +3972,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="150"/>
+      <c r="A124" s="151"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -3983,7 +3983,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="150"/>
+      <c r="A125" s="151"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -3994,7 +3994,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="150"/>
+      <c r="A126" s="151"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4005,7 +4005,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="150"/>
+      <c r="A127" s="151"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4016,7 +4016,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="150"/>
+      <c r="A128" s="151"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4027,7 +4027,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="150"/>
+      <c r="A129" s="151"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4038,7 +4038,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="150"/>
+      <c r="A130" s="151"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4049,7 +4049,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="150"/>
+      <c r="A131" s="151"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4060,7 +4060,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="150"/>
+      <c r="A132" s="151"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4071,7 +4071,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="150"/>
+      <c r="A133" s="151"/>
       <c r="B133" s="98" t="s">
         <v>187</v>
       </c>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A135" s="149" t="s">
+      <c r="A135" s="150" t="s">
         <v>176</v>
       </c>
       <c r="B135" s="113" t="s">
@@ -4105,7 +4105,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="150"/>
+      <c r="A136" s="151"/>
       <c r="B136" s="98" t="s">
         <v>184</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="F136" s="104"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="150"/>
+      <c r="A137" s="151"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4129,7 +4129,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A138" s="150"/>
+      <c r="A138" s="151"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4140,7 +4140,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A139" s="150"/>
+      <c r="A139" s="151"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4151,7 +4151,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A140" s="150"/>
+      <c r="A140" s="151"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4162,7 +4162,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A141" s="150"/>
+      <c r="A141" s="151"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4173,7 +4173,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="150"/>
+      <c r="A142" s="151"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4184,7 +4184,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A143" s="150"/>
+      <c r="A143" s="151"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4195,7 +4195,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="150"/>
+      <c r="A144" s="151"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4206,7 +4206,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="150"/>
+      <c r="A145" s="151"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4217,7 +4217,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="150"/>
+      <c r="A146" s="151"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4228,7 +4228,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="150"/>
+      <c r="A147" s="151"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4239,7 +4239,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="150"/>
+      <c r="A148" s="151"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4250,7 +4250,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="150"/>
+      <c r="A149" s="151"/>
       <c r="B149" s="98" t="s">
         <v>187</v>
       </c>
@@ -4265,6 +4265,11 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4273,11 +4278,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4309,13 +4309,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4345,18 +4345,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4508,9 +4508,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="161"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="165"/>
+      <c r="E21" s="165"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4661,9 +4661,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="158"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4814,9 +4814,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="158"/>
-      <c r="D55" s="159"/>
-      <c r="E55" s="159"/>
+      <c r="C55" s="162"/>
+      <c r="D55" s="163"/>
+      <c r="E55" s="163"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -4967,9 +4967,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="158"/>
-      <c r="D72" s="159"/>
-      <c r="E72" s="159"/>
+      <c r="C72" s="162"/>
+      <c r="D72" s="163"/>
+      <c r="E72" s="163"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5120,9 +5120,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="158"/>
-      <c r="D89" s="159"/>
-      <c r="E89" s="159"/>
+      <c r="C89" s="162"/>
+      <c r="D89" s="163"/>
+      <c r="E89" s="163"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5273,9 +5273,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="158"/>
-      <c r="D106" s="159"/>
-      <c r="E106" s="159"/>
+      <c r="C106" s="162"/>
+      <c r="D106" s="163"/>
+      <c r="E106" s="163"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5426,9 +5426,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="158"/>
-      <c r="D123" s="159"/>
-      <c r="E123" s="159"/>
+      <c r="C123" s="162"/>
+      <c r="D123" s="163"/>
+      <c r="E123" s="163"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5579,9 +5579,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="158"/>
-      <c r="D140" s="159"/>
-      <c r="E140" s="159"/>
+      <c r="C140" s="162"/>
+      <c r="D140" s="163"/>
+      <c r="E140" s="163"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5732,9 +5732,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="158"/>
-      <c r="D157" s="159"/>
-      <c r="E157" s="159"/>
+      <c r="C157" s="162"/>
+      <c r="D157" s="163"/>
+      <c r="E157" s="163"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5885,9 +5885,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="158"/>
-      <c r="D174" s="159"/>
-      <c r="E174" s="159"/>
+      <c r="C174" s="162"/>
+      <c r="D174" s="163"/>
+      <c r="E174" s="163"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6038,9 +6038,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="158"/>
-      <c r="D191" s="159"/>
-      <c r="E191" s="159"/>
+      <c r="C191" s="162"/>
+      <c r="D191" s="163"/>
+      <c r="E191" s="163"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6191,9 +6191,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="158"/>
-      <c r="D208" s="159"/>
-      <c r="E208" s="159"/>
+      <c r="C208" s="162"/>
+      <c r="D208" s="163"/>
+      <c r="E208" s="163"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6344,9 +6344,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="158"/>
-      <c r="D225" s="159"/>
-      <c r="E225" s="159"/>
+      <c r="C225" s="162"/>
+      <c r="D225" s="163"/>
+      <c r="E225" s="163"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6497,9 +6497,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="158"/>
-      <c r="D242" s="159"/>
-      <c r="E242" s="159"/>
+      <c r="C242" s="162"/>
+      <c r="D242" s="163"/>
+      <c r="E242" s="163"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6650,9 +6650,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="158"/>
-      <c r="D259" s="159"/>
-      <c r="E259" s="159"/>
+      <c r="C259" s="162"/>
+      <c r="D259" s="163"/>
+      <c r="E259" s="163"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6803,18 +6803,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="174"/>
-      <c r="D276" s="175"/>
-      <c r="E276" s="175"/>
+      <c r="C276" s="166"/>
+      <c r="D276" s="167"/>
+      <c r="E276" s="167"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="158"/>
-      <c r="D277" s="159"/>
-      <c r="E277" s="159"/>
+      <c r="C277" s="162"/>
+      <c r="D277" s="163"/>
+      <c r="E277" s="163"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -6965,9 +6965,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="160"/>
-      <c r="D294" s="161"/>
-      <c r="E294" s="161"/>
+      <c r="C294" s="164"/>
+      <c r="D294" s="165"/>
+      <c r="E294" s="165"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7118,9 +7118,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="158"/>
-      <c r="D311" s="159"/>
-      <c r="E311" s="159"/>
+      <c r="C311" s="162"/>
+      <c r="D311" s="163"/>
+      <c r="E311" s="163"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7271,9 +7271,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="158"/>
-      <c r="D328" s="159"/>
-      <c r="E328" s="159"/>
+      <c r="C328" s="162"/>
+      <c r="D328" s="163"/>
+      <c r="E328" s="163"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7424,9 +7424,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="158"/>
-      <c r="D345" s="159"/>
-      <c r="E345" s="159"/>
+      <c r="C345" s="162"/>
+      <c r="D345" s="163"/>
+      <c r="E345" s="163"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7577,9 +7577,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="158"/>
-      <c r="D362" s="159"/>
-      <c r="E362" s="159"/>
+      <c r="C362" s="162"/>
+      <c r="D362" s="163"/>
+      <c r="E362" s="163"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7730,9 +7730,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="158"/>
-      <c r="D379" s="159"/>
-      <c r="E379" s="159"/>
+      <c r="C379" s="162"/>
+      <c r="D379" s="163"/>
+      <c r="E379" s="163"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7883,9 +7883,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="158"/>
-      <c r="D396" s="159"/>
-      <c r="E396" s="159"/>
+      <c r="C396" s="162"/>
+      <c r="D396" s="163"/>
+      <c r="E396" s="163"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8036,9 +8036,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="158"/>
-      <c r="D413" s="159"/>
-      <c r="E413" s="159"/>
+      <c r="C413" s="162"/>
+      <c r="D413" s="163"/>
+      <c r="E413" s="163"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8189,9 +8189,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="158"/>
-      <c r="D430" s="159"/>
-      <c r="E430" s="159"/>
+      <c r="C430" s="162"/>
+      <c r="D430" s="163"/>
+      <c r="E430" s="163"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8342,9 +8342,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="158"/>
-      <c r="D447" s="159"/>
-      <c r="E447" s="159"/>
+      <c r="C447" s="162"/>
+      <c r="D447" s="163"/>
+      <c r="E447" s="163"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8495,9 +8495,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="158"/>
-      <c r="D464" s="159"/>
-      <c r="E464" s="159"/>
+      <c r="C464" s="162"/>
+      <c r="D464" s="163"/>
+      <c r="E464" s="163"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8648,9 +8648,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="158"/>
-      <c r="D481" s="159"/>
-      <c r="E481" s="159"/>
+      <c r="C481" s="162"/>
+      <c r="D481" s="163"/>
+      <c r="E481" s="163"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8801,9 +8801,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="158"/>
-      <c r="D498" s="159"/>
-      <c r="E498" s="159"/>
+      <c r="C498" s="162"/>
+      <c r="D498" s="163"/>
+      <c r="E498" s="163"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -8954,9 +8954,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="158"/>
-      <c r="D515" s="159"/>
-      <c r="E515" s="159"/>
+      <c r="C515" s="162"/>
+      <c r="D515" s="163"/>
+      <c r="E515" s="163"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9107,9 +9107,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="158"/>
-      <c r="D532" s="159"/>
-      <c r="E532" s="159"/>
+      <c r="C532" s="162"/>
+      <c r="D532" s="163"/>
+      <c r="E532" s="163"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9260,18 +9260,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="172"/>
-      <c r="D549" s="173"/>
-      <c r="E549" s="173"/>
+      <c r="C549" s="168"/>
+      <c r="D549" s="169"/>
+      <c r="E549" s="169"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="158"/>
-      <c r="D550" s="159"/>
-      <c r="E550" s="159"/>
+      <c r="C550" s="162"/>
+      <c r="D550" s="163"/>
+      <c r="E550" s="163"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9422,9 +9422,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="160"/>
-      <c r="D567" s="161"/>
-      <c r="E567" s="161"/>
+      <c r="C567" s="164"/>
+      <c r="D567" s="165"/>
+      <c r="E567" s="165"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9575,9 +9575,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="158"/>
-      <c r="D584" s="159"/>
-      <c r="E584" s="159"/>
+      <c r="C584" s="162"/>
+      <c r="D584" s="163"/>
+      <c r="E584" s="163"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9728,9 +9728,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="158"/>
-      <c r="D601" s="159"/>
-      <c r="E601" s="159"/>
+      <c r="C601" s="162"/>
+      <c r="D601" s="163"/>
+      <c r="E601" s="163"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9881,9 +9881,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="158"/>
-      <c r="D618" s="159"/>
-      <c r="E618" s="159"/>
+      <c r="C618" s="162"/>
+      <c r="D618" s="163"/>
+      <c r="E618" s="163"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10034,9 +10034,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="158"/>
-      <c r="D635" s="159"/>
-      <c r="E635" s="159"/>
+      <c r="C635" s="162"/>
+      <c r="D635" s="163"/>
+      <c r="E635" s="163"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10187,9 +10187,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="158"/>
-      <c r="D652" s="159"/>
-      <c r="E652" s="159"/>
+      <c r="C652" s="162"/>
+      <c r="D652" s="163"/>
+      <c r="E652" s="163"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10340,9 +10340,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="158"/>
-      <c r="D669" s="159"/>
-      <c r="E669" s="159"/>
+      <c r="C669" s="162"/>
+      <c r="D669" s="163"/>
+      <c r="E669" s="163"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10493,9 +10493,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="158"/>
-      <c r="D686" s="159"/>
-      <c r="E686" s="159"/>
+      <c r="C686" s="162"/>
+      <c r="D686" s="163"/>
+      <c r="E686" s="163"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10646,9 +10646,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="158"/>
-      <c r="D703" s="159"/>
-      <c r="E703" s="159"/>
+      <c r="C703" s="162"/>
+      <c r="D703" s="163"/>
+      <c r="E703" s="163"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10799,9 +10799,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="158"/>
-      <c r="D720" s="159"/>
-      <c r="E720" s="159"/>
+      <c r="C720" s="162"/>
+      <c r="D720" s="163"/>
+      <c r="E720" s="163"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -10952,9 +10952,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="158"/>
-      <c r="D737" s="159"/>
-      <c r="E737" s="159"/>
+      <c r="C737" s="162"/>
+      <c r="D737" s="163"/>
+      <c r="E737" s="163"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11105,9 +11105,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="158"/>
-      <c r="D754" s="159"/>
-      <c r="E754" s="159"/>
+      <c r="C754" s="162"/>
+      <c r="D754" s="163"/>
+      <c r="E754" s="163"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11258,9 +11258,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="158"/>
-      <c r="D771" s="159"/>
-      <c r="E771" s="159"/>
+      <c r="C771" s="162"/>
+      <c r="D771" s="163"/>
+      <c r="E771" s="163"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11411,9 +11411,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="158"/>
-      <c r="D788" s="159"/>
-      <c r="E788" s="159"/>
+      <c r="C788" s="162"/>
+      <c r="D788" s="163"/>
+      <c r="E788" s="163"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11564,9 +11564,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="158"/>
-      <c r="D805" s="159"/>
-      <c r="E805" s="159"/>
+      <c r="C805" s="162"/>
+      <c r="D805" s="163"/>
+      <c r="E805" s="163"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11726,9 +11726,9 @@
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="158"/>
-      <c r="D823" s="159"/>
-      <c r="E823" s="159"/>
+      <c r="C823" s="162"/>
+      <c r="D823" s="163"/>
+      <c r="E823" s="163"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11879,9 +11879,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="160"/>
-      <c r="D840" s="161"/>
-      <c r="E840" s="161"/>
+      <c r="C840" s="164"/>
+      <c r="D840" s="165"/>
+      <c r="E840" s="165"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12032,9 +12032,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="158"/>
-      <c r="D857" s="159"/>
-      <c r="E857" s="159"/>
+      <c r="C857" s="162"/>
+      <c r="D857" s="163"/>
+      <c r="E857" s="163"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12185,9 +12185,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="158"/>
-      <c r="D874" s="159"/>
-      <c r="E874" s="159"/>
+      <c r="C874" s="162"/>
+      <c r="D874" s="163"/>
+      <c r="E874" s="163"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12338,9 +12338,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="158"/>
-      <c r="D891" s="159"/>
-      <c r="E891" s="159"/>
+      <c r="C891" s="162"/>
+      <c r="D891" s="163"/>
+      <c r="E891" s="163"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12491,9 +12491,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="158"/>
-      <c r="D908" s="159"/>
-      <c r="E908" s="159"/>
+      <c r="C908" s="162"/>
+      <c r="D908" s="163"/>
+      <c r="E908" s="163"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12644,9 +12644,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="158"/>
-      <c r="D925" s="159"/>
-      <c r="E925" s="159"/>
+      <c r="C925" s="162"/>
+      <c r="D925" s="163"/>
+      <c r="E925" s="163"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12797,9 +12797,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="158"/>
-      <c r="D942" s="159"/>
-      <c r="E942" s="159"/>
+      <c r="C942" s="162"/>
+      <c r="D942" s="163"/>
+      <c r="E942" s="163"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -12950,9 +12950,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="158"/>
-      <c r="D959" s="159"/>
-      <c r="E959" s="159"/>
+      <c r="C959" s="162"/>
+      <c r="D959" s="163"/>
+      <c r="E959" s="163"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13103,9 +13103,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="158"/>
-      <c r="D976" s="159"/>
-      <c r="E976" s="159"/>
+      <c r="C976" s="162"/>
+      <c r="D976" s="163"/>
+      <c r="E976" s="163"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13256,9 +13256,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="158"/>
-      <c r="D993" s="159"/>
-      <c r="E993" s="159"/>
+      <c r="C993" s="162"/>
+      <c r="D993" s="163"/>
+      <c r="E993" s="163"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13409,9 +13409,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="158"/>
-      <c r="D1010" s="159"/>
-      <c r="E1010" s="159"/>
+      <c r="C1010" s="162"/>
+      <c r="D1010" s="163"/>
+      <c r="E1010" s="163"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13562,9 +13562,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="158"/>
-      <c r="D1027" s="159"/>
-      <c r="E1027" s="159"/>
+      <c r="C1027" s="162"/>
+      <c r="D1027" s="163"/>
+      <c r="E1027" s="163"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13715,9 +13715,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="158"/>
-      <c r="D1044" s="159"/>
-      <c r="E1044" s="159"/>
+      <c r="C1044" s="162"/>
+      <c r="D1044" s="163"/>
+      <c r="E1044" s="163"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13868,9 +13868,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="158"/>
-      <c r="D1061" s="159"/>
-      <c r="E1061" s="159"/>
+      <c r="C1061" s="162"/>
+      <c r="D1061" s="163"/>
+      <c r="E1061" s="163"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14021,9 +14021,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="158"/>
-      <c r="D1078" s="159"/>
-      <c r="E1078" s="159"/>
+      <c r="C1078" s="162"/>
+      <c r="D1078" s="163"/>
+      <c r="E1078" s="163"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14174,18 +14174,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="168"/>
-      <c r="D1095" s="169"/>
-      <c r="E1095" s="169"/>
+      <c r="C1095" s="172"/>
+      <c r="D1095" s="173"/>
+      <c r="E1095" s="173"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="158"/>
-      <c r="D1096" s="159"/>
-      <c r="E1096" s="159"/>
+      <c r="C1096" s="162"/>
+      <c r="D1096" s="163"/>
+      <c r="E1096" s="163"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14336,9 +14336,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="160"/>
-      <c r="D1113" s="161"/>
-      <c r="E1113" s="161"/>
+      <c r="C1113" s="164"/>
+      <c r="D1113" s="165"/>
+      <c r="E1113" s="165"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14489,9 +14489,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="158"/>
-      <c r="D1130" s="159"/>
-      <c r="E1130" s="159"/>
+      <c r="C1130" s="162"/>
+      <c r="D1130" s="163"/>
+      <c r="E1130" s="163"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14642,9 +14642,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="158"/>
-      <c r="D1147" s="159"/>
-      <c r="E1147" s="159"/>
+      <c r="C1147" s="162"/>
+      <c r="D1147" s="163"/>
+      <c r="E1147" s="163"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14795,9 +14795,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="158"/>
-      <c r="D1164" s="159"/>
-      <c r="E1164" s="159"/>
+      <c r="C1164" s="162"/>
+      <c r="D1164" s="163"/>
+      <c r="E1164" s="163"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -14948,9 +14948,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="158"/>
-      <c r="D1181" s="159"/>
-      <c r="E1181" s="159"/>
+      <c r="C1181" s="162"/>
+      <c r="D1181" s="163"/>
+      <c r="E1181" s="163"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15101,9 +15101,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="158"/>
-      <c r="D1198" s="159"/>
-      <c r="E1198" s="159"/>
+      <c r="C1198" s="162"/>
+      <c r="D1198" s="163"/>
+      <c r="E1198" s="163"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15254,9 +15254,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="158"/>
-      <c r="D1215" s="159"/>
-      <c r="E1215" s="159"/>
+      <c r="C1215" s="162"/>
+      <c r="D1215" s="163"/>
+      <c r="E1215" s="163"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15407,9 +15407,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="158"/>
-      <c r="D1232" s="159"/>
-      <c r="E1232" s="159"/>
+      <c r="C1232" s="162"/>
+      <c r="D1232" s="163"/>
+      <c r="E1232" s="163"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15560,9 +15560,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="158"/>
-      <c r="D1249" s="159"/>
-      <c r="E1249" s="159"/>
+      <c r="C1249" s="162"/>
+      <c r="D1249" s="163"/>
+      <c r="E1249" s="163"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15713,9 +15713,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="158"/>
-      <c r="D1266" s="159"/>
-      <c r="E1266" s="159"/>
+      <c r="C1266" s="162"/>
+      <c r="D1266" s="163"/>
+      <c r="E1266" s="163"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15866,9 +15866,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="158"/>
-      <c r="D1283" s="159"/>
-      <c r="E1283" s="159"/>
+      <c r="C1283" s="162"/>
+      <c r="D1283" s="163"/>
+      <c r="E1283" s="163"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16019,9 +16019,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="158"/>
-      <c r="D1300" s="159"/>
-      <c r="E1300" s="159"/>
+      <c r="C1300" s="162"/>
+      <c r="D1300" s="163"/>
+      <c r="E1300" s="163"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16172,9 +16172,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="158"/>
-      <c r="D1317" s="159"/>
-      <c r="E1317" s="159"/>
+      <c r="C1317" s="162"/>
+      <c r="D1317" s="163"/>
+      <c r="E1317" s="163"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16325,9 +16325,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="158"/>
-      <c r="D1334" s="159"/>
-      <c r="E1334" s="159"/>
+      <c r="C1334" s="162"/>
+      <c r="D1334" s="163"/>
+      <c r="E1334" s="163"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16478,9 +16478,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="158"/>
-      <c r="D1351" s="159"/>
-      <c r="E1351" s="159"/>
+      <c r="C1351" s="162"/>
+      <c r="D1351" s="163"/>
+      <c r="E1351" s="163"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16631,18 +16631,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="166"/>
-      <c r="D1368" s="167"/>
-      <c r="E1368" s="167"/>
+      <c r="C1368" s="174"/>
+      <c r="D1368" s="175"/>
+      <c r="E1368" s="175"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="158"/>
-      <c r="D1369" s="159"/>
-      <c r="E1369" s="159"/>
+      <c r="C1369" s="162"/>
+      <c r="D1369" s="163"/>
+      <c r="E1369" s="163"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16793,9 +16793,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="160"/>
-      <c r="D1386" s="161"/>
-      <c r="E1386" s="161"/>
+      <c r="C1386" s="164"/>
+      <c r="D1386" s="165"/>
+      <c r="E1386" s="165"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -16946,9 +16946,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="158"/>
-      <c r="D1403" s="159"/>
-      <c r="E1403" s="159"/>
+      <c r="C1403" s="162"/>
+      <c r="D1403" s="163"/>
+      <c r="E1403" s="163"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17099,9 +17099,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="158"/>
-      <c r="D1420" s="159"/>
-      <c r="E1420" s="159"/>
+      <c r="C1420" s="162"/>
+      <c r="D1420" s="163"/>
+      <c r="E1420" s="163"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17252,9 +17252,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="158"/>
-      <c r="D1437" s="159"/>
-      <c r="E1437" s="159"/>
+      <c r="C1437" s="162"/>
+      <c r="D1437" s="163"/>
+      <c r="E1437" s="163"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17405,9 +17405,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="158"/>
-      <c r="D1454" s="159"/>
-      <c r="E1454" s="159"/>
+      <c r="C1454" s="162"/>
+      <c r="D1454" s="163"/>
+      <c r="E1454" s="163"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17558,9 +17558,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="158"/>
-      <c r="D1471" s="159"/>
-      <c r="E1471" s="159"/>
+      <c r="C1471" s="162"/>
+      <c r="D1471" s="163"/>
+      <c r="E1471" s="163"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17711,9 +17711,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="158"/>
-      <c r="D1488" s="159"/>
-      <c r="E1488" s="159"/>
+      <c r="C1488" s="162"/>
+      <c r="D1488" s="163"/>
+      <c r="E1488" s="163"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17864,9 +17864,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="158"/>
-      <c r="D1505" s="159"/>
-      <c r="E1505" s="159"/>
+      <c r="C1505" s="162"/>
+      <c r="D1505" s="163"/>
+      <c r="E1505" s="163"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18017,9 +18017,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="158"/>
-      <c r="D1522" s="159"/>
-      <c r="E1522" s="159"/>
+      <c r="C1522" s="162"/>
+      <c r="D1522" s="163"/>
+      <c r="E1522" s="163"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18170,9 +18170,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="158"/>
-      <c r="D1539" s="159"/>
-      <c r="E1539" s="159"/>
+      <c r="C1539" s="162"/>
+      <c r="D1539" s="163"/>
+      <c r="E1539" s="163"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18323,9 +18323,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="158"/>
-      <c r="D1556" s="159"/>
-      <c r="E1556" s="159"/>
+      <c r="C1556" s="162"/>
+      <c r="D1556" s="163"/>
+      <c r="E1556" s="163"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18476,9 +18476,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="158"/>
-      <c r="D1573" s="159"/>
-      <c r="E1573" s="159"/>
+      <c r="C1573" s="162"/>
+      <c r="D1573" s="163"/>
+      <c r="E1573" s="163"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18629,9 +18629,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="158"/>
-      <c r="D1590" s="159"/>
-      <c r="E1590" s="159"/>
+      <c r="C1590" s="162"/>
+      <c r="D1590" s="163"/>
+      <c r="E1590" s="163"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18782,9 +18782,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="158"/>
-      <c r="D1607" s="159"/>
-      <c r="E1607" s="159"/>
+      <c r="C1607" s="162"/>
+      <c r="D1607" s="163"/>
+      <c r="E1607" s="163"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18935,9 +18935,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="158"/>
-      <c r="D1624" s="159"/>
-      <c r="E1624" s="159"/>
+      <c r="C1624" s="162"/>
+      <c r="D1624" s="163"/>
+      <c r="E1624" s="163"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19088,18 +19088,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="164"/>
-      <c r="D1641" s="165"/>
-      <c r="E1641" s="165"/>
+      <c r="C1641" s="176"/>
+      <c r="D1641" s="177"/>
+      <c r="E1641" s="177"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="158"/>
-      <c r="D1642" s="159"/>
-      <c r="E1642" s="159"/>
+      <c r="C1642" s="162"/>
+      <c r="D1642" s="163"/>
+      <c r="E1642" s="163"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19250,9 +19250,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="160"/>
-      <c r="D1659" s="161"/>
-      <c r="E1659" s="161"/>
+      <c r="C1659" s="164"/>
+      <c r="D1659" s="165"/>
+      <c r="E1659" s="165"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19403,9 +19403,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="158"/>
-      <c r="D1676" s="159"/>
-      <c r="E1676" s="159"/>
+      <c r="C1676" s="162"/>
+      <c r="D1676" s="163"/>
+      <c r="E1676" s="163"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19556,9 +19556,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="158"/>
-      <c r="D1693" s="159"/>
-      <c r="E1693" s="159"/>
+      <c r="C1693" s="162"/>
+      <c r="D1693" s="163"/>
+      <c r="E1693" s="163"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19709,9 +19709,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="158"/>
-      <c r="D1710" s="159"/>
-      <c r="E1710" s="159"/>
+      <c r="C1710" s="162"/>
+      <c r="D1710" s="163"/>
+      <c r="E1710" s="163"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19862,9 +19862,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="158"/>
-      <c r="D1727" s="159"/>
-      <c r="E1727" s="159"/>
+      <c r="C1727" s="162"/>
+      <c r="D1727" s="163"/>
+      <c r="E1727" s="163"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20015,9 +20015,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="158"/>
-      <c r="D1744" s="159"/>
-      <c r="E1744" s="159"/>
+      <c r="C1744" s="162"/>
+      <c r="D1744" s="163"/>
+      <c r="E1744" s="163"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20168,9 +20168,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="158"/>
-      <c r="D1761" s="159"/>
-      <c r="E1761" s="159"/>
+      <c r="C1761" s="162"/>
+      <c r="D1761" s="163"/>
+      <c r="E1761" s="163"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20321,9 +20321,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="158"/>
-      <c r="D1778" s="159"/>
-      <c r="E1778" s="159"/>
+      <c r="C1778" s="162"/>
+      <c r="D1778" s="163"/>
+      <c r="E1778" s="163"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20474,9 +20474,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="158"/>
-      <c r="D1795" s="159"/>
-      <c r="E1795" s="159"/>
+      <c r="C1795" s="162"/>
+      <c r="D1795" s="163"/>
+      <c r="E1795" s="163"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20627,9 +20627,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="158"/>
-      <c r="D1812" s="159"/>
-      <c r="E1812" s="159"/>
+      <c r="C1812" s="162"/>
+      <c r="D1812" s="163"/>
+      <c r="E1812" s="163"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20780,9 +20780,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="158"/>
-      <c r="D1829" s="159"/>
-      <c r="E1829" s="159"/>
+      <c r="C1829" s="162"/>
+      <c r="D1829" s="163"/>
+      <c r="E1829" s="163"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20933,9 +20933,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="158"/>
-      <c r="D1846" s="159"/>
-      <c r="E1846" s="159"/>
+      <c r="C1846" s="162"/>
+      <c r="D1846" s="163"/>
+      <c r="E1846" s="163"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21086,9 +21086,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="158"/>
-      <c r="D1863" s="159"/>
-      <c r="E1863" s="159"/>
+      <c r="C1863" s="162"/>
+      <c r="D1863" s="163"/>
+      <c r="E1863" s="163"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21239,9 +21239,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="158"/>
-      <c r="D1880" s="159"/>
-      <c r="E1880" s="159"/>
+      <c r="C1880" s="162"/>
+      <c r="D1880" s="163"/>
+      <c r="E1880" s="163"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21392,9 +21392,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="158"/>
-      <c r="D1897" s="159"/>
-      <c r="E1897" s="159"/>
+      <c r="C1897" s="162"/>
+      <c r="D1897" s="163"/>
+      <c r="E1897" s="163"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21545,18 +21545,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="162"/>
-      <c r="D1914" s="163"/>
-      <c r="E1914" s="163"/>
+      <c r="C1914" s="178"/>
+      <c r="D1914" s="179"/>
+      <c r="E1914" s="179"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="158"/>
-      <c r="D1915" s="159"/>
-      <c r="E1915" s="159"/>
+      <c r="C1915" s="162"/>
+      <c r="D1915" s="163"/>
+      <c r="E1915" s="163"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21707,9 +21707,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="160"/>
-      <c r="D1932" s="161"/>
-      <c r="E1932" s="161"/>
+      <c r="C1932" s="164"/>
+      <c r="D1932" s="165"/>
+      <c r="E1932" s="165"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21860,9 +21860,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="158"/>
-      <c r="D1949" s="159"/>
-      <c r="E1949" s="159"/>
+      <c r="C1949" s="162"/>
+      <c r="D1949" s="163"/>
+      <c r="E1949" s="163"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22013,9 +22013,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="158"/>
-      <c r="D1966" s="159"/>
-      <c r="E1966" s="159"/>
+      <c r="C1966" s="162"/>
+      <c r="D1966" s="163"/>
+      <c r="E1966" s="163"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22166,9 +22166,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="158"/>
-      <c r="D1983" s="159"/>
-      <c r="E1983" s="159"/>
+      <c r="C1983" s="162"/>
+      <c r="D1983" s="163"/>
+      <c r="E1983" s="163"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22319,9 +22319,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="158"/>
-      <c r="D2000" s="159"/>
-      <c r="E2000" s="159"/>
+      <c r="C2000" s="162"/>
+      <c r="D2000" s="163"/>
+      <c r="E2000" s="163"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22472,9 +22472,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="158"/>
-      <c r="D2017" s="159"/>
-      <c r="E2017" s="159"/>
+      <c r="C2017" s="162"/>
+      <c r="D2017" s="163"/>
+      <c r="E2017" s="163"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22625,9 +22625,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="158"/>
-      <c r="D2034" s="159"/>
-      <c r="E2034" s="159"/>
+      <c r="C2034" s="162"/>
+      <c r="D2034" s="163"/>
+      <c r="E2034" s="163"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22778,9 +22778,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="158"/>
-      <c r="D2051" s="159"/>
-      <c r="E2051" s="159"/>
+      <c r="C2051" s="162"/>
+      <c r="D2051" s="163"/>
+      <c r="E2051" s="163"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22931,9 +22931,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="158"/>
-      <c r="D2068" s="159"/>
-      <c r="E2068" s="159"/>
+      <c r="C2068" s="162"/>
+      <c r="D2068" s="163"/>
+      <c r="E2068" s="163"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23084,9 +23084,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="158"/>
-      <c r="D2085" s="159"/>
-      <c r="E2085" s="159"/>
+      <c r="C2085" s="162"/>
+      <c r="D2085" s="163"/>
+      <c r="E2085" s="163"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23237,9 +23237,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="158"/>
-      <c r="D2102" s="159"/>
-      <c r="E2102" s="159"/>
+      <c r="C2102" s="162"/>
+      <c r="D2102" s="163"/>
+      <c r="E2102" s="163"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23390,9 +23390,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="158"/>
-      <c r="D2119" s="159"/>
-      <c r="E2119" s="159"/>
+      <c r="C2119" s="162"/>
+      <c r="D2119" s="163"/>
+      <c r="E2119" s="163"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23543,9 +23543,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="158"/>
-      <c r="D2136" s="159"/>
-      <c r="E2136" s="159"/>
+      <c r="C2136" s="162"/>
+      <c r="D2136" s="163"/>
+      <c r="E2136" s="163"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23696,9 +23696,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="158"/>
-      <c r="D2153" s="159"/>
-      <c r="E2153" s="159"/>
+      <c r="C2153" s="162"/>
+      <c r="D2153" s="163"/>
+      <c r="E2153" s="163"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23849,9 +23849,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="158"/>
-      <c r="D2170" s="159"/>
-      <c r="E2170" s="159"/>
+      <c r="C2170" s="162"/>
+      <c r="D2170" s="163"/>
+      <c r="E2170" s="163"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -23999,26 +23999,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24031,111 +24116,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24162,51 +24162,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="186" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
-      <c r="L1" s="185"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
+      <c r="K1" s="186"/>
+      <c r="L1" s="186"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="183" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="184"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="185"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="180" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="181"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="181"/>
+      <c r="K3" s="182"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24423,19 +24423,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="179" t="s">
+      <c r="A20" s="180" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="180"/>
-      <c r="C20" s="180"/>
-      <c r="D20" s="180"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="181"/>
+      <c r="B20" s="181"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="182"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24652,19 +24652,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="179" t="s">
+      <c r="A37" s="180" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="180"/>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="180"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="180"/>
-      <c r="K37" s="181"/>
+      <c r="B37" s="181"/>
+      <c r="C37" s="181"/>
+      <c r="D37" s="181"/>
+      <c r="E37" s="181"/>
+      <c r="F37" s="181"/>
+      <c r="G37" s="181"/>
+      <c r="H37" s="181"/>
+      <c r="I37" s="181"/>
+      <c r="J37" s="181"/>
+      <c r="K37" s="182"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -24922,28 +24922,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="186"/>
+      <c r="A3" s="187"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="187"/>
+      <c r="A4" s="188"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="187"/>
+      <c r="A5" s="188"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="187"/>
+      <c r="A6" s="188"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="187"/>
+      <c r="A7" s="188"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="187"/>
+      <c r="A8" s="188"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="187"/>
+      <c r="A9" s="188"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="188"/>
+      <c r="A10" s="189"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25126,10 +25126,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="190" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="190"/>
+      <c r="C1" s="191"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25140,7 +25140,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="192" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25154,7 +25154,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="192"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25166,7 +25166,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="192"/>
+      <c r="A5" s="193"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25175,7 +25175,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="192"/>
+      <c r="A6" s="193"/>
       <c r="B6" s="139" t="s">
         <v>212</v>
       </c>
@@ -25187,7 +25187,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="192"/>
+      <c r="A7" s="193"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25199,7 +25199,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="192"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25208,7 +25208,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="193"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25223,7 +25223,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="191" t="s">
+      <c r="A11" s="192" t="s">
         <v>211</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25237,7 +25237,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="192"/>
+      <c r="A12" s="193"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25249,7 +25249,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="192"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25258,7 +25258,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="192"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="139" t="s">
         <v>212</v>
       </c>
@@ -25270,7 +25270,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="192"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25282,7 +25282,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="192"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25291,7 +25291,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25306,7 +25306,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="191" t="s">
+      <c r="A19" s="192" t="s">
         <v>211</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25315,7 +25315,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="192"/>
+      <c r="A20" s="193"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25325,14 +25325,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="192"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="192"/>
+      <c r="A22" s="193"/>
       <c r="B22" s="139" t="s">
         <v>212</v>
       </c>
@@ -25342,7 +25342,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="192"/>
+      <c r="A23" s="193"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25352,14 +25352,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="192"/>
+      <c r="A24" s="193"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193"/>
+      <c r="A25" s="194"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25394,163 +25394,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="206"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="200" t="s">
+      <c r="A2" s="211" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="201"/>
+      <c r="B2" s="212"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="213" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="201"/>
+      <c r="B3" s="212"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
+      <c r="A4" s="209"/>
+      <c r="B4" s="210"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="205" t="s">
+      <c r="A5" s="207" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="206"/>
+      <c r="B5" s="208"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="211" t="s">
+      <c r="A7" s="199" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="212"/>
+      <c r="B7" s="200"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="209" t="s">
+      <c r="A9" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="210"/>
+      <c r="B9" s="202"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="196"/>
-      <c r="B10" s="197"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="195" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="199"/>
+      <c r="B11" s="196"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="198" t="s">
+      <c r="A12" s="195" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="199"/>
+      <c r="B12" s="196"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="195" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="199"/>
+      <c r="B13" s="196"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="198" t="s">
+      <c r="A14" s="195" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="199"/>
+      <c r="B14" s="196"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="198" t="s">
+      <c r="A15" s="195" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="199"/>
+      <c r="B15" s="196"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="198" t="s">
+      <c r="A16" s="195" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="199"/>
+      <c r="B16" s="196"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="194" t="s">
+      <c r="A17" s="197" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="195"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="211" t="s">
+      <c r="A19" s="199" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="212"/>
+      <c r="B19" s="200"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="209" t="s">
+      <c r="A21" s="201" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="210"/>
+      <c r="B21" s="202"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="196"/>
-      <c r="B22" s="197"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="204"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="198" t="s">
+      <c r="A23" s="195" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="199"/>
+      <c r="B23" s="196"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="198"/>
-      <c r="B24" s="199"/>
+      <c r="A24" s="195"/>
+      <c r="B24" s="196"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="198" t="s">
+      <c r="A25" s="195" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="199"/>
+      <c r="B25" s="196"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="198" t="s">
+      <c r="A26" s="195" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="199"/>
+      <c r="B26" s="196"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="194"/>
-      <c r="B27" s="195"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25561,6 +25548,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Dragon Egg - Up to the shop exit, 53 frames ahead of my previous TAS.
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="228">
   <si>
     <t>Notes</t>
   </si>
@@ -730,6 +730,9 @@
   <si>
     <t>Exit Shop</t>
   </si>
+  <si>
+    <t>Screen 3 end</t>
+  </si>
 </sst>
 </file>
 
@@ -739,10 +742,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1655,34 +1665,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1690,208 +1700,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1901,10 +1911,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1925,139 +1935,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2376,8 +2389,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2576,14 +2589,14 @@
         <v>216</v>
       </c>
       <c r="C11" s="101">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D11" s="101">
         <v>390</v>
       </c>
       <c r="E11" s="101">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="105"/>
     </row>
@@ -2593,14 +2606,14 @@
         <v>217</v>
       </c>
       <c r="C12" s="101">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D12" s="101">
         <v>550</v>
       </c>
       <c r="E12" s="101">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="105"/>
     </row>
@@ -2632,14 +2645,14 @@
         <v>186</v>
       </c>
       <c r="C15" s="101">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D15" s="101">
         <v>835</v>
       </c>
       <c r="E15" s="121">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="105"/>
     </row>
@@ -2649,14 +2662,14 @@
         <v>187</v>
       </c>
       <c r="C16" s="99">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D16" s="99">
         <v>835</v>
       </c>
       <c r="E16" s="101">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="104"/>
     </row>
@@ -2669,7 +2682,7 @@
       </c>
       <c r="C17" s="103">
         <f>C16-C9</f>
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D17" s="103">
         <f>D16-D9</f>
@@ -2677,12 +2690,12 @@
       </c>
       <c r="E17" s="122">
         <f>E16-E9</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="106"/>
       <c r="G17" s="112">
         <f>E17</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2712,14 +2725,14 @@
         <v>184</v>
       </c>
       <c r="C20" s="99">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D20" s="99">
         <v>835</v>
       </c>
       <c r="E20" s="123">
         <f t="shared" ref="E20:E33" si="1">IF(AND(C20&gt;0,D20&gt;0), D20-C20, 0)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="104"/>
     </row>
@@ -2729,14 +2742,14 @@
         <v>218</v>
       </c>
       <c r="C21" s="101">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D21" s="101">
         <v>835</v>
       </c>
       <c r="E21" s="124">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="105"/>
     </row>
@@ -2746,14 +2759,14 @@
         <v>219</v>
       </c>
       <c r="C22" s="101">
-        <v>1466</v>
+        <v>1364</v>
       </c>
       <c r="D22" s="101">
         <v>1418</v>
       </c>
       <c r="E22" s="123">
         <f t="shared" si="1"/>
-        <v>-48</v>
+        <v>54</v>
       </c>
       <c r="F22" s="105"/>
       <c r="H22" t="s">
@@ -2769,14 +2782,14 @@
         <v>226</v>
       </c>
       <c r="C23" s="101">
-        <v>1605</v>
+        <v>1502</v>
       </c>
       <c r="D23" s="101">
         <v>1555</v>
       </c>
       <c r="E23" s="123">
         <f t="shared" si="1"/>
-        <v>-50</v>
+        <v>53</v>
       </c>
       <c r="F23" s="105"/>
       <c r="J23" t="s">
@@ -2788,15 +2801,13 @@
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="C24" s="101">
-        <v>1892</v>
-      </c>
+      <c r="C24" s="101"/>
       <c r="D24" s="101">
         <v>2000</v>
       </c>
       <c r="E24" s="123">
         <f t="shared" ref="E24:E25" si="2">IF(AND(C24&gt;0,D24&gt;0), D24-C24, 0)</f>
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="F24" s="105"/>
     </row>
@@ -2805,21 +2816,21 @@
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="101">
-        <v>2899</v>
-      </c>
+      <c r="C25" s="101"/>
       <c r="D25" s="101">
         <v>2990</v>
       </c>
       <c r="E25" s="123">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="151"/>
-      <c r="B26" s="100"/>
+      <c r="B26" s="214" t="s">
+        <v>227</v>
+      </c>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
       <c r="E26" s="123">
@@ -2919,7 +2930,7 @@
       </c>
       <c r="C34" s="103">
         <f>C33-C20</f>
-        <v>-805</v>
+        <v>-806</v>
       </c>
       <c r="D34" s="103">
         <f>D33-D20</f>
@@ -2927,12 +2938,12 @@
       </c>
       <c r="E34" s="126">
         <f>E33-E20</f>
-        <v>-30</v>
+        <v>-29</v>
       </c>
       <c r="F34" s="108"/>
       <c r="G34" s="112">
         <f>E34</f>
-        <v>-30</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -4265,11 +4276,6 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4278,6 +4284,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4309,13 +4320,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4345,18 +4356,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4508,9 +4519,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="164"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="165"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="162"/>
+      <c r="E21" s="162"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4661,9 +4672,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="162"/>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="160"/>
+      <c r="E38" s="160"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4814,9 +4825,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="162"/>
-      <c r="D55" s="163"/>
-      <c r="E55" s="163"/>
+      <c r="C55" s="159"/>
+      <c r="D55" s="160"/>
+      <c r="E55" s="160"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -4967,9 +4978,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="162"/>
-      <c r="D72" s="163"/>
-      <c r="E72" s="163"/>
+      <c r="C72" s="159"/>
+      <c r="D72" s="160"/>
+      <c r="E72" s="160"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5120,9 +5131,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="162"/>
-      <c r="D89" s="163"/>
-      <c r="E89" s="163"/>
+      <c r="C89" s="159"/>
+      <c r="D89" s="160"/>
+      <c r="E89" s="160"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5273,9 +5284,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="162"/>
-      <c r="D106" s="163"/>
-      <c r="E106" s="163"/>
+      <c r="C106" s="159"/>
+      <c r="D106" s="160"/>
+      <c r="E106" s="160"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5426,9 +5437,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="162"/>
-      <c r="D123" s="163"/>
-      <c r="E123" s="163"/>
+      <c r="C123" s="159"/>
+      <c r="D123" s="160"/>
+      <c r="E123" s="160"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5579,9 +5590,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="162"/>
-      <c r="D140" s="163"/>
-      <c r="E140" s="163"/>
+      <c r="C140" s="159"/>
+      <c r="D140" s="160"/>
+      <c r="E140" s="160"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5732,9 +5743,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="162"/>
-      <c r="D157" s="163"/>
-      <c r="E157" s="163"/>
+      <c r="C157" s="159"/>
+      <c r="D157" s="160"/>
+      <c r="E157" s="160"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5885,9 +5896,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="162"/>
-      <c r="D174" s="163"/>
-      <c r="E174" s="163"/>
+      <c r="C174" s="159"/>
+      <c r="D174" s="160"/>
+      <c r="E174" s="160"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6038,9 +6049,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="162"/>
-      <c r="D191" s="163"/>
-      <c r="E191" s="163"/>
+      <c r="C191" s="159"/>
+      <c r="D191" s="160"/>
+      <c r="E191" s="160"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6191,9 +6202,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="162"/>
-      <c r="D208" s="163"/>
-      <c r="E208" s="163"/>
+      <c r="C208" s="159"/>
+      <c r="D208" s="160"/>
+      <c r="E208" s="160"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6344,9 +6355,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="162"/>
-      <c r="D225" s="163"/>
-      <c r="E225" s="163"/>
+      <c r="C225" s="159"/>
+      <c r="D225" s="160"/>
+      <c r="E225" s="160"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6497,9 +6508,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="162"/>
-      <c r="D242" s="163"/>
-      <c r="E242" s="163"/>
+      <c r="C242" s="159"/>
+      <c r="D242" s="160"/>
+      <c r="E242" s="160"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6650,9 +6661,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="162"/>
-      <c r="D259" s="163"/>
-      <c r="E259" s="163"/>
+      <c r="C259" s="159"/>
+      <c r="D259" s="160"/>
+      <c r="E259" s="160"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6803,18 +6814,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="166"/>
-      <c r="D276" s="167"/>
-      <c r="E276" s="167"/>
+      <c r="C276" s="175"/>
+      <c r="D276" s="176"/>
+      <c r="E276" s="176"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="162"/>
-      <c r="D277" s="163"/>
-      <c r="E277" s="163"/>
+      <c r="C277" s="159"/>
+      <c r="D277" s="160"/>
+      <c r="E277" s="160"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -6965,9 +6976,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="164"/>
-      <c r="D294" s="165"/>
-      <c r="E294" s="165"/>
+      <c r="C294" s="161"/>
+      <c r="D294" s="162"/>
+      <c r="E294" s="162"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7118,9 +7129,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="162"/>
-      <c r="D311" s="163"/>
-      <c r="E311" s="163"/>
+      <c r="C311" s="159"/>
+      <c r="D311" s="160"/>
+      <c r="E311" s="160"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7271,9 +7282,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="162"/>
-      <c r="D328" s="163"/>
-      <c r="E328" s="163"/>
+      <c r="C328" s="159"/>
+      <c r="D328" s="160"/>
+      <c r="E328" s="160"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7424,9 +7435,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="162"/>
-      <c r="D345" s="163"/>
-      <c r="E345" s="163"/>
+      <c r="C345" s="159"/>
+      <c r="D345" s="160"/>
+      <c r="E345" s="160"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7577,9 +7588,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="162"/>
-      <c r="D362" s="163"/>
-      <c r="E362" s="163"/>
+      <c r="C362" s="159"/>
+      <c r="D362" s="160"/>
+      <c r="E362" s="160"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7730,9 +7741,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="162"/>
-      <c r="D379" s="163"/>
-      <c r="E379" s="163"/>
+      <c r="C379" s="159"/>
+      <c r="D379" s="160"/>
+      <c r="E379" s="160"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7883,9 +7894,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="162"/>
-      <c r="D396" s="163"/>
-      <c r="E396" s="163"/>
+      <c r="C396" s="159"/>
+      <c r="D396" s="160"/>
+      <c r="E396" s="160"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8036,9 +8047,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="162"/>
-      <c r="D413" s="163"/>
-      <c r="E413" s="163"/>
+      <c r="C413" s="159"/>
+      <c r="D413" s="160"/>
+      <c r="E413" s="160"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8189,9 +8200,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="162"/>
-      <c r="D430" s="163"/>
-      <c r="E430" s="163"/>
+      <c r="C430" s="159"/>
+      <c r="D430" s="160"/>
+      <c r="E430" s="160"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8342,9 +8353,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="162"/>
-      <c r="D447" s="163"/>
-      <c r="E447" s="163"/>
+      <c r="C447" s="159"/>
+      <c r="D447" s="160"/>
+      <c r="E447" s="160"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8495,9 +8506,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="162"/>
-      <c r="D464" s="163"/>
-      <c r="E464" s="163"/>
+      <c r="C464" s="159"/>
+      <c r="D464" s="160"/>
+      <c r="E464" s="160"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8648,9 +8659,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="162"/>
-      <c r="D481" s="163"/>
-      <c r="E481" s="163"/>
+      <c r="C481" s="159"/>
+      <c r="D481" s="160"/>
+      <c r="E481" s="160"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8801,9 +8812,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="162"/>
-      <c r="D498" s="163"/>
-      <c r="E498" s="163"/>
+      <c r="C498" s="159"/>
+      <c r="D498" s="160"/>
+      <c r="E498" s="160"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -8954,9 +8965,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="162"/>
-      <c r="D515" s="163"/>
-      <c r="E515" s="163"/>
+      <c r="C515" s="159"/>
+      <c r="D515" s="160"/>
+      <c r="E515" s="160"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9107,9 +9118,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="162"/>
-      <c r="D532" s="163"/>
-      <c r="E532" s="163"/>
+      <c r="C532" s="159"/>
+      <c r="D532" s="160"/>
+      <c r="E532" s="160"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9260,18 +9271,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="168"/>
-      <c r="D549" s="169"/>
-      <c r="E549" s="169"/>
+      <c r="C549" s="173"/>
+      <c r="D549" s="174"/>
+      <c r="E549" s="174"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="162"/>
-      <c r="D550" s="163"/>
-      <c r="E550" s="163"/>
+      <c r="C550" s="159"/>
+      <c r="D550" s="160"/>
+      <c r="E550" s="160"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9422,9 +9433,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="164"/>
-      <c r="D567" s="165"/>
-      <c r="E567" s="165"/>
+      <c r="C567" s="161"/>
+      <c r="D567" s="162"/>
+      <c r="E567" s="162"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9575,9 +9586,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="162"/>
-      <c r="D584" s="163"/>
-      <c r="E584" s="163"/>
+      <c r="C584" s="159"/>
+      <c r="D584" s="160"/>
+      <c r="E584" s="160"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9728,9 +9739,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="162"/>
-      <c r="D601" s="163"/>
-      <c r="E601" s="163"/>
+      <c r="C601" s="159"/>
+      <c r="D601" s="160"/>
+      <c r="E601" s="160"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9881,9 +9892,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="162"/>
-      <c r="D618" s="163"/>
-      <c r="E618" s="163"/>
+      <c r="C618" s="159"/>
+      <c r="D618" s="160"/>
+      <c r="E618" s="160"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10034,9 +10045,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="162"/>
-      <c r="D635" s="163"/>
-      <c r="E635" s="163"/>
+      <c r="C635" s="159"/>
+      <c r="D635" s="160"/>
+      <c r="E635" s="160"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10187,9 +10198,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="162"/>
-      <c r="D652" s="163"/>
-      <c r="E652" s="163"/>
+      <c r="C652" s="159"/>
+      <c r="D652" s="160"/>
+      <c r="E652" s="160"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10340,9 +10351,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="162"/>
-      <c r="D669" s="163"/>
-      <c r="E669" s="163"/>
+      <c r="C669" s="159"/>
+      <c r="D669" s="160"/>
+      <c r="E669" s="160"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10493,9 +10504,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="162"/>
-      <c r="D686" s="163"/>
-      <c r="E686" s="163"/>
+      <c r="C686" s="159"/>
+      <c r="D686" s="160"/>
+      <c r="E686" s="160"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10646,9 +10657,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="162"/>
-      <c r="D703" s="163"/>
-      <c r="E703" s="163"/>
+      <c r="C703" s="159"/>
+      <c r="D703" s="160"/>
+      <c r="E703" s="160"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10799,9 +10810,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="162"/>
-      <c r="D720" s="163"/>
-      <c r="E720" s="163"/>
+      <c r="C720" s="159"/>
+      <c r="D720" s="160"/>
+      <c r="E720" s="160"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -10952,9 +10963,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="162"/>
-      <c r="D737" s="163"/>
-      <c r="E737" s="163"/>
+      <c r="C737" s="159"/>
+      <c r="D737" s="160"/>
+      <c r="E737" s="160"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11105,9 +11116,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="162"/>
-      <c r="D754" s="163"/>
-      <c r="E754" s="163"/>
+      <c r="C754" s="159"/>
+      <c r="D754" s="160"/>
+      <c r="E754" s="160"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11258,9 +11269,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="162"/>
-      <c r="D771" s="163"/>
-      <c r="E771" s="163"/>
+      <c r="C771" s="159"/>
+      <c r="D771" s="160"/>
+      <c r="E771" s="160"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11411,9 +11422,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="162"/>
-      <c r="D788" s="163"/>
-      <c r="E788" s="163"/>
+      <c r="C788" s="159"/>
+      <c r="D788" s="160"/>
+      <c r="E788" s="160"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11564,9 +11575,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="162"/>
-      <c r="D805" s="163"/>
-      <c r="E805" s="163"/>
+      <c r="C805" s="159"/>
+      <c r="D805" s="160"/>
+      <c r="E805" s="160"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11717,18 +11728,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="170"/>
-      <c r="D822" s="171"/>
-      <c r="E822" s="171"/>
+      <c r="C822" s="171"/>
+      <c r="D822" s="172"/>
+      <c r="E822" s="172"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="162"/>
-      <c r="D823" s="163"/>
-      <c r="E823" s="163"/>
+      <c r="C823" s="159"/>
+      <c r="D823" s="160"/>
+      <c r="E823" s="160"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11879,9 +11890,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="164"/>
-      <c r="D840" s="165"/>
-      <c r="E840" s="165"/>
+      <c r="C840" s="161"/>
+      <c r="D840" s="162"/>
+      <c r="E840" s="162"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12032,9 +12043,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="162"/>
-      <c r="D857" s="163"/>
-      <c r="E857" s="163"/>
+      <c r="C857" s="159"/>
+      <c r="D857" s="160"/>
+      <c r="E857" s="160"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12185,9 +12196,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="162"/>
-      <c r="D874" s="163"/>
-      <c r="E874" s="163"/>
+      <c r="C874" s="159"/>
+      <c r="D874" s="160"/>
+      <c r="E874" s="160"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12338,9 +12349,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="162"/>
-      <c r="D891" s="163"/>
-      <c r="E891" s="163"/>
+      <c r="C891" s="159"/>
+      <c r="D891" s="160"/>
+      <c r="E891" s="160"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12491,9 +12502,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="162"/>
-      <c r="D908" s="163"/>
-      <c r="E908" s="163"/>
+      <c r="C908" s="159"/>
+      <c r="D908" s="160"/>
+      <c r="E908" s="160"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12644,9 +12655,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="162"/>
-      <c r="D925" s="163"/>
-      <c r="E925" s="163"/>
+      <c r="C925" s="159"/>
+      <c r="D925" s="160"/>
+      <c r="E925" s="160"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12797,9 +12808,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="162"/>
-      <c r="D942" s="163"/>
-      <c r="E942" s="163"/>
+      <c r="C942" s="159"/>
+      <c r="D942" s="160"/>
+      <c r="E942" s="160"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -12950,9 +12961,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="162"/>
-      <c r="D959" s="163"/>
-      <c r="E959" s="163"/>
+      <c r="C959" s="159"/>
+      <c r="D959" s="160"/>
+      <c r="E959" s="160"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13103,9 +13114,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="162"/>
-      <c r="D976" s="163"/>
-      <c r="E976" s="163"/>
+      <c r="C976" s="159"/>
+      <c r="D976" s="160"/>
+      <c r="E976" s="160"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13256,9 +13267,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="162"/>
-      <c r="D993" s="163"/>
-      <c r="E993" s="163"/>
+      <c r="C993" s="159"/>
+      <c r="D993" s="160"/>
+      <c r="E993" s="160"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13409,9 +13420,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="162"/>
-      <c r="D1010" s="163"/>
-      <c r="E1010" s="163"/>
+      <c r="C1010" s="159"/>
+      <c r="D1010" s="160"/>
+      <c r="E1010" s="160"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13562,9 +13573,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="162"/>
-      <c r="D1027" s="163"/>
-      <c r="E1027" s="163"/>
+      <c r="C1027" s="159"/>
+      <c r="D1027" s="160"/>
+      <c r="E1027" s="160"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13715,9 +13726,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="162"/>
-      <c r="D1044" s="163"/>
-      <c r="E1044" s="163"/>
+      <c r="C1044" s="159"/>
+      <c r="D1044" s="160"/>
+      <c r="E1044" s="160"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13868,9 +13879,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="162"/>
-      <c r="D1061" s="163"/>
-      <c r="E1061" s="163"/>
+      <c r="C1061" s="159"/>
+      <c r="D1061" s="160"/>
+      <c r="E1061" s="160"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14021,9 +14032,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="162"/>
-      <c r="D1078" s="163"/>
-      <c r="E1078" s="163"/>
+      <c r="C1078" s="159"/>
+      <c r="D1078" s="160"/>
+      <c r="E1078" s="160"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14174,18 +14185,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="172"/>
-      <c r="D1095" s="173"/>
-      <c r="E1095" s="173"/>
+      <c r="C1095" s="169"/>
+      <c r="D1095" s="170"/>
+      <c r="E1095" s="170"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="162"/>
-      <c r="D1096" s="163"/>
-      <c r="E1096" s="163"/>
+      <c r="C1096" s="159"/>
+      <c r="D1096" s="160"/>
+      <c r="E1096" s="160"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14336,9 +14347,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="164"/>
-      <c r="D1113" s="165"/>
-      <c r="E1113" s="165"/>
+      <c r="C1113" s="161"/>
+      <c r="D1113" s="162"/>
+      <c r="E1113" s="162"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14489,9 +14500,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="162"/>
-      <c r="D1130" s="163"/>
-      <c r="E1130" s="163"/>
+      <c r="C1130" s="159"/>
+      <c r="D1130" s="160"/>
+      <c r="E1130" s="160"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14642,9 +14653,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="162"/>
-      <c r="D1147" s="163"/>
-      <c r="E1147" s="163"/>
+      <c r="C1147" s="159"/>
+      <c r="D1147" s="160"/>
+      <c r="E1147" s="160"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14795,9 +14806,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="162"/>
-      <c r="D1164" s="163"/>
-      <c r="E1164" s="163"/>
+      <c r="C1164" s="159"/>
+      <c r="D1164" s="160"/>
+      <c r="E1164" s="160"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -14948,9 +14959,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="162"/>
-      <c r="D1181" s="163"/>
-      <c r="E1181" s="163"/>
+      <c r="C1181" s="159"/>
+      <c r="D1181" s="160"/>
+      <c r="E1181" s="160"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15101,9 +15112,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="162"/>
-      <c r="D1198" s="163"/>
-      <c r="E1198" s="163"/>
+      <c r="C1198" s="159"/>
+      <c r="D1198" s="160"/>
+      <c r="E1198" s="160"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15254,9 +15265,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="162"/>
-      <c r="D1215" s="163"/>
-      <c r="E1215" s="163"/>
+      <c r="C1215" s="159"/>
+      <c r="D1215" s="160"/>
+      <c r="E1215" s="160"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15407,9 +15418,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="162"/>
-      <c r="D1232" s="163"/>
-      <c r="E1232" s="163"/>
+      <c r="C1232" s="159"/>
+      <c r="D1232" s="160"/>
+      <c r="E1232" s="160"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15560,9 +15571,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="162"/>
-      <c r="D1249" s="163"/>
-      <c r="E1249" s="163"/>
+      <c r="C1249" s="159"/>
+      <c r="D1249" s="160"/>
+      <c r="E1249" s="160"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15713,9 +15724,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="162"/>
-      <c r="D1266" s="163"/>
-      <c r="E1266" s="163"/>
+      <c r="C1266" s="159"/>
+      <c r="D1266" s="160"/>
+      <c r="E1266" s="160"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15866,9 +15877,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="162"/>
-      <c r="D1283" s="163"/>
-      <c r="E1283" s="163"/>
+      <c r="C1283" s="159"/>
+      <c r="D1283" s="160"/>
+      <c r="E1283" s="160"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16019,9 +16030,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="162"/>
-      <c r="D1300" s="163"/>
-      <c r="E1300" s="163"/>
+      <c r="C1300" s="159"/>
+      <c r="D1300" s="160"/>
+      <c r="E1300" s="160"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16172,9 +16183,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="162"/>
-      <c r="D1317" s="163"/>
-      <c r="E1317" s="163"/>
+      <c r="C1317" s="159"/>
+      <c r="D1317" s="160"/>
+      <c r="E1317" s="160"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16325,9 +16336,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="162"/>
-      <c r="D1334" s="163"/>
-      <c r="E1334" s="163"/>
+      <c r="C1334" s="159"/>
+      <c r="D1334" s="160"/>
+      <c r="E1334" s="160"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16478,9 +16489,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="162"/>
-      <c r="D1351" s="163"/>
-      <c r="E1351" s="163"/>
+      <c r="C1351" s="159"/>
+      <c r="D1351" s="160"/>
+      <c r="E1351" s="160"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16631,18 +16642,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="174"/>
-      <c r="D1368" s="175"/>
-      <c r="E1368" s="175"/>
+      <c r="C1368" s="167"/>
+      <c r="D1368" s="168"/>
+      <c r="E1368" s="168"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="162"/>
-      <c r="D1369" s="163"/>
-      <c r="E1369" s="163"/>
+      <c r="C1369" s="159"/>
+      <c r="D1369" s="160"/>
+      <c r="E1369" s="160"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16793,9 +16804,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="164"/>
-      <c r="D1386" s="165"/>
-      <c r="E1386" s="165"/>
+      <c r="C1386" s="161"/>
+      <c r="D1386" s="162"/>
+      <c r="E1386" s="162"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -16946,9 +16957,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="162"/>
-      <c r="D1403" s="163"/>
-      <c r="E1403" s="163"/>
+      <c r="C1403" s="159"/>
+      <c r="D1403" s="160"/>
+      <c r="E1403" s="160"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17099,9 +17110,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="162"/>
-      <c r="D1420" s="163"/>
-      <c r="E1420" s="163"/>
+      <c r="C1420" s="159"/>
+      <c r="D1420" s="160"/>
+      <c r="E1420" s="160"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17252,9 +17263,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="162"/>
-      <c r="D1437" s="163"/>
-      <c r="E1437" s="163"/>
+      <c r="C1437" s="159"/>
+      <c r="D1437" s="160"/>
+      <c r="E1437" s="160"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17405,9 +17416,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="162"/>
-      <c r="D1454" s="163"/>
-      <c r="E1454" s="163"/>
+      <c r="C1454" s="159"/>
+      <c r="D1454" s="160"/>
+      <c r="E1454" s="160"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17558,9 +17569,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="162"/>
-      <c r="D1471" s="163"/>
-      <c r="E1471" s="163"/>
+      <c r="C1471" s="159"/>
+      <c r="D1471" s="160"/>
+      <c r="E1471" s="160"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17711,9 +17722,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="162"/>
-      <c r="D1488" s="163"/>
-      <c r="E1488" s="163"/>
+      <c r="C1488" s="159"/>
+      <c r="D1488" s="160"/>
+      <c r="E1488" s="160"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17864,9 +17875,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="162"/>
-      <c r="D1505" s="163"/>
-      <c r="E1505" s="163"/>
+      <c r="C1505" s="159"/>
+      <c r="D1505" s="160"/>
+      <c r="E1505" s="160"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18017,9 +18028,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="162"/>
-      <c r="D1522" s="163"/>
-      <c r="E1522" s="163"/>
+      <c r="C1522" s="159"/>
+      <c r="D1522" s="160"/>
+      <c r="E1522" s="160"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18170,9 +18181,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="162"/>
-      <c r="D1539" s="163"/>
-      <c r="E1539" s="163"/>
+      <c r="C1539" s="159"/>
+      <c r="D1539" s="160"/>
+      <c r="E1539" s="160"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18323,9 +18334,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="162"/>
-      <c r="D1556" s="163"/>
-      <c r="E1556" s="163"/>
+      <c r="C1556" s="159"/>
+      <c r="D1556" s="160"/>
+      <c r="E1556" s="160"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18476,9 +18487,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="162"/>
-      <c r="D1573" s="163"/>
-      <c r="E1573" s="163"/>
+      <c r="C1573" s="159"/>
+      <c r="D1573" s="160"/>
+      <c r="E1573" s="160"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18629,9 +18640,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="162"/>
-      <c r="D1590" s="163"/>
-      <c r="E1590" s="163"/>
+      <c r="C1590" s="159"/>
+      <c r="D1590" s="160"/>
+      <c r="E1590" s="160"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18782,9 +18793,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="162"/>
-      <c r="D1607" s="163"/>
-      <c r="E1607" s="163"/>
+      <c r="C1607" s="159"/>
+      <c r="D1607" s="160"/>
+      <c r="E1607" s="160"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18935,9 +18946,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="162"/>
-      <c r="D1624" s="163"/>
-      <c r="E1624" s="163"/>
+      <c r="C1624" s="159"/>
+      <c r="D1624" s="160"/>
+      <c r="E1624" s="160"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19088,18 +19099,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="176"/>
-      <c r="D1641" s="177"/>
-      <c r="E1641" s="177"/>
+      <c r="C1641" s="165"/>
+      <c r="D1641" s="166"/>
+      <c r="E1641" s="166"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="162"/>
-      <c r="D1642" s="163"/>
-      <c r="E1642" s="163"/>
+      <c r="C1642" s="159"/>
+      <c r="D1642" s="160"/>
+      <c r="E1642" s="160"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19250,9 +19261,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="164"/>
-      <c r="D1659" s="165"/>
-      <c r="E1659" s="165"/>
+      <c r="C1659" s="161"/>
+      <c r="D1659" s="162"/>
+      <c r="E1659" s="162"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19403,9 +19414,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="162"/>
-      <c r="D1676" s="163"/>
-      <c r="E1676" s="163"/>
+      <c r="C1676" s="159"/>
+      <c r="D1676" s="160"/>
+      <c r="E1676" s="160"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19556,9 +19567,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="162"/>
-      <c r="D1693" s="163"/>
-      <c r="E1693" s="163"/>
+      <c r="C1693" s="159"/>
+      <c r="D1693" s="160"/>
+      <c r="E1693" s="160"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19709,9 +19720,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="162"/>
-      <c r="D1710" s="163"/>
-      <c r="E1710" s="163"/>
+      <c r="C1710" s="159"/>
+      <c r="D1710" s="160"/>
+      <c r="E1710" s="160"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19862,9 +19873,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="162"/>
-      <c r="D1727" s="163"/>
-      <c r="E1727" s="163"/>
+      <c r="C1727" s="159"/>
+      <c r="D1727" s="160"/>
+      <c r="E1727" s="160"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20015,9 +20026,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="162"/>
-      <c r="D1744" s="163"/>
-      <c r="E1744" s="163"/>
+      <c r="C1744" s="159"/>
+      <c r="D1744" s="160"/>
+      <c r="E1744" s="160"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20168,9 +20179,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="162"/>
-      <c r="D1761" s="163"/>
-      <c r="E1761" s="163"/>
+      <c r="C1761" s="159"/>
+      <c r="D1761" s="160"/>
+      <c r="E1761" s="160"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20321,9 +20332,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="162"/>
-      <c r="D1778" s="163"/>
-      <c r="E1778" s="163"/>
+      <c r="C1778" s="159"/>
+      <c r="D1778" s="160"/>
+      <c r="E1778" s="160"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20474,9 +20485,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="162"/>
-      <c r="D1795" s="163"/>
-      <c r="E1795" s="163"/>
+      <c r="C1795" s="159"/>
+      <c r="D1795" s="160"/>
+      <c r="E1795" s="160"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20627,9 +20638,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="162"/>
-      <c r="D1812" s="163"/>
-      <c r="E1812" s="163"/>
+      <c r="C1812" s="159"/>
+      <c r="D1812" s="160"/>
+      <c r="E1812" s="160"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20780,9 +20791,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="162"/>
-      <c r="D1829" s="163"/>
-      <c r="E1829" s="163"/>
+      <c r="C1829" s="159"/>
+      <c r="D1829" s="160"/>
+      <c r="E1829" s="160"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20933,9 +20944,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="162"/>
-      <c r="D1846" s="163"/>
-      <c r="E1846" s="163"/>
+      <c r="C1846" s="159"/>
+      <c r="D1846" s="160"/>
+      <c r="E1846" s="160"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21086,9 +21097,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="162"/>
-      <c r="D1863" s="163"/>
-      <c r="E1863" s="163"/>
+      <c r="C1863" s="159"/>
+      <c r="D1863" s="160"/>
+      <c r="E1863" s="160"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21239,9 +21250,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="162"/>
-      <c r="D1880" s="163"/>
-      <c r="E1880" s="163"/>
+      <c r="C1880" s="159"/>
+      <c r="D1880" s="160"/>
+      <c r="E1880" s="160"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21392,9 +21403,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="162"/>
-      <c r="D1897" s="163"/>
-      <c r="E1897" s="163"/>
+      <c r="C1897" s="159"/>
+      <c r="D1897" s="160"/>
+      <c r="E1897" s="160"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21545,18 +21556,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="178"/>
-      <c r="D1914" s="179"/>
-      <c r="E1914" s="179"/>
+      <c r="C1914" s="163"/>
+      <c r="D1914" s="164"/>
+      <c r="E1914" s="164"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="162"/>
-      <c r="D1915" s="163"/>
-      <c r="E1915" s="163"/>
+      <c r="C1915" s="159"/>
+      <c r="D1915" s="160"/>
+      <c r="E1915" s="160"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21707,9 +21718,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="164"/>
-      <c r="D1932" s="165"/>
-      <c r="E1932" s="165"/>
+      <c r="C1932" s="161"/>
+      <c r="D1932" s="162"/>
+      <c r="E1932" s="162"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21860,9 +21871,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="162"/>
-      <c r="D1949" s="163"/>
-      <c r="E1949" s="163"/>
+      <c r="C1949" s="159"/>
+      <c r="D1949" s="160"/>
+      <c r="E1949" s="160"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22013,9 +22024,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="162"/>
-      <c r="D1966" s="163"/>
-      <c r="E1966" s="163"/>
+      <c r="C1966" s="159"/>
+      <c r="D1966" s="160"/>
+      <c r="E1966" s="160"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22166,9 +22177,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="162"/>
-      <c r="D1983" s="163"/>
-      <c r="E1983" s="163"/>
+      <c r="C1983" s="159"/>
+      <c r="D1983" s="160"/>
+      <c r="E1983" s="160"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22319,9 +22330,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="162"/>
-      <c r="D2000" s="163"/>
-      <c r="E2000" s="163"/>
+      <c r="C2000" s="159"/>
+      <c r="D2000" s="160"/>
+      <c r="E2000" s="160"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22472,9 +22483,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="162"/>
-      <c r="D2017" s="163"/>
-      <c r="E2017" s="163"/>
+      <c r="C2017" s="159"/>
+      <c r="D2017" s="160"/>
+      <c r="E2017" s="160"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22625,9 +22636,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="162"/>
-      <c r="D2034" s="163"/>
-      <c r="E2034" s="163"/>
+      <c r="C2034" s="159"/>
+      <c r="D2034" s="160"/>
+      <c r="E2034" s="160"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22778,9 +22789,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="162"/>
-      <c r="D2051" s="163"/>
-      <c r="E2051" s="163"/>
+      <c r="C2051" s="159"/>
+      <c r="D2051" s="160"/>
+      <c r="E2051" s="160"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22931,9 +22942,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="162"/>
-      <c r="D2068" s="163"/>
-      <c r="E2068" s="163"/>
+      <c r="C2068" s="159"/>
+      <c r="D2068" s="160"/>
+      <c r="E2068" s="160"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23084,9 +23095,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="162"/>
-      <c r="D2085" s="163"/>
-      <c r="E2085" s="163"/>
+      <c r="C2085" s="159"/>
+      <c r="D2085" s="160"/>
+      <c r="E2085" s="160"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23237,9 +23248,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="162"/>
-      <c r="D2102" s="163"/>
-      <c r="E2102" s="163"/>
+      <c r="C2102" s="159"/>
+      <c r="D2102" s="160"/>
+      <c r="E2102" s="160"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23390,9 +23401,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="162"/>
-      <c r="D2119" s="163"/>
-      <c r="E2119" s="163"/>
+      <c r="C2119" s="159"/>
+      <c r="D2119" s="160"/>
+      <c r="E2119" s="160"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23543,9 +23554,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="162"/>
-      <c r="D2136" s="163"/>
-      <c r="E2136" s="163"/>
+      <c r="C2136" s="159"/>
+      <c r="D2136" s="160"/>
+      <c r="E2136" s="160"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23696,9 +23707,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="162"/>
-      <c r="D2153" s="163"/>
-      <c r="E2153" s="163"/>
+      <c r="C2153" s="159"/>
+      <c r="D2153" s="160"/>
+      <c r="E2153" s="160"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23849,9 +23860,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="162"/>
-      <c r="D2170" s="163"/>
-      <c r="E2170" s="163"/>
+      <c r="C2170" s="159"/>
+      <c r="D2170" s="160"/>
+      <c r="E2170" s="160"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -23999,15 +24010,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24020,124 +24138,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24888,7 +24899,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25099,7 +25110,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25372,7 +25383,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25394,150 +25405,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="206"/>
+      <c r="B1" s="205"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="201" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="212"/>
+      <c r="B2" s="202"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="213" t="s">
+      <c r="A3" s="203" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="212"/>
+      <c r="B3" s="202"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="209"/>
-      <c r="B4" s="210"/>
+      <c r="A4" s="208"/>
+      <c r="B4" s="209"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="207" t="s">
+      <c r="A5" s="206" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="208"/>
+      <c r="B5" s="207"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="200"/>
+      <c r="B7" s="213"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="201" t="s">
+      <c r="A9" s="210" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="202"/>
+      <c r="B9" s="211"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="197"/>
+      <c r="B10" s="198"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="199" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="196"/>
+      <c r="B11" s="200"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="199" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="196"/>
+      <c r="B12" s="200"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="199" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="196"/>
+      <c r="B13" s="200"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="199" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="196"/>
+      <c r="B14" s="200"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="195" t="s">
+      <c r="A15" s="199" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="196"/>
+      <c r="B15" s="200"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="195" t="s">
+      <c r="A16" s="199" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="196"/>
+      <c r="B16" s="200"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="195" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="196"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="199" t="s">
+      <c r="A19" s="212" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="200"/>
+      <c r="B19" s="213"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="201" t="s">
+      <c r="A21" s="210" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="202"/>
+      <c r="B21" s="211"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="197"/>
+      <c r="B22" s="198"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="195" t="s">
+      <c r="A23" s="199" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="196"/>
+      <c r="B23" s="200"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="195"/>
-      <c r="B24" s="196"/>
+      <c r="A24" s="199"/>
+      <c r="B24" s="200"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="199" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="196"/>
+      <c r="B25" s="200"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="195" t="s">
+      <c r="A26" s="199" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="196"/>
+      <c r="B26" s="200"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="195"/>
+      <c r="B27" s="196"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25548,19 +25572,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Dragon Egg - Level 1 done, 40 frames ahead.  (Previous commit suggested 50+ frames of improvement but that was due to an incorrect calculation due to the previous TAS taking the time to manipulate an orb before entering the shop)
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="230">
   <si>
     <t>Notes</t>
   </si>
@@ -733,6 +733,12 @@
   <si>
     <t>Screen 3 end</t>
   </si>
+  <si>
+    <t>Boss end black screen</t>
+  </si>
+  <si>
+    <t>Player appears</t>
+  </si>
 </sst>
 </file>
 
@@ -742,10 +748,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1665,34 +1678,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,208 +1713,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1911,10 +1924,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1935,140 +1948,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2389,8 +2405,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2406,16 +2422,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="156" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="157" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
@@ -2493,10 +2509,10 @@
       <c r="B5" s="147" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2512,10 +2528,10 @@
       <c r="B6" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="154" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2533,7 +2549,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="159" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2553,7 +2569,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="151"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
@@ -2567,7 +2583,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2584,7 +2600,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2601,7 +2617,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2618,7 +2634,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="151"/>
+      <c r="A13" s="152"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2629,7 +2645,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="151"/>
+      <c r="A14" s="152"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2640,7 +2656,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
+      <c r="A15" s="152"/>
       <c r="B15" s="148" t="s">
         <v>186</v>
       </c>
@@ -2657,7 +2673,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="151"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
@@ -2700,7 +2716,7 @@
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="153" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2720,7 +2736,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
+      <c r="A20" s="152"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
@@ -2737,7 +2753,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="151"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="148" t="s">
         <v>218</v>
       </c>
@@ -2754,7 +2770,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="151"/>
+      <c r="A22" s="152"/>
       <c r="B22" s="148" t="s">
         <v>219</v>
       </c>
@@ -2777,7 +2793,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="151"/>
+      <c r="A23" s="152"/>
       <c r="B23" s="149" t="s">
         <v>226</v>
       </c>
@@ -2797,45 +2813,53 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="151"/>
+      <c r="A24" s="152"/>
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="C24" s="101"/>
+      <c r="C24" s="101">
+        <v>1975</v>
+      </c>
       <c r="D24" s="101">
         <v>2000</v>
       </c>
       <c r="E24" s="123">
         <f t="shared" ref="E24:E25" si="2">IF(AND(C24&gt;0,D24&gt;0), D24-C24, 0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="151"/>
+      <c r="A25" s="152"/>
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="101"/>
+      <c r="C25" s="101">
+        <v>2958</v>
+      </c>
       <c r="D25" s="101">
         <v>2990</v>
       </c>
       <c r="E25" s="123">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="151"/>
-      <c r="B26" s="214" t="s">
+      <c r="A26" s="152"/>
+      <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
+      <c r="C26" s="101">
+        <v>3853</v>
+      </c>
+      <c r="D26" s="101">
+        <v>3887</v>
+      </c>
       <c r="E26" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F26" s="105"/>
       <c r="H26" t="s">
@@ -2843,18 +2867,24 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="151"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
+      <c r="A27" s="152"/>
+      <c r="B27" s="215" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="101">
+        <v>5039</v>
+      </c>
+      <c r="D27" s="101">
+        <v>5079</v>
+      </c>
       <c r="E27" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="151"/>
+      <c r="A28" s="152"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2865,7 +2895,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="151"/>
+      <c r="A29" s="152"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2876,7 +2906,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="151"/>
+      <c r="A30" s="152"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2887,7 +2917,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="151"/>
+      <c r="A31" s="152"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2898,7 +2928,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="151"/>
+      <c r="A32" s="152"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2909,15 +2939,19 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="151"/>
+      <c r="A33" s="152"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
+      <c r="C33" s="99">
+        <v>5414</v>
+      </c>
+      <c r="D33" s="99">
+        <v>5454</v>
+      </c>
       <c r="E33" s="125">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F33" s="104"/>
     </row>
@@ -2930,25 +2964,25 @@
       </c>
       <c r="C34" s="103">
         <f>C33-C20</f>
-        <v>-806</v>
+        <v>4608</v>
       </c>
       <c r="D34" s="103">
         <f>D33-D20</f>
-        <v>-835</v>
+        <v>4619</v>
       </c>
       <c r="E34" s="126">
         <f>E33-E20</f>
-        <v>-29</v>
+        <v>11</v>
       </c>
       <c r="F34" s="108"/>
       <c r="G34" s="112">
         <f>E34</f>
-        <v>-29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150" t="s">
+    <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="151" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2967,32 +3001,42 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="151"/>
+    <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="152"/>
       <c r="B37" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
+      <c r="C37" s="99">
+        <v>5414</v>
+      </c>
+      <c r="D37" s="99">
+        <v>5454</v>
+      </c>
       <c r="E37" s="123">
         <f t="shared" ref="E37:E50" si="3">IF(AND(C37&gt;0,D37&gt;0), D37-C37, 0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F37" s="104"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="151"/>
-      <c r="B38" s="100"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
+    <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="152"/>
+      <c r="B38" s="215" t="s">
+        <v>229</v>
+      </c>
+      <c r="C38" s="101">
+        <v>5414</v>
+      </c>
+      <c r="D38" s="101">
+        <v>5454</v>
+      </c>
       <c r="E38" s="124">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F38" s="105"/>
     </row>
-    <row r="39" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="151"/>
+    <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="152"/>
       <c r="B39" s="100"/>
       <c r="C39" s="101"/>
       <c r="D39" s="101"/>
@@ -3002,8 +3046,8 @@
       </c>
       <c r="F39" s="105"/>
     </row>
-    <row r="40" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="151"/>
+    <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="152"/>
       <c r="B40" s="100"/>
       <c r="C40" s="101"/>
       <c r="D40" s="101"/>
@@ -3013,8 +3057,8 @@
       </c>
       <c r="F40" s="105"/>
     </row>
-    <row r="41" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="151"/>
+    <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="152"/>
       <c r="B41" s="100"/>
       <c r="C41" s="101"/>
       <c r="D41" s="101"/>
@@ -3024,8 +3068,8 @@
       </c>
       <c r="F41" s="105"/>
     </row>
-    <row r="42" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="151"/>
+    <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="152"/>
       <c r="B42" s="100"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -3035,8 +3079,8 @@
       </c>
       <c r="F42" s="105"/>
     </row>
-    <row r="43" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="151"/>
+    <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="152"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3046,8 +3090,8 @@
       </c>
       <c r="F43" s="105"/>
     </row>
-    <row r="44" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="151"/>
+    <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="152"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3057,8 +3101,8 @@
       </c>
       <c r="F44" s="105"/>
     </row>
-    <row r="45" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="151"/>
+    <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="152"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3068,8 +3112,8 @@
       </c>
       <c r="F45" s="105"/>
     </row>
-    <row r="46" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="151"/>
+    <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="152"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3079,8 +3123,8 @@
       </c>
       <c r="F46" s="105"/>
     </row>
-    <row r="47" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="151"/>
+    <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="152"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3090,8 +3134,8 @@
       </c>
       <c r="F47" s="105"/>
     </row>
-    <row r="48" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="151"/>
+    <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="152"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3101,8 +3145,8 @@
       </c>
       <c r="F48" s="105"/>
     </row>
-    <row r="49" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="151"/>
+    <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="152"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3112,8 +3156,8 @@
       </c>
       <c r="F49" s="105"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="151"/>
+    <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="152"/>
       <c r="B50" s="98" t="s">
         <v>187</v>
       </c>
@@ -3125,7 +3169,7 @@
       </c>
       <c r="F50" s="104"/>
     </row>
-    <row r="51" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="116">
         <v>2</v>
       </c>
@@ -3134,25 +3178,25 @@
       </c>
       <c r="C51" s="103">
         <f>C50-C37</f>
-        <v>0</v>
+        <v>-5414</v>
       </c>
       <c r="D51" s="103">
         <f>D50-D37</f>
-        <v>0</v>
+        <v>-5454</v>
       </c>
       <c r="E51" s="126">
         <f>E50-E37</f>
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="F51" s="107"/>
       <c r="G51" s="112">
         <f>E51</f>
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="152" t="s">
+      <c r="A53" s="153" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3172,7 +3216,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="151"/>
+      <c r="A54" s="152"/>
       <c r="B54" s="98" t="s">
         <v>184</v>
       </c>
@@ -3185,7 +3229,7 @@
       <c r="F54" s="104"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="151"/>
+      <c r="A55" s="152"/>
       <c r="B55" s="100"/>
       <c r="C55" s="101"/>
       <c r="D55" s="101"/>
@@ -3196,7 +3240,7 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="151"/>
+      <c r="A56" s="152"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3207,7 +3251,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="151"/>
+      <c r="A57" s="152"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3218,7 +3262,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="151"/>
+      <c r="A58" s="152"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3229,7 +3273,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="151"/>
+      <c r="A59" s="152"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3240,7 +3284,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="151"/>
+      <c r="A60" s="152"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3251,7 +3295,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="151"/>
+      <c r="A61" s="152"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3262,7 +3306,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="151"/>
+      <c r="A62" s="152"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3273,7 +3317,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="151"/>
+      <c r="A63" s="152"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3284,7 +3328,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="151"/>
+      <c r="A64" s="152"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3295,7 +3339,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="151"/>
+      <c r="A65" s="152"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3306,7 +3350,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="151"/>
+      <c r="A66" s="152"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3317,7 +3361,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="151"/>
+      <c r="A67" s="152"/>
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
@@ -3356,7 +3400,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="150" t="s">
+      <c r="A70" s="151" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3376,7 +3420,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="151"/>
+      <c r="A71" s="152"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
@@ -3389,7 +3433,7 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="151"/>
+      <c r="A72" s="152"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3400,7 +3444,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="151"/>
+      <c r="A73" s="152"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3411,7 +3455,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="151"/>
+      <c r="A74" s="152"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3422,7 +3466,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="151"/>
+      <c r="A75" s="152"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3433,7 +3477,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="151"/>
+      <c r="A76" s="152"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3444,7 +3488,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="151"/>
+      <c r="A77" s="152"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3455,7 +3499,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="151"/>
+      <c r="A78" s="152"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3466,7 +3510,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="151"/>
+      <c r="A79" s="152"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3477,7 +3521,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="151"/>
+      <c r="A80" s="152"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3488,7 +3532,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="151"/>
+      <c r="A81" s="152"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3499,7 +3543,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="151"/>
+      <c r="A82" s="152"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3510,7 +3554,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="151"/>
+      <c r="A83" s="152"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3521,7 +3565,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="151"/>
+      <c r="A84" s="152"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
@@ -3559,7 +3603,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="152" t="s">
+      <c r="A87" s="153" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3579,7 +3623,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="151"/>
+      <c r="A88" s="152"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
@@ -3592,7 +3636,7 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="151"/>
+      <c r="A89" s="152"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3603,7 +3647,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="151"/>
+      <c r="A90" s="152"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3614,7 +3658,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="151"/>
+      <c r="A91" s="152"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3625,7 +3669,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="151"/>
+      <c r="A92" s="152"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3636,7 +3680,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="151"/>
+      <c r="A93" s="152"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3647,7 +3691,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="151"/>
+      <c r="A94" s="152"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3658,7 +3702,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="151"/>
+      <c r="A95" s="152"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3669,7 +3713,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="151"/>
+      <c r="A96" s="152"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3680,7 +3724,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="151"/>
+      <c r="A97" s="152"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3691,7 +3735,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="151"/>
+      <c r="A98" s="152"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3702,7 +3746,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="151"/>
+      <c r="A99" s="152"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3713,7 +3757,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="151"/>
+      <c r="A100" s="152"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3724,7 +3768,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="151"/>
+      <c r="A101" s="152"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
       </c>
@@ -3738,7 +3782,7 @@
     </row>
     <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="150" t="s">
+      <c r="A103" s="151" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="113" t="s">
@@ -3758,7 +3802,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="151"/>
+      <c r="A104" s="152"/>
       <c r="B104" s="98" t="s">
         <v>184</v>
       </c>
@@ -3771,7 +3815,7 @@
       <c r="F104" s="104"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="151"/>
+      <c r="A105" s="152"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3782,7 +3826,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="151"/>
+      <c r="A106" s="152"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3793,7 +3837,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="151"/>
+      <c r="A107" s="152"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3804,7 +3848,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="151"/>
+      <c r="A108" s="152"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3815,7 +3859,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="151"/>
+      <c r="A109" s="152"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3826,7 +3870,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="151"/>
+      <c r="A110" s="152"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3837,7 +3881,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="151"/>
+      <c r="A111" s="152"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3848,7 +3892,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="151"/>
+      <c r="A112" s="152"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3859,7 +3903,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="151"/>
+      <c r="A113" s="152"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3870,7 +3914,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="151"/>
+      <c r="A114" s="152"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3881,7 +3925,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="151"/>
+      <c r="A115" s="152"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3892,7 +3936,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="151"/>
+      <c r="A116" s="152"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3903,7 +3947,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="151"/>
+      <c r="A117" s="152"/>
       <c r="B117" s="98" t="s">
         <v>187</v>
       </c>
@@ -3917,7 +3961,7 @@
     </row>
     <row r="118" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="119" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="152" t="s">
+      <c r="A119" s="153" t="s">
         <v>175</v>
       </c>
       <c r="B119" s="109" t="s">
@@ -3937,7 +3981,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="151"/>
+      <c r="A120" s="152"/>
       <c r="B120" s="98" t="s">
         <v>184</v>
       </c>
@@ -3950,7 +3994,7 @@
       <c r="F120" s="104"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="151"/>
+      <c r="A121" s="152"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -3961,7 +4005,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="151"/>
+      <c r="A122" s="152"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -3972,7 +4016,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="151"/>
+      <c r="A123" s="152"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -3983,7 +4027,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="151"/>
+      <c r="A124" s="152"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -3994,7 +4038,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="151"/>
+      <c r="A125" s="152"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4005,7 +4049,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="151"/>
+      <c r="A126" s="152"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4016,7 +4060,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="151"/>
+      <c r="A127" s="152"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4027,7 +4071,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="151"/>
+      <c r="A128" s="152"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4038,7 +4082,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="151"/>
+      <c r="A129" s="152"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4049,7 +4093,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="151"/>
+      <c r="A130" s="152"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4060,7 +4104,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="151"/>
+      <c r="A131" s="152"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4071,7 +4115,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="151"/>
+      <c r="A132" s="152"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4082,7 +4126,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="151"/>
+      <c r="A133" s="152"/>
       <c r="B133" s="98" t="s">
         <v>187</v>
       </c>
@@ -4096,7 +4140,7 @@
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A135" s="150" t="s">
+      <c r="A135" s="151" t="s">
         <v>176</v>
       </c>
       <c r="B135" s="113" t="s">
@@ -4116,7 +4160,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="151"/>
+      <c r="A136" s="152"/>
       <c r="B136" s="98" t="s">
         <v>184</v>
       </c>
@@ -4129,7 +4173,7 @@
       <c r="F136" s="104"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="151"/>
+      <c r="A137" s="152"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4140,7 +4184,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A138" s="151"/>
+      <c r="A138" s="152"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4151,7 +4195,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A139" s="151"/>
+      <c r="A139" s="152"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4162,7 +4206,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A140" s="151"/>
+      <c r="A140" s="152"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4173,7 +4217,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A141" s="151"/>
+      <c r="A141" s="152"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4184,7 +4228,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="151"/>
+      <c r="A142" s="152"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4195,7 +4239,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A143" s="151"/>
+      <c r="A143" s="152"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4206,7 +4250,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="151"/>
+      <c r="A144" s="152"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4217,7 +4261,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="151"/>
+      <c r="A145" s="152"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4228,7 +4272,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="151"/>
+      <c r="A146" s="152"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4239,7 +4283,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="151"/>
+      <c r="A147" s="152"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4250,7 +4294,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="151"/>
+      <c r="A148" s="152"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4261,7 +4305,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="151"/>
+      <c r="A149" s="152"/>
       <c r="B149" s="98" t="s">
         <v>187</v>
       </c>
@@ -4276,6 +4320,11 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4284,11 +4333,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4320,13 +4364,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4356,18 +4400,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4519,9 +4563,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="162"/>
+      <c r="C21" s="165"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4672,9 +4716,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4825,9 +4869,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="159"/>
-      <c r="D55" s="160"/>
-      <c r="E55" s="160"/>
+      <c r="C55" s="163"/>
+      <c r="D55" s="164"/>
+      <c r="E55" s="164"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -4978,9 +5022,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="159"/>
-      <c r="D72" s="160"/>
-      <c r="E72" s="160"/>
+      <c r="C72" s="163"/>
+      <c r="D72" s="164"/>
+      <c r="E72" s="164"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5131,9 +5175,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="159"/>
-      <c r="D89" s="160"/>
-      <c r="E89" s="160"/>
+      <c r="C89" s="163"/>
+      <c r="D89" s="164"/>
+      <c r="E89" s="164"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5284,9 +5328,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="159"/>
-      <c r="D106" s="160"/>
-      <c r="E106" s="160"/>
+      <c r="C106" s="163"/>
+      <c r="D106" s="164"/>
+      <c r="E106" s="164"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5437,9 +5481,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="159"/>
-      <c r="D123" s="160"/>
-      <c r="E123" s="160"/>
+      <c r="C123" s="163"/>
+      <c r="D123" s="164"/>
+      <c r="E123" s="164"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5590,9 +5634,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="159"/>
-      <c r="D140" s="160"/>
-      <c r="E140" s="160"/>
+      <c r="C140" s="163"/>
+      <c r="D140" s="164"/>
+      <c r="E140" s="164"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5743,9 +5787,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="159"/>
-      <c r="D157" s="160"/>
-      <c r="E157" s="160"/>
+      <c r="C157" s="163"/>
+      <c r="D157" s="164"/>
+      <c r="E157" s="164"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5896,9 +5940,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="159"/>
-      <c r="D174" s="160"/>
-      <c r="E174" s="160"/>
+      <c r="C174" s="163"/>
+      <c r="D174" s="164"/>
+      <c r="E174" s="164"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6049,9 +6093,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="159"/>
-      <c r="D191" s="160"/>
-      <c r="E191" s="160"/>
+      <c r="C191" s="163"/>
+      <c r="D191" s="164"/>
+      <c r="E191" s="164"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6202,9 +6246,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="159"/>
-      <c r="D208" s="160"/>
-      <c r="E208" s="160"/>
+      <c r="C208" s="163"/>
+      <c r="D208" s="164"/>
+      <c r="E208" s="164"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6355,9 +6399,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="159"/>
-      <c r="D225" s="160"/>
-      <c r="E225" s="160"/>
+      <c r="C225" s="163"/>
+      <c r="D225" s="164"/>
+      <c r="E225" s="164"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6508,9 +6552,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="159"/>
-      <c r="D242" s="160"/>
-      <c r="E242" s="160"/>
+      <c r="C242" s="163"/>
+      <c r="D242" s="164"/>
+      <c r="E242" s="164"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6661,9 +6705,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="159"/>
-      <c r="D259" s="160"/>
-      <c r="E259" s="160"/>
+      <c r="C259" s="163"/>
+      <c r="D259" s="164"/>
+      <c r="E259" s="164"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6814,18 +6858,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="175"/>
-      <c r="D276" s="176"/>
-      <c r="E276" s="176"/>
+      <c r="C276" s="167"/>
+      <c r="D276" s="168"/>
+      <c r="E276" s="168"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="159"/>
-      <c r="D277" s="160"/>
-      <c r="E277" s="160"/>
+      <c r="C277" s="163"/>
+      <c r="D277" s="164"/>
+      <c r="E277" s="164"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -6976,9 +7020,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="161"/>
-      <c r="D294" s="162"/>
-      <c r="E294" s="162"/>
+      <c r="C294" s="165"/>
+      <c r="D294" s="166"/>
+      <c r="E294" s="166"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7129,9 +7173,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="159"/>
-      <c r="D311" s="160"/>
-      <c r="E311" s="160"/>
+      <c r="C311" s="163"/>
+      <c r="D311" s="164"/>
+      <c r="E311" s="164"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7282,9 +7326,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="159"/>
-      <c r="D328" s="160"/>
-      <c r="E328" s="160"/>
+      <c r="C328" s="163"/>
+      <c r="D328" s="164"/>
+      <c r="E328" s="164"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7435,9 +7479,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="159"/>
-      <c r="D345" s="160"/>
-      <c r="E345" s="160"/>
+      <c r="C345" s="163"/>
+      <c r="D345" s="164"/>
+      <c r="E345" s="164"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7588,9 +7632,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="159"/>
-      <c r="D362" s="160"/>
-      <c r="E362" s="160"/>
+      <c r="C362" s="163"/>
+      <c r="D362" s="164"/>
+      <c r="E362" s="164"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7741,9 +7785,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="159"/>
-      <c r="D379" s="160"/>
-      <c r="E379" s="160"/>
+      <c r="C379" s="163"/>
+      <c r="D379" s="164"/>
+      <c r="E379" s="164"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7894,9 +7938,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="159"/>
-      <c r="D396" s="160"/>
-      <c r="E396" s="160"/>
+      <c r="C396" s="163"/>
+      <c r="D396" s="164"/>
+      <c r="E396" s="164"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8047,9 +8091,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="159"/>
-      <c r="D413" s="160"/>
-      <c r="E413" s="160"/>
+      <c r="C413" s="163"/>
+      <c r="D413" s="164"/>
+      <c r="E413" s="164"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8200,9 +8244,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="159"/>
-      <c r="D430" s="160"/>
-      <c r="E430" s="160"/>
+      <c r="C430" s="163"/>
+      <c r="D430" s="164"/>
+      <c r="E430" s="164"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8353,9 +8397,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="159"/>
-      <c r="D447" s="160"/>
-      <c r="E447" s="160"/>
+      <c r="C447" s="163"/>
+      <c r="D447" s="164"/>
+      <c r="E447" s="164"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8506,9 +8550,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="159"/>
-      <c r="D464" s="160"/>
-      <c r="E464" s="160"/>
+      <c r="C464" s="163"/>
+      <c r="D464" s="164"/>
+      <c r="E464" s="164"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8659,9 +8703,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="159"/>
-      <c r="D481" s="160"/>
-      <c r="E481" s="160"/>
+      <c r="C481" s="163"/>
+      <c r="D481" s="164"/>
+      <c r="E481" s="164"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8812,9 +8856,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="159"/>
-      <c r="D498" s="160"/>
-      <c r="E498" s="160"/>
+      <c r="C498" s="163"/>
+      <c r="D498" s="164"/>
+      <c r="E498" s="164"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -8965,9 +9009,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="159"/>
-      <c r="D515" s="160"/>
-      <c r="E515" s="160"/>
+      <c r="C515" s="163"/>
+      <c r="D515" s="164"/>
+      <c r="E515" s="164"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9118,9 +9162,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="159"/>
-      <c r="D532" s="160"/>
-      <c r="E532" s="160"/>
+      <c r="C532" s="163"/>
+      <c r="D532" s="164"/>
+      <c r="E532" s="164"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9271,18 +9315,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="173"/>
-      <c r="D549" s="174"/>
-      <c r="E549" s="174"/>
+      <c r="C549" s="169"/>
+      <c r="D549" s="170"/>
+      <c r="E549" s="170"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="159"/>
-      <c r="D550" s="160"/>
-      <c r="E550" s="160"/>
+      <c r="C550" s="163"/>
+      <c r="D550" s="164"/>
+      <c r="E550" s="164"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9433,9 +9477,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="161"/>
-      <c r="D567" s="162"/>
-      <c r="E567" s="162"/>
+      <c r="C567" s="165"/>
+      <c r="D567" s="166"/>
+      <c r="E567" s="166"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9586,9 +9630,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="159"/>
-      <c r="D584" s="160"/>
-      <c r="E584" s="160"/>
+      <c r="C584" s="163"/>
+      <c r="D584" s="164"/>
+      <c r="E584" s="164"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9739,9 +9783,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="159"/>
-      <c r="D601" s="160"/>
-      <c r="E601" s="160"/>
+      <c r="C601" s="163"/>
+      <c r="D601" s="164"/>
+      <c r="E601" s="164"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9892,9 +9936,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="159"/>
-      <c r="D618" s="160"/>
-      <c r="E618" s="160"/>
+      <c r="C618" s="163"/>
+      <c r="D618" s="164"/>
+      <c r="E618" s="164"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10045,9 +10089,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="159"/>
-      <c r="D635" s="160"/>
-      <c r="E635" s="160"/>
+      <c r="C635" s="163"/>
+      <c r="D635" s="164"/>
+      <c r="E635" s="164"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10198,9 +10242,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="159"/>
-      <c r="D652" s="160"/>
-      <c r="E652" s="160"/>
+      <c r="C652" s="163"/>
+      <c r="D652" s="164"/>
+      <c r="E652" s="164"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10351,9 +10395,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="159"/>
-      <c r="D669" s="160"/>
-      <c r="E669" s="160"/>
+      <c r="C669" s="163"/>
+      <c r="D669" s="164"/>
+      <c r="E669" s="164"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10504,9 +10548,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="159"/>
-      <c r="D686" s="160"/>
-      <c r="E686" s="160"/>
+      <c r="C686" s="163"/>
+      <c r="D686" s="164"/>
+      <c r="E686" s="164"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10657,9 +10701,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="159"/>
-      <c r="D703" s="160"/>
-      <c r="E703" s="160"/>
+      <c r="C703" s="163"/>
+      <c r="D703" s="164"/>
+      <c r="E703" s="164"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10810,9 +10854,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="159"/>
-      <c r="D720" s="160"/>
-      <c r="E720" s="160"/>
+      <c r="C720" s="163"/>
+      <c r="D720" s="164"/>
+      <c r="E720" s="164"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -10963,9 +11007,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="159"/>
-      <c r="D737" s="160"/>
-      <c r="E737" s="160"/>
+      <c r="C737" s="163"/>
+      <c r="D737" s="164"/>
+      <c r="E737" s="164"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11116,9 +11160,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="159"/>
-      <c r="D754" s="160"/>
-      <c r="E754" s="160"/>
+      <c r="C754" s="163"/>
+      <c r="D754" s="164"/>
+      <c r="E754" s="164"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11269,9 +11313,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="159"/>
-      <c r="D771" s="160"/>
-      <c r="E771" s="160"/>
+      <c r="C771" s="163"/>
+      <c r="D771" s="164"/>
+      <c r="E771" s="164"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11422,9 +11466,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="159"/>
-      <c r="D788" s="160"/>
-      <c r="E788" s="160"/>
+      <c r="C788" s="163"/>
+      <c r="D788" s="164"/>
+      <c r="E788" s="164"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11575,9 +11619,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="159"/>
-      <c r="D805" s="160"/>
-      <c r="E805" s="160"/>
+      <c r="C805" s="163"/>
+      <c r="D805" s="164"/>
+      <c r="E805" s="164"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11737,9 +11781,9 @@
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="159"/>
-      <c r="D823" s="160"/>
-      <c r="E823" s="160"/>
+      <c r="C823" s="163"/>
+      <c r="D823" s="164"/>
+      <c r="E823" s="164"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11890,9 +11934,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="161"/>
-      <c r="D840" s="162"/>
-      <c r="E840" s="162"/>
+      <c r="C840" s="165"/>
+      <c r="D840" s="166"/>
+      <c r="E840" s="166"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12043,9 +12087,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="159"/>
-      <c r="D857" s="160"/>
-      <c r="E857" s="160"/>
+      <c r="C857" s="163"/>
+      <c r="D857" s="164"/>
+      <c r="E857" s="164"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12196,9 +12240,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="159"/>
-      <c r="D874" s="160"/>
-      <c r="E874" s="160"/>
+      <c r="C874" s="163"/>
+      <c r="D874" s="164"/>
+      <c r="E874" s="164"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12349,9 +12393,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="159"/>
-      <c r="D891" s="160"/>
-      <c r="E891" s="160"/>
+      <c r="C891" s="163"/>
+      <c r="D891" s="164"/>
+      <c r="E891" s="164"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12502,9 +12546,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="159"/>
-      <c r="D908" s="160"/>
-      <c r="E908" s="160"/>
+      <c r="C908" s="163"/>
+      <c r="D908" s="164"/>
+      <c r="E908" s="164"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12655,9 +12699,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="159"/>
-      <c r="D925" s="160"/>
-      <c r="E925" s="160"/>
+      <c r="C925" s="163"/>
+      <c r="D925" s="164"/>
+      <c r="E925" s="164"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12808,9 +12852,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="159"/>
-      <c r="D942" s="160"/>
-      <c r="E942" s="160"/>
+      <c r="C942" s="163"/>
+      <c r="D942" s="164"/>
+      <c r="E942" s="164"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -12961,9 +13005,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="159"/>
-      <c r="D959" s="160"/>
-      <c r="E959" s="160"/>
+      <c r="C959" s="163"/>
+      <c r="D959" s="164"/>
+      <c r="E959" s="164"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13114,9 +13158,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="159"/>
-      <c r="D976" s="160"/>
-      <c r="E976" s="160"/>
+      <c r="C976" s="163"/>
+      <c r="D976" s="164"/>
+      <c r="E976" s="164"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13267,9 +13311,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="159"/>
-      <c r="D993" s="160"/>
-      <c r="E993" s="160"/>
+      <c r="C993" s="163"/>
+      <c r="D993" s="164"/>
+      <c r="E993" s="164"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13420,9 +13464,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="159"/>
-      <c r="D1010" s="160"/>
-      <c r="E1010" s="160"/>
+      <c r="C1010" s="163"/>
+      <c r="D1010" s="164"/>
+      <c r="E1010" s="164"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13573,9 +13617,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="159"/>
-      <c r="D1027" s="160"/>
-      <c r="E1027" s="160"/>
+      <c r="C1027" s="163"/>
+      <c r="D1027" s="164"/>
+      <c r="E1027" s="164"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13726,9 +13770,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="159"/>
-      <c r="D1044" s="160"/>
-      <c r="E1044" s="160"/>
+      <c r="C1044" s="163"/>
+      <c r="D1044" s="164"/>
+      <c r="E1044" s="164"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13879,9 +13923,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="159"/>
-      <c r="D1061" s="160"/>
-      <c r="E1061" s="160"/>
+      <c r="C1061" s="163"/>
+      <c r="D1061" s="164"/>
+      <c r="E1061" s="164"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14032,9 +14076,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="159"/>
-      <c r="D1078" s="160"/>
-      <c r="E1078" s="160"/>
+      <c r="C1078" s="163"/>
+      <c r="D1078" s="164"/>
+      <c r="E1078" s="164"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14185,18 +14229,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="169"/>
-      <c r="D1095" s="170"/>
-      <c r="E1095" s="170"/>
+      <c r="C1095" s="173"/>
+      <c r="D1095" s="174"/>
+      <c r="E1095" s="174"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="159"/>
-      <c r="D1096" s="160"/>
-      <c r="E1096" s="160"/>
+      <c r="C1096" s="163"/>
+      <c r="D1096" s="164"/>
+      <c r="E1096" s="164"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14347,9 +14391,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="161"/>
-      <c r="D1113" s="162"/>
-      <c r="E1113" s="162"/>
+      <c r="C1113" s="165"/>
+      <c r="D1113" s="166"/>
+      <c r="E1113" s="166"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14500,9 +14544,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="159"/>
-      <c r="D1130" s="160"/>
-      <c r="E1130" s="160"/>
+      <c r="C1130" s="163"/>
+      <c r="D1130" s="164"/>
+      <c r="E1130" s="164"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14653,9 +14697,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="159"/>
-      <c r="D1147" s="160"/>
-      <c r="E1147" s="160"/>
+      <c r="C1147" s="163"/>
+      <c r="D1147" s="164"/>
+      <c r="E1147" s="164"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14806,9 +14850,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="159"/>
-      <c r="D1164" s="160"/>
-      <c r="E1164" s="160"/>
+      <c r="C1164" s="163"/>
+      <c r="D1164" s="164"/>
+      <c r="E1164" s="164"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -14959,9 +15003,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="159"/>
-      <c r="D1181" s="160"/>
-      <c r="E1181" s="160"/>
+      <c r="C1181" s="163"/>
+      <c r="D1181" s="164"/>
+      <c r="E1181" s="164"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15112,9 +15156,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="159"/>
-      <c r="D1198" s="160"/>
-      <c r="E1198" s="160"/>
+      <c r="C1198" s="163"/>
+      <c r="D1198" s="164"/>
+      <c r="E1198" s="164"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15265,9 +15309,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="159"/>
-      <c r="D1215" s="160"/>
-      <c r="E1215" s="160"/>
+      <c r="C1215" s="163"/>
+      <c r="D1215" s="164"/>
+      <c r="E1215" s="164"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15418,9 +15462,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="159"/>
-      <c r="D1232" s="160"/>
-      <c r="E1232" s="160"/>
+      <c r="C1232" s="163"/>
+      <c r="D1232" s="164"/>
+      <c r="E1232" s="164"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15571,9 +15615,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="159"/>
-      <c r="D1249" s="160"/>
-      <c r="E1249" s="160"/>
+      <c r="C1249" s="163"/>
+      <c r="D1249" s="164"/>
+      <c r="E1249" s="164"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15724,9 +15768,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="159"/>
-      <c r="D1266" s="160"/>
-      <c r="E1266" s="160"/>
+      <c r="C1266" s="163"/>
+      <c r="D1266" s="164"/>
+      <c r="E1266" s="164"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15877,9 +15921,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="159"/>
-      <c r="D1283" s="160"/>
-      <c r="E1283" s="160"/>
+      <c r="C1283" s="163"/>
+      <c r="D1283" s="164"/>
+      <c r="E1283" s="164"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16030,9 +16074,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="159"/>
-      <c r="D1300" s="160"/>
-      <c r="E1300" s="160"/>
+      <c r="C1300" s="163"/>
+      <c r="D1300" s="164"/>
+      <c r="E1300" s="164"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16183,9 +16227,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="159"/>
-      <c r="D1317" s="160"/>
-      <c r="E1317" s="160"/>
+      <c r="C1317" s="163"/>
+      <c r="D1317" s="164"/>
+      <c r="E1317" s="164"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16336,9 +16380,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="159"/>
-      <c r="D1334" s="160"/>
-      <c r="E1334" s="160"/>
+      <c r="C1334" s="163"/>
+      <c r="D1334" s="164"/>
+      <c r="E1334" s="164"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16489,9 +16533,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="159"/>
-      <c r="D1351" s="160"/>
-      <c r="E1351" s="160"/>
+      <c r="C1351" s="163"/>
+      <c r="D1351" s="164"/>
+      <c r="E1351" s="164"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16642,18 +16686,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="167"/>
-      <c r="D1368" s="168"/>
-      <c r="E1368" s="168"/>
+      <c r="C1368" s="175"/>
+      <c r="D1368" s="176"/>
+      <c r="E1368" s="176"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="159"/>
-      <c r="D1369" s="160"/>
-      <c r="E1369" s="160"/>
+      <c r="C1369" s="163"/>
+      <c r="D1369" s="164"/>
+      <c r="E1369" s="164"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16804,9 +16848,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="161"/>
-      <c r="D1386" s="162"/>
-      <c r="E1386" s="162"/>
+      <c r="C1386" s="165"/>
+      <c r="D1386" s="166"/>
+      <c r="E1386" s="166"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -16957,9 +17001,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="159"/>
-      <c r="D1403" s="160"/>
-      <c r="E1403" s="160"/>
+      <c r="C1403" s="163"/>
+      <c r="D1403" s="164"/>
+      <c r="E1403" s="164"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17110,9 +17154,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="159"/>
-      <c r="D1420" s="160"/>
-      <c r="E1420" s="160"/>
+      <c r="C1420" s="163"/>
+      <c r="D1420" s="164"/>
+      <c r="E1420" s="164"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17263,9 +17307,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="159"/>
-      <c r="D1437" s="160"/>
-      <c r="E1437" s="160"/>
+      <c r="C1437" s="163"/>
+      <c r="D1437" s="164"/>
+      <c r="E1437" s="164"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17416,9 +17460,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="159"/>
-      <c r="D1454" s="160"/>
-      <c r="E1454" s="160"/>
+      <c r="C1454" s="163"/>
+      <c r="D1454" s="164"/>
+      <c r="E1454" s="164"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17569,9 +17613,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="159"/>
-      <c r="D1471" s="160"/>
-      <c r="E1471" s="160"/>
+      <c r="C1471" s="163"/>
+      <c r="D1471" s="164"/>
+      <c r="E1471" s="164"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17722,9 +17766,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="159"/>
-      <c r="D1488" s="160"/>
-      <c r="E1488" s="160"/>
+      <c r="C1488" s="163"/>
+      <c r="D1488" s="164"/>
+      <c r="E1488" s="164"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17875,9 +17919,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="159"/>
-      <c r="D1505" s="160"/>
-      <c r="E1505" s="160"/>
+      <c r="C1505" s="163"/>
+      <c r="D1505" s="164"/>
+      <c r="E1505" s="164"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18028,9 +18072,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="159"/>
-      <c r="D1522" s="160"/>
-      <c r="E1522" s="160"/>
+      <c r="C1522" s="163"/>
+      <c r="D1522" s="164"/>
+      <c r="E1522" s="164"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18181,9 +18225,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="159"/>
-      <c r="D1539" s="160"/>
-      <c r="E1539" s="160"/>
+      <c r="C1539" s="163"/>
+      <c r="D1539" s="164"/>
+      <c r="E1539" s="164"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18334,9 +18378,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="159"/>
-      <c r="D1556" s="160"/>
-      <c r="E1556" s="160"/>
+      <c r="C1556" s="163"/>
+      <c r="D1556" s="164"/>
+      <c r="E1556" s="164"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18487,9 +18531,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="159"/>
-      <c r="D1573" s="160"/>
-      <c r="E1573" s="160"/>
+      <c r="C1573" s="163"/>
+      <c r="D1573" s="164"/>
+      <c r="E1573" s="164"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18640,9 +18684,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="159"/>
-      <c r="D1590" s="160"/>
-      <c r="E1590" s="160"/>
+      <c r="C1590" s="163"/>
+      <c r="D1590" s="164"/>
+      <c r="E1590" s="164"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18793,9 +18837,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="159"/>
-      <c r="D1607" s="160"/>
-      <c r="E1607" s="160"/>
+      <c r="C1607" s="163"/>
+      <c r="D1607" s="164"/>
+      <c r="E1607" s="164"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18946,9 +18990,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="159"/>
-      <c r="D1624" s="160"/>
-      <c r="E1624" s="160"/>
+      <c r="C1624" s="163"/>
+      <c r="D1624" s="164"/>
+      <c r="E1624" s="164"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19099,18 +19143,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="165"/>
-      <c r="D1641" s="166"/>
-      <c r="E1641" s="166"/>
+      <c r="C1641" s="177"/>
+      <c r="D1641" s="178"/>
+      <c r="E1641" s="178"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="159"/>
-      <c r="D1642" s="160"/>
-      <c r="E1642" s="160"/>
+      <c r="C1642" s="163"/>
+      <c r="D1642" s="164"/>
+      <c r="E1642" s="164"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19261,9 +19305,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="161"/>
-      <c r="D1659" s="162"/>
-      <c r="E1659" s="162"/>
+      <c r="C1659" s="165"/>
+      <c r="D1659" s="166"/>
+      <c r="E1659" s="166"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19414,9 +19458,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="159"/>
-      <c r="D1676" s="160"/>
-      <c r="E1676" s="160"/>
+      <c r="C1676" s="163"/>
+      <c r="D1676" s="164"/>
+      <c r="E1676" s="164"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19567,9 +19611,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="159"/>
-      <c r="D1693" s="160"/>
-      <c r="E1693" s="160"/>
+      <c r="C1693" s="163"/>
+      <c r="D1693" s="164"/>
+      <c r="E1693" s="164"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19720,9 +19764,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="159"/>
-      <c r="D1710" s="160"/>
-      <c r="E1710" s="160"/>
+      <c r="C1710" s="163"/>
+      <c r="D1710" s="164"/>
+      <c r="E1710" s="164"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19873,9 +19917,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="159"/>
-      <c r="D1727" s="160"/>
-      <c r="E1727" s="160"/>
+      <c r="C1727" s="163"/>
+      <c r="D1727" s="164"/>
+      <c r="E1727" s="164"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20026,9 +20070,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="159"/>
-      <c r="D1744" s="160"/>
-      <c r="E1744" s="160"/>
+      <c r="C1744" s="163"/>
+      <c r="D1744" s="164"/>
+      <c r="E1744" s="164"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20179,9 +20223,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="159"/>
-      <c r="D1761" s="160"/>
-      <c r="E1761" s="160"/>
+      <c r="C1761" s="163"/>
+      <c r="D1761" s="164"/>
+      <c r="E1761" s="164"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20332,9 +20376,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="159"/>
-      <c r="D1778" s="160"/>
-      <c r="E1778" s="160"/>
+      <c r="C1778" s="163"/>
+      <c r="D1778" s="164"/>
+      <c r="E1778" s="164"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20485,9 +20529,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="159"/>
-      <c r="D1795" s="160"/>
-      <c r="E1795" s="160"/>
+      <c r="C1795" s="163"/>
+      <c r="D1795" s="164"/>
+      <c r="E1795" s="164"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20638,9 +20682,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="159"/>
-      <c r="D1812" s="160"/>
-      <c r="E1812" s="160"/>
+      <c r="C1812" s="163"/>
+      <c r="D1812" s="164"/>
+      <c r="E1812" s="164"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20791,9 +20835,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="159"/>
-      <c r="D1829" s="160"/>
-      <c r="E1829" s="160"/>
+      <c r="C1829" s="163"/>
+      <c r="D1829" s="164"/>
+      <c r="E1829" s="164"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20944,9 +20988,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="159"/>
-      <c r="D1846" s="160"/>
-      <c r="E1846" s="160"/>
+      <c r="C1846" s="163"/>
+      <c r="D1846" s="164"/>
+      <c r="E1846" s="164"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21097,9 +21141,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="159"/>
-      <c r="D1863" s="160"/>
-      <c r="E1863" s="160"/>
+      <c r="C1863" s="163"/>
+      <c r="D1863" s="164"/>
+      <c r="E1863" s="164"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21250,9 +21294,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="159"/>
-      <c r="D1880" s="160"/>
-      <c r="E1880" s="160"/>
+      <c r="C1880" s="163"/>
+      <c r="D1880" s="164"/>
+      <c r="E1880" s="164"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21403,9 +21447,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="159"/>
-      <c r="D1897" s="160"/>
-      <c r="E1897" s="160"/>
+      <c r="C1897" s="163"/>
+      <c r="D1897" s="164"/>
+      <c r="E1897" s="164"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21556,18 +21600,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="163"/>
-      <c r="D1914" s="164"/>
-      <c r="E1914" s="164"/>
+      <c r="C1914" s="179"/>
+      <c r="D1914" s="180"/>
+      <c r="E1914" s="180"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="159"/>
-      <c r="D1915" s="160"/>
-      <c r="E1915" s="160"/>
+      <c r="C1915" s="163"/>
+      <c r="D1915" s="164"/>
+      <c r="E1915" s="164"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21718,9 +21762,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="161"/>
-      <c r="D1932" s="162"/>
-      <c r="E1932" s="162"/>
+      <c r="C1932" s="165"/>
+      <c r="D1932" s="166"/>
+      <c r="E1932" s="166"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21871,9 +21915,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="159"/>
-      <c r="D1949" s="160"/>
-      <c r="E1949" s="160"/>
+      <c r="C1949" s="163"/>
+      <c r="D1949" s="164"/>
+      <c r="E1949" s="164"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22024,9 +22068,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="159"/>
-      <c r="D1966" s="160"/>
-      <c r="E1966" s="160"/>
+      <c r="C1966" s="163"/>
+      <c r="D1966" s="164"/>
+      <c r="E1966" s="164"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22177,9 +22221,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="159"/>
-      <c r="D1983" s="160"/>
-      <c r="E1983" s="160"/>
+      <c r="C1983" s="163"/>
+      <c r="D1983" s="164"/>
+      <c r="E1983" s="164"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22330,9 +22374,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="159"/>
-      <c r="D2000" s="160"/>
-      <c r="E2000" s="160"/>
+      <c r="C2000" s="163"/>
+      <c r="D2000" s="164"/>
+      <c r="E2000" s="164"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22483,9 +22527,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="159"/>
-      <c r="D2017" s="160"/>
-      <c r="E2017" s="160"/>
+      <c r="C2017" s="163"/>
+      <c r="D2017" s="164"/>
+      <c r="E2017" s="164"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22636,9 +22680,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="159"/>
-      <c r="D2034" s="160"/>
-      <c r="E2034" s="160"/>
+      <c r="C2034" s="163"/>
+      <c r="D2034" s="164"/>
+      <c r="E2034" s="164"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22789,9 +22833,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="159"/>
-      <c r="D2051" s="160"/>
-      <c r="E2051" s="160"/>
+      <c r="C2051" s="163"/>
+      <c r="D2051" s="164"/>
+      <c r="E2051" s="164"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22942,9 +22986,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="159"/>
-      <c r="D2068" s="160"/>
-      <c r="E2068" s="160"/>
+      <c r="C2068" s="163"/>
+      <c r="D2068" s="164"/>
+      <c r="E2068" s="164"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23095,9 +23139,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="159"/>
-      <c r="D2085" s="160"/>
-      <c r="E2085" s="160"/>
+      <c r="C2085" s="163"/>
+      <c r="D2085" s="164"/>
+      <c r="E2085" s="164"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23248,9 +23292,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="159"/>
-      <c r="D2102" s="160"/>
-      <c r="E2102" s="160"/>
+      <c r="C2102" s="163"/>
+      <c r="D2102" s="164"/>
+      <c r="E2102" s="164"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23401,9 +23445,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="159"/>
-      <c r="D2119" s="160"/>
-      <c r="E2119" s="160"/>
+      <c r="C2119" s="163"/>
+      <c r="D2119" s="164"/>
+      <c r="E2119" s="164"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23554,9 +23598,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="159"/>
-      <c r="D2136" s="160"/>
-      <c r="E2136" s="160"/>
+      <c r="C2136" s="163"/>
+      <c r="D2136" s="164"/>
+      <c r="E2136" s="164"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23707,9 +23751,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="159"/>
-      <c r="D2153" s="160"/>
-      <c r="E2153" s="160"/>
+      <c r="C2153" s="163"/>
+      <c r="D2153" s="164"/>
+      <c r="E2153" s="164"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23860,9 +23904,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="159"/>
-      <c r="D2170" s="160"/>
-      <c r="E2170" s="160"/>
+      <c r="C2170" s="163"/>
+      <c r="D2170" s="164"/>
+      <c r="E2170" s="164"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24010,26 +24054,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24042,113 +24171,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24173,51 +24217,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="187"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="184" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="185"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="181" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="182"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="183"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24434,19 +24478,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="180" t="s">
+      <c r="A20" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="183"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24663,19 +24707,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
+      <c r="B37" s="182"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
+      <c r="K37" s="183"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -24899,7 +24943,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24933,28 +24977,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="187"/>
+      <c r="A3" s="188"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="188"/>
+      <c r="A4" s="189"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="188"/>
+      <c r="A5" s="189"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="188"/>
+      <c r="A6" s="189"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="188"/>
+      <c r="A7" s="189"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="188"/>
+      <c r="A8" s="189"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="188"/>
+      <c r="A9" s="189"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="189"/>
+      <c r="A10" s="190"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25110,7 +25154,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25137,10 +25181,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="191" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="191"/>
+      <c r="C1" s="192"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25151,7 +25195,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="193" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25165,7 +25209,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="193"/>
+      <c r="A4" s="194"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25177,7 +25221,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="193"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25186,7 +25230,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="193"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="139" t="s">
         <v>212</v>
       </c>
@@ -25198,7 +25242,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="193"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25210,7 +25254,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="193"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25219,7 +25263,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="194"/>
+      <c r="A9" s="195"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25234,7 +25278,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="193" t="s">
         <v>211</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25248,7 +25292,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="193"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25260,7 +25304,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="193"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25269,7 +25313,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="193"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="139" t="s">
         <v>212</v>
       </c>
@@ -25281,7 +25325,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="193"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25293,7 +25337,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="193"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25302,7 +25346,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="194"/>
+      <c r="A17" s="195"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25317,7 +25361,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="192" t="s">
+      <c r="A19" s="193" t="s">
         <v>211</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25326,7 +25370,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="193"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25336,14 +25380,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="193"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="193"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="139" t="s">
         <v>212</v>
       </c>
@@ -25353,7 +25397,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="193"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25363,14 +25407,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="193"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="194"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25383,7 +25427,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25405,163 +25449,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="206" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="205"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="212" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="202"/>
+      <c r="B2" s="213"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="214" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="202"/>
+      <c r="B3" s="213"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="208"/>
-      <c r="B4" s="209"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="206" t="s">
+      <c r="A5" s="208" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="207"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="212" t="s">
+      <c r="A7" s="200" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="213"/>
+      <c r="B7" s="201"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="210" t="s">
+      <c r="A9" s="202" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="211"/>
+      <c r="B9" s="203"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="197"/>
-      <c r="B10" s="198"/>
+      <c r="A10" s="204"/>
+      <c r="B10" s="205"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="196" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="200"/>
+      <c r="B11" s="197"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="199" t="s">
+      <c r="A12" s="196" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="200"/>
+      <c r="B12" s="197"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="199" t="s">
+      <c r="A13" s="196" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="200"/>
+      <c r="B13" s="197"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="199" t="s">
+      <c r="A14" s="196" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="200"/>
+      <c r="B14" s="197"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="199" t="s">
+      <c r="A15" s="196" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="200"/>
+      <c r="B15" s="197"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="199" t="s">
+      <c r="A16" s="196" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="200"/>
+      <c r="B16" s="197"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="198" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="196"/>
+      <c r="B17" s="199"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="212" t="s">
+      <c r="A19" s="200" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="213"/>
+      <c r="B19" s="201"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="210" t="s">
+      <c r="A21" s="202" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="211"/>
+      <c r="B21" s="203"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="197"/>
-      <c r="B22" s="198"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="205"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="199" t="s">
+      <c r="A23" s="196" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="200"/>
+      <c r="B23" s="197"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="199"/>
-      <c r="B24" s="200"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="197"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="199" t="s">
+      <c r="A25" s="196" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="200"/>
+      <c r="B25" s="197"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="199" t="s">
+      <c r="A26" s="196" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="200"/>
+      <c r="B26" s="197"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25572,6 +25603,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Dragon Egg - Most of level 2 done (over 9000 frames!) 231 frames ahead of the published movie
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="232">
   <si>
     <t>Notes</t>
   </si>
@@ -739,6 +739,12 @@
   <si>
     <t>Player appears</t>
   </si>
+  <si>
+    <t>Screen 1 End</t>
+  </si>
+  <si>
+    <t>Screen 2 End</t>
+  </si>
 </sst>
 </file>
 
@@ -748,10 +754,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1678,34 +1691,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1713,208 +1726,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1924,10 +1937,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1948,18 +1961,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1969,122 +1985,122 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2406,7 +2422,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2422,16 +2438,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="157" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="157" t="s">
+      <c r="B1" s="156"/>
+      <c r="C1" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
@@ -2509,10 +2525,10 @@
       <c r="B5" s="147" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="154" t="s">
+      <c r="C5" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="155"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2528,10 +2544,10 @@
       <c r="B6" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="154" t="s">
+      <c r="C6" s="155" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="155"/>
+      <c r="D6" s="156"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2549,7 +2565,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="160" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2569,7 +2585,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="152"/>
+      <c r="A9" s="153"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
@@ -2583,7 +2599,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2600,7 +2616,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="152"/>
+      <c r="A11" s="153"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2617,7 +2633,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="153"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2634,7 +2650,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="152"/>
+      <c r="A13" s="153"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2645,7 +2661,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2656,7 +2672,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="152"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="148" t="s">
         <v>186</v>
       </c>
@@ -2673,7 +2689,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
@@ -2716,7 +2732,7 @@
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="153" t="s">
+      <c r="A19" s="154" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2736,7 +2752,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
@@ -2753,7 +2769,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="148" t="s">
         <v>218</v>
       </c>
@@ -2770,7 +2786,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="148" t="s">
         <v>219</v>
       </c>
@@ -2793,7 +2809,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="B23" s="149" t="s">
         <v>226</v>
       </c>
@@ -2813,7 +2829,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
+      <c r="A24" s="153"/>
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
@@ -2830,7 +2846,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="152"/>
+      <c r="A25" s="153"/>
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
@@ -2847,7 +2863,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="152"/>
+      <c r="A26" s="153"/>
       <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
@@ -2867,8 +2883,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="152"/>
-      <c r="B27" s="215" t="s">
+      <c r="A27" s="153"/>
+      <c r="B27" s="151" t="s">
         <v>228</v>
       </c>
       <c r="C27" s="101">
@@ -2884,7 +2900,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="152"/>
+      <c r="A28" s="153"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2895,7 +2911,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="152"/>
+      <c r="A29" s="153"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2906,7 +2922,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="152"/>
+      <c r="A30" s="153"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2917,7 +2933,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="152"/>
+      <c r="A31" s="153"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2928,7 +2944,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="152"/>
+      <c r="A32" s="153"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2939,7 +2955,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="152"/>
+      <c r="A33" s="153"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
       </c>
@@ -2982,7 +2998,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="151" t="s">
+      <c r="A36" s="152" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -3002,7 +3018,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="152"/>
+      <c r="A37" s="153"/>
       <c r="B37" s="98" t="s">
         <v>184</v>
       </c>
@@ -3019,8 +3035,8 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="152"/>
-      <c r="B38" s="215" t="s">
+      <c r="A38" s="153"/>
+      <c r="B38" s="151" t="s">
         <v>229</v>
       </c>
       <c r="C38" s="101">
@@ -3036,29 +3052,41 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
-      <c r="B39" s="100"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
+      <c r="A39" s="153"/>
+      <c r="B39" s="216" t="s">
+        <v>230</v>
+      </c>
+      <c r="C39" s="101">
+        <v>6011</v>
+      </c>
+      <c r="D39" s="101">
+        <v>6154</v>
+      </c>
       <c r="E39" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
-      <c r="B40" s="100"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
+      <c r="A40" s="153"/>
+      <c r="B40" s="216" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="101">
+        <v>7173</v>
+      </c>
+      <c r="D40" s="101">
+        <v>7404</v>
+      </c>
       <c r="E40" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="152"/>
+      <c r="A41" s="153"/>
       <c r="B41" s="100"/>
       <c r="C41" s="101"/>
       <c r="D41" s="101"/>
@@ -3069,7 +3097,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="152"/>
+      <c r="A42" s="153"/>
       <c r="B42" s="100"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -3080,7 +3108,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="152"/>
+      <c r="A43" s="153"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3091,7 +3119,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="152"/>
+      <c r="A44" s="153"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3102,7 +3130,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="152"/>
+      <c r="A45" s="153"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3113,7 +3141,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="152"/>
+      <c r="A46" s="153"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3124,7 +3152,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="152"/>
+      <c r="A47" s="153"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3135,7 +3163,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="152"/>
+      <c r="A48" s="153"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3146,7 +3174,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="152"/>
+      <c r="A49" s="153"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3157,7 +3185,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="152"/>
+      <c r="A50" s="153"/>
       <c r="B50" s="98" t="s">
         <v>187</v>
       </c>
@@ -3196,7 +3224,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="153" t="s">
+      <c r="A53" s="154" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3216,7 +3244,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
+      <c r="A54" s="153"/>
       <c r="B54" s="98" t="s">
         <v>184</v>
       </c>
@@ -3229,7 +3257,7 @@
       <c r="F54" s="104"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="152"/>
+      <c r="A55" s="153"/>
       <c r="B55" s="100"/>
       <c r="C55" s="101"/>
       <c r="D55" s="101"/>
@@ -3240,7 +3268,7 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="152"/>
+      <c r="A56" s="153"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3251,7 +3279,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="152"/>
+      <c r="A57" s="153"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3262,7 +3290,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="152"/>
+      <c r="A58" s="153"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3273,7 +3301,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="152"/>
+      <c r="A59" s="153"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3284,7 +3312,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="152"/>
+      <c r="A60" s="153"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3295,7 +3323,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="152"/>
+      <c r="A61" s="153"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3306,7 +3334,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="152"/>
+      <c r="A62" s="153"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3317,7 +3345,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="152"/>
+      <c r="A63" s="153"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3328,7 +3356,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="152"/>
+      <c r="A64" s="153"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3339,7 +3367,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="152"/>
+      <c r="A65" s="153"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3350,7 +3378,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
+      <c r="A66" s="153"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3361,7 +3389,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="152"/>
+      <c r="A67" s="153"/>
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
@@ -3400,7 +3428,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="151" t="s">
+      <c r="A70" s="152" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3420,7 +3448,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="152"/>
+      <c r="A71" s="153"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
@@ -3433,7 +3461,7 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
+      <c r="A72" s="153"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3444,7 +3472,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="152"/>
+      <c r="A73" s="153"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3455,7 +3483,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="152"/>
+      <c r="A74" s="153"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3466,7 +3494,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="152"/>
+      <c r="A75" s="153"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3477,7 +3505,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="152"/>
+      <c r="A76" s="153"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3488,7 +3516,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="152"/>
+      <c r="A77" s="153"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3499,7 +3527,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="152"/>
+      <c r="A78" s="153"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3510,7 +3538,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="152"/>
+      <c r="A79" s="153"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3521,7 +3549,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="152"/>
+      <c r="A80" s="153"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3532,7 +3560,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="152"/>
+      <c r="A81" s="153"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3543,7 +3571,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="152"/>
+      <c r="A82" s="153"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3554,7 +3582,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="152"/>
+      <c r="A83" s="153"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3565,7 +3593,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="152"/>
+      <c r="A84" s="153"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
@@ -3603,7 +3631,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="153" t="s">
+      <c r="A87" s="154" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3623,7 +3651,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="152"/>
+      <c r="A88" s="153"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
@@ -3636,7 +3664,7 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="152"/>
+      <c r="A89" s="153"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3647,7 +3675,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="152"/>
+      <c r="A90" s="153"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3658,7 +3686,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="152"/>
+      <c r="A91" s="153"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3669,7 +3697,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="152"/>
+      <c r="A92" s="153"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3680,7 +3708,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="152"/>
+      <c r="A93" s="153"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3691,7 +3719,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="152"/>
+      <c r="A94" s="153"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3702,7 +3730,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="152"/>
+      <c r="A95" s="153"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3713,7 +3741,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="152"/>
+      <c r="A96" s="153"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3724,7 +3752,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="152"/>
+      <c r="A97" s="153"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3735,7 +3763,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="152"/>
+      <c r="A98" s="153"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3746,7 +3774,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="152"/>
+      <c r="A99" s="153"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3757,7 +3785,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="152"/>
+      <c r="A100" s="153"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3768,7 +3796,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="152"/>
+      <c r="A101" s="153"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
       </c>
@@ -3782,7 +3810,7 @@
     </row>
     <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="151" t="s">
+      <c r="A103" s="152" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="113" t="s">
@@ -3802,7 +3830,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="152"/>
+      <c r="A104" s="153"/>
       <c r="B104" s="98" t="s">
         <v>184</v>
       </c>
@@ -3815,7 +3843,7 @@
       <c r="F104" s="104"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="152"/>
+      <c r="A105" s="153"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3826,7 +3854,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="152"/>
+      <c r="A106" s="153"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3837,7 +3865,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="152"/>
+      <c r="A107" s="153"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3848,7 +3876,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="152"/>
+      <c r="A108" s="153"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3859,7 +3887,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="152"/>
+      <c r="A109" s="153"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3870,7 +3898,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="152"/>
+      <c r="A110" s="153"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3881,7 +3909,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="152"/>
+      <c r="A111" s="153"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3892,7 +3920,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="152"/>
+      <c r="A112" s="153"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3903,7 +3931,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="152"/>
+      <c r="A113" s="153"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3914,7 +3942,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="152"/>
+      <c r="A114" s="153"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3925,7 +3953,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="152"/>
+      <c r="A115" s="153"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3936,7 +3964,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="152"/>
+      <c r="A116" s="153"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3947,7 +3975,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="152"/>
+      <c r="A117" s="153"/>
       <c r="B117" s="98" t="s">
         <v>187</v>
       </c>
@@ -3961,7 +3989,7 @@
     </row>
     <row r="118" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="119" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="153" t="s">
+      <c r="A119" s="154" t="s">
         <v>175</v>
       </c>
       <c r="B119" s="109" t="s">
@@ -3981,7 +4009,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="152"/>
+      <c r="A120" s="153"/>
       <c r="B120" s="98" t="s">
         <v>184</v>
       </c>
@@ -3994,7 +4022,7 @@
       <c r="F120" s="104"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="152"/>
+      <c r="A121" s="153"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4005,7 +4033,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="152"/>
+      <c r="A122" s="153"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4016,7 +4044,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="152"/>
+      <c r="A123" s="153"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4027,7 +4055,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="152"/>
+      <c r="A124" s="153"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -4038,7 +4066,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="152"/>
+      <c r="A125" s="153"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4049,7 +4077,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="152"/>
+      <c r="A126" s="153"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4060,7 +4088,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="152"/>
+      <c r="A127" s="153"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4071,7 +4099,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="152"/>
+      <c r="A128" s="153"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4082,7 +4110,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="152"/>
+      <c r="A129" s="153"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4093,7 +4121,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="152"/>
+      <c r="A130" s="153"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4104,7 +4132,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="152"/>
+      <c r="A131" s="153"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4115,7 +4143,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="152"/>
+      <c r="A132" s="153"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4126,7 +4154,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="152"/>
+      <c r="A133" s="153"/>
       <c r="B133" s="98" t="s">
         <v>187</v>
       </c>
@@ -4140,7 +4168,7 @@
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A135" s="151" t="s">
+      <c r="A135" s="152" t="s">
         <v>176</v>
       </c>
       <c r="B135" s="113" t="s">
@@ -4160,7 +4188,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="152"/>
+      <c r="A136" s="153"/>
       <c r="B136" s="98" t="s">
         <v>184</v>
       </c>
@@ -4173,7 +4201,7 @@
       <c r="F136" s="104"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="152"/>
+      <c r="A137" s="153"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4184,7 +4212,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A138" s="152"/>
+      <c r="A138" s="153"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4195,7 +4223,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A139" s="152"/>
+      <c r="A139" s="153"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4206,7 +4234,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A140" s="152"/>
+      <c r="A140" s="153"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4217,7 +4245,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A141" s="152"/>
+      <c r="A141" s="153"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4228,7 +4256,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="152"/>
+      <c r="A142" s="153"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4239,7 +4267,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A143" s="152"/>
+      <c r="A143" s="153"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4250,7 +4278,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="152"/>
+      <c r="A144" s="153"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4261,7 +4289,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="152"/>
+      <c r="A145" s="153"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4272,7 +4300,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="152"/>
+      <c r="A146" s="153"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4283,7 +4311,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="152"/>
+      <c r="A147" s="153"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4294,7 +4322,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="152"/>
+      <c r="A148" s="153"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4305,7 +4333,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="152"/>
+      <c r="A149" s="153"/>
       <c r="B149" s="98" t="s">
         <v>187</v>
       </c>
@@ -4320,11 +4348,6 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4333,6 +4356,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4364,13 +4392,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4400,18 +4428,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4563,9 +4591,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="165"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="166"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4716,9 +4744,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
+      <c r="C38" s="161"/>
+      <c r="D38" s="162"/>
+      <c r="E38" s="162"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4869,9 +4897,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="163"/>
-      <c r="D55" s="164"/>
-      <c r="E55" s="164"/>
+      <c r="C55" s="161"/>
+      <c r="D55" s="162"/>
+      <c r="E55" s="162"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5022,9 +5050,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="163"/>
-      <c r="D72" s="164"/>
-      <c r="E72" s="164"/>
+      <c r="C72" s="161"/>
+      <c r="D72" s="162"/>
+      <c r="E72" s="162"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5175,9 +5203,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="163"/>
-      <c r="D89" s="164"/>
-      <c r="E89" s="164"/>
+      <c r="C89" s="161"/>
+      <c r="D89" s="162"/>
+      <c r="E89" s="162"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5328,9 +5356,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="163"/>
-      <c r="D106" s="164"/>
-      <c r="E106" s="164"/>
+      <c r="C106" s="161"/>
+      <c r="D106" s="162"/>
+      <c r="E106" s="162"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5481,9 +5509,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="163"/>
-      <c r="D123" s="164"/>
-      <c r="E123" s="164"/>
+      <c r="C123" s="161"/>
+      <c r="D123" s="162"/>
+      <c r="E123" s="162"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5634,9 +5662,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="163"/>
-      <c r="D140" s="164"/>
-      <c r="E140" s="164"/>
+      <c r="C140" s="161"/>
+      <c r="D140" s="162"/>
+      <c r="E140" s="162"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5787,9 +5815,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="163"/>
-      <c r="D157" s="164"/>
-      <c r="E157" s="164"/>
+      <c r="C157" s="161"/>
+      <c r="D157" s="162"/>
+      <c r="E157" s="162"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5940,9 +5968,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="163"/>
-      <c r="D174" s="164"/>
-      <c r="E174" s="164"/>
+      <c r="C174" s="161"/>
+      <c r="D174" s="162"/>
+      <c r="E174" s="162"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6093,9 +6121,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="163"/>
-      <c r="D191" s="164"/>
-      <c r="E191" s="164"/>
+      <c r="C191" s="161"/>
+      <c r="D191" s="162"/>
+      <c r="E191" s="162"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6246,9 +6274,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="163"/>
-      <c r="D208" s="164"/>
-      <c r="E208" s="164"/>
+      <c r="C208" s="161"/>
+      <c r="D208" s="162"/>
+      <c r="E208" s="162"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6399,9 +6427,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="163"/>
-      <c r="D225" s="164"/>
-      <c r="E225" s="164"/>
+      <c r="C225" s="161"/>
+      <c r="D225" s="162"/>
+      <c r="E225" s="162"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6552,9 +6580,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="163"/>
-      <c r="D242" s="164"/>
-      <c r="E242" s="164"/>
+      <c r="C242" s="161"/>
+      <c r="D242" s="162"/>
+      <c r="E242" s="162"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6705,9 +6733,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="163"/>
-      <c r="D259" s="164"/>
-      <c r="E259" s="164"/>
+      <c r="C259" s="161"/>
+      <c r="D259" s="162"/>
+      <c r="E259" s="162"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6858,18 +6886,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="167"/>
-      <c r="D276" s="168"/>
-      <c r="E276" s="168"/>
+      <c r="C276" s="177"/>
+      <c r="D276" s="178"/>
+      <c r="E276" s="178"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="163"/>
-      <c r="D277" s="164"/>
-      <c r="E277" s="164"/>
+      <c r="C277" s="161"/>
+      <c r="D277" s="162"/>
+      <c r="E277" s="162"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7020,9 +7048,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="165"/>
-      <c r="D294" s="166"/>
-      <c r="E294" s="166"/>
+      <c r="C294" s="163"/>
+      <c r="D294" s="164"/>
+      <c r="E294" s="164"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7173,9 +7201,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="163"/>
-      <c r="D311" s="164"/>
-      <c r="E311" s="164"/>
+      <c r="C311" s="161"/>
+      <c r="D311" s="162"/>
+      <c r="E311" s="162"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7326,9 +7354,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="163"/>
-      <c r="D328" s="164"/>
-      <c r="E328" s="164"/>
+      <c r="C328" s="161"/>
+      <c r="D328" s="162"/>
+      <c r="E328" s="162"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7479,9 +7507,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="163"/>
-      <c r="D345" s="164"/>
-      <c r="E345" s="164"/>
+      <c r="C345" s="161"/>
+      <c r="D345" s="162"/>
+      <c r="E345" s="162"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7632,9 +7660,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="163"/>
-      <c r="D362" s="164"/>
-      <c r="E362" s="164"/>
+      <c r="C362" s="161"/>
+      <c r="D362" s="162"/>
+      <c r="E362" s="162"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7785,9 +7813,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="163"/>
-      <c r="D379" s="164"/>
-      <c r="E379" s="164"/>
+      <c r="C379" s="161"/>
+      <c r="D379" s="162"/>
+      <c r="E379" s="162"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7938,9 +7966,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="163"/>
-      <c r="D396" s="164"/>
-      <c r="E396" s="164"/>
+      <c r="C396" s="161"/>
+      <c r="D396" s="162"/>
+      <c r="E396" s="162"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8091,9 +8119,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="163"/>
-      <c r="D413" s="164"/>
-      <c r="E413" s="164"/>
+      <c r="C413" s="161"/>
+      <c r="D413" s="162"/>
+      <c r="E413" s="162"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8244,9 +8272,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="163"/>
-      <c r="D430" s="164"/>
-      <c r="E430" s="164"/>
+      <c r="C430" s="161"/>
+      <c r="D430" s="162"/>
+      <c r="E430" s="162"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8397,9 +8425,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="163"/>
-      <c r="D447" s="164"/>
-      <c r="E447" s="164"/>
+      <c r="C447" s="161"/>
+      <c r="D447" s="162"/>
+      <c r="E447" s="162"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8550,9 +8578,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="163"/>
-      <c r="D464" s="164"/>
-      <c r="E464" s="164"/>
+      <c r="C464" s="161"/>
+      <c r="D464" s="162"/>
+      <c r="E464" s="162"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8703,9 +8731,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="163"/>
-      <c r="D481" s="164"/>
-      <c r="E481" s="164"/>
+      <c r="C481" s="161"/>
+      <c r="D481" s="162"/>
+      <c r="E481" s="162"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8856,9 +8884,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="163"/>
-      <c r="D498" s="164"/>
-      <c r="E498" s="164"/>
+      <c r="C498" s="161"/>
+      <c r="D498" s="162"/>
+      <c r="E498" s="162"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9009,9 +9037,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="163"/>
-      <c r="D515" s="164"/>
-      <c r="E515" s="164"/>
+      <c r="C515" s="161"/>
+      <c r="D515" s="162"/>
+      <c r="E515" s="162"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9162,9 +9190,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="163"/>
-      <c r="D532" s="164"/>
-      <c r="E532" s="164"/>
+      <c r="C532" s="161"/>
+      <c r="D532" s="162"/>
+      <c r="E532" s="162"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9315,18 +9343,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="169"/>
-      <c r="D549" s="170"/>
-      <c r="E549" s="170"/>
+      <c r="C549" s="175"/>
+      <c r="D549" s="176"/>
+      <c r="E549" s="176"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="163"/>
-      <c r="D550" s="164"/>
-      <c r="E550" s="164"/>
+      <c r="C550" s="161"/>
+      <c r="D550" s="162"/>
+      <c r="E550" s="162"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9477,9 +9505,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="165"/>
-      <c r="D567" s="166"/>
-      <c r="E567" s="166"/>
+      <c r="C567" s="163"/>
+      <c r="D567" s="164"/>
+      <c r="E567" s="164"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9630,9 +9658,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="163"/>
-      <c r="D584" s="164"/>
-      <c r="E584" s="164"/>
+      <c r="C584" s="161"/>
+      <c r="D584" s="162"/>
+      <c r="E584" s="162"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9783,9 +9811,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="163"/>
-      <c r="D601" s="164"/>
-      <c r="E601" s="164"/>
+      <c r="C601" s="161"/>
+      <c r="D601" s="162"/>
+      <c r="E601" s="162"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9936,9 +9964,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="163"/>
-      <c r="D618" s="164"/>
-      <c r="E618" s="164"/>
+      <c r="C618" s="161"/>
+      <c r="D618" s="162"/>
+      <c r="E618" s="162"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10089,9 +10117,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="163"/>
-      <c r="D635" s="164"/>
-      <c r="E635" s="164"/>
+      <c r="C635" s="161"/>
+      <c r="D635" s="162"/>
+      <c r="E635" s="162"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10242,9 +10270,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="163"/>
-      <c r="D652" s="164"/>
-      <c r="E652" s="164"/>
+      <c r="C652" s="161"/>
+      <c r="D652" s="162"/>
+      <c r="E652" s="162"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10395,9 +10423,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="163"/>
-      <c r="D669" s="164"/>
-      <c r="E669" s="164"/>
+      <c r="C669" s="161"/>
+      <c r="D669" s="162"/>
+      <c r="E669" s="162"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10548,9 +10576,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="163"/>
-      <c r="D686" s="164"/>
-      <c r="E686" s="164"/>
+      <c r="C686" s="161"/>
+      <c r="D686" s="162"/>
+      <c r="E686" s="162"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10701,9 +10729,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="163"/>
-      <c r="D703" s="164"/>
-      <c r="E703" s="164"/>
+      <c r="C703" s="161"/>
+      <c r="D703" s="162"/>
+      <c r="E703" s="162"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10854,9 +10882,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="163"/>
-      <c r="D720" s="164"/>
-      <c r="E720" s="164"/>
+      <c r="C720" s="161"/>
+      <c r="D720" s="162"/>
+      <c r="E720" s="162"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11007,9 +11035,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="163"/>
-      <c r="D737" s="164"/>
-      <c r="E737" s="164"/>
+      <c r="C737" s="161"/>
+      <c r="D737" s="162"/>
+      <c r="E737" s="162"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11160,9 +11188,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="163"/>
-      <c r="D754" s="164"/>
-      <c r="E754" s="164"/>
+      <c r="C754" s="161"/>
+      <c r="D754" s="162"/>
+      <c r="E754" s="162"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11313,9 +11341,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="163"/>
-      <c r="D771" s="164"/>
-      <c r="E771" s="164"/>
+      <c r="C771" s="161"/>
+      <c r="D771" s="162"/>
+      <c r="E771" s="162"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11466,9 +11494,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="163"/>
-      <c r="D788" s="164"/>
-      <c r="E788" s="164"/>
+      <c r="C788" s="161"/>
+      <c r="D788" s="162"/>
+      <c r="E788" s="162"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11619,9 +11647,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="163"/>
-      <c r="D805" s="164"/>
-      <c r="E805" s="164"/>
+      <c r="C805" s="161"/>
+      <c r="D805" s="162"/>
+      <c r="E805" s="162"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11772,18 +11800,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="171"/>
-      <c r="D822" s="172"/>
-      <c r="E822" s="172"/>
+      <c r="C822" s="173"/>
+      <c r="D822" s="174"/>
+      <c r="E822" s="174"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="163"/>
-      <c r="D823" s="164"/>
-      <c r="E823" s="164"/>
+      <c r="C823" s="161"/>
+      <c r="D823" s="162"/>
+      <c r="E823" s="162"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11934,9 +11962,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="165"/>
-      <c r="D840" s="166"/>
-      <c r="E840" s="166"/>
+      <c r="C840" s="163"/>
+      <c r="D840" s="164"/>
+      <c r="E840" s="164"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12087,9 +12115,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="163"/>
-      <c r="D857" s="164"/>
-      <c r="E857" s="164"/>
+      <c r="C857" s="161"/>
+      <c r="D857" s="162"/>
+      <c r="E857" s="162"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12240,9 +12268,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="163"/>
-      <c r="D874" s="164"/>
-      <c r="E874" s="164"/>
+      <c r="C874" s="161"/>
+      <c r="D874" s="162"/>
+      <c r="E874" s="162"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12393,9 +12421,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="163"/>
-      <c r="D891" s="164"/>
-      <c r="E891" s="164"/>
+      <c r="C891" s="161"/>
+      <c r="D891" s="162"/>
+      <c r="E891" s="162"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12546,9 +12574,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="163"/>
-      <c r="D908" s="164"/>
-      <c r="E908" s="164"/>
+      <c r="C908" s="161"/>
+      <c r="D908" s="162"/>
+      <c r="E908" s="162"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12699,9 +12727,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="163"/>
-      <c r="D925" s="164"/>
-      <c r="E925" s="164"/>
+      <c r="C925" s="161"/>
+      <c r="D925" s="162"/>
+      <c r="E925" s="162"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12852,9 +12880,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="163"/>
-      <c r="D942" s="164"/>
-      <c r="E942" s="164"/>
+      <c r="C942" s="161"/>
+      <c r="D942" s="162"/>
+      <c r="E942" s="162"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13005,9 +13033,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="163"/>
-      <c r="D959" s="164"/>
-      <c r="E959" s="164"/>
+      <c r="C959" s="161"/>
+      <c r="D959" s="162"/>
+      <c r="E959" s="162"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13158,9 +13186,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="163"/>
-      <c r="D976" s="164"/>
-      <c r="E976" s="164"/>
+      <c r="C976" s="161"/>
+      <c r="D976" s="162"/>
+      <c r="E976" s="162"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13311,9 +13339,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="163"/>
-      <c r="D993" s="164"/>
-      <c r="E993" s="164"/>
+      <c r="C993" s="161"/>
+      <c r="D993" s="162"/>
+      <c r="E993" s="162"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13464,9 +13492,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="163"/>
-      <c r="D1010" s="164"/>
-      <c r="E1010" s="164"/>
+      <c r="C1010" s="161"/>
+      <c r="D1010" s="162"/>
+      <c r="E1010" s="162"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13617,9 +13645,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="163"/>
-      <c r="D1027" s="164"/>
-      <c r="E1027" s="164"/>
+      <c r="C1027" s="161"/>
+      <c r="D1027" s="162"/>
+      <c r="E1027" s="162"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13770,9 +13798,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="163"/>
-      <c r="D1044" s="164"/>
-      <c r="E1044" s="164"/>
+      <c r="C1044" s="161"/>
+      <c r="D1044" s="162"/>
+      <c r="E1044" s="162"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13923,9 +13951,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="163"/>
-      <c r="D1061" s="164"/>
-      <c r="E1061" s="164"/>
+      <c r="C1061" s="161"/>
+      <c r="D1061" s="162"/>
+      <c r="E1061" s="162"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14076,9 +14104,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="163"/>
-      <c r="D1078" s="164"/>
-      <c r="E1078" s="164"/>
+      <c r="C1078" s="161"/>
+      <c r="D1078" s="162"/>
+      <c r="E1078" s="162"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14229,18 +14257,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="173"/>
-      <c r="D1095" s="174"/>
-      <c r="E1095" s="174"/>
+      <c r="C1095" s="171"/>
+      <c r="D1095" s="172"/>
+      <c r="E1095" s="172"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="163"/>
-      <c r="D1096" s="164"/>
-      <c r="E1096" s="164"/>
+      <c r="C1096" s="161"/>
+      <c r="D1096" s="162"/>
+      <c r="E1096" s="162"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14391,9 +14419,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="165"/>
-      <c r="D1113" s="166"/>
-      <c r="E1113" s="166"/>
+      <c r="C1113" s="163"/>
+      <c r="D1113" s="164"/>
+      <c r="E1113" s="164"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14544,9 +14572,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="163"/>
-      <c r="D1130" s="164"/>
-      <c r="E1130" s="164"/>
+      <c r="C1130" s="161"/>
+      <c r="D1130" s="162"/>
+      <c r="E1130" s="162"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14697,9 +14725,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="163"/>
-      <c r="D1147" s="164"/>
-      <c r="E1147" s="164"/>
+      <c r="C1147" s="161"/>
+      <c r="D1147" s="162"/>
+      <c r="E1147" s="162"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14850,9 +14878,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="163"/>
-      <c r="D1164" s="164"/>
-      <c r="E1164" s="164"/>
+      <c r="C1164" s="161"/>
+      <c r="D1164" s="162"/>
+      <c r="E1164" s="162"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15003,9 +15031,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="163"/>
-      <c r="D1181" s="164"/>
-      <c r="E1181" s="164"/>
+      <c r="C1181" s="161"/>
+      <c r="D1181" s="162"/>
+      <c r="E1181" s="162"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15156,9 +15184,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="163"/>
-      <c r="D1198" s="164"/>
-      <c r="E1198" s="164"/>
+      <c r="C1198" s="161"/>
+      <c r="D1198" s="162"/>
+      <c r="E1198" s="162"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15309,9 +15337,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="163"/>
-      <c r="D1215" s="164"/>
-      <c r="E1215" s="164"/>
+      <c r="C1215" s="161"/>
+      <c r="D1215" s="162"/>
+      <c r="E1215" s="162"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15462,9 +15490,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="163"/>
-      <c r="D1232" s="164"/>
-      <c r="E1232" s="164"/>
+      <c r="C1232" s="161"/>
+      <c r="D1232" s="162"/>
+      <c r="E1232" s="162"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15615,9 +15643,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="163"/>
-      <c r="D1249" s="164"/>
-      <c r="E1249" s="164"/>
+      <c r="C1249" s="161"/>
+      <c r="D1249" s="162"/>
+      <c r="E1249" s="162"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15768,9 +15796,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="163"/>
-      <c r="D1266" s="164"/>
-      <c r="E1266" s="164"/>
+      <c r="C1266" s="161"/>
+      <c r="D1266" s="162"/>
+      <c r="E1266" s="162"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15921,9 +15949,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="163"/>
-      <c r="D1283" s="164"/>
-      <c r="E1283" s="164"/>
+      <c r="C1283" s="161"/>
+      <c r="D1283" s="162"/>
+      <c r="E1283" s="162"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16074,9 +16102,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="163"/>
-      <c r="D1300" s="164"/>
-      <c r="E1300" s="164"/>
+      <c r="C1300" s="161"/>
+      <c r="D1300" s="162"/>
+      <c r="E1300" s="162"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16227,9 +16255,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="163"/>
-      <c r="D1317" s="164"/>
-      <c r="E1317" s="164"/>
+      <c r="C1317" s="161"/>
+      <c r="D1317" s="162"/>
+      <c r="E1317" s="162"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16380,9 +16408,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="163"/>
-      <c r="D1334" s="164"/>
-      <c r="E1334" s="164"/>
+      <c r="C1334" s="161"/>
+      <c r="D1334" s="162"/>
+      <c r="E1334" s="162"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16533,9 +16561,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="163"/>
-      <c r="D1351" s="164"/>
-      <c r="E1351" s="164"/>
+      <c r="C1351" s="161"/>
+      <c r="D1351" s="162"/>
+      <c r="E1351" s="162"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16686,18 +16714,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="175"/>
-      <c r="D1368" s="176"/>
-      <c r="E1368" s="176"/>
+      <c r="C1368" s="169"/>
+      <c r="D1368" s="170"/>
+      <c r="E1368" s="170"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="163"/>
-      <c r="D1369" s="164"/>
-      <c r="E1369" s="164"/>
+      <c r="C1369" s="161"/>
+      <c r="D1369" s="162"/>
+      <c r="E1369" s="162"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16848,9 +16876,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="165"/>
-      <c r="D1386" s="166"/>
-      <c r="E1386" s="166"/>
+      <c r="C1386" s="163"/>
+      <c r="D1386" s="164"/>
+      <c r="E1386" s="164"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17001,9 +17029,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="163"/>
-      <c r="D1403" s="164"/>
-      <c r="E1403" s="164"/>
+      <c r="C1403" s="161"/>
+      <c r="D1403" s="162"/>
+      <c r="E1403" s="162"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17154,9 +17182,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="163"/>
-      <c r="D1420" s="164"/>
-      <c r="E1420" s="164"/>
+      <c r="C1420" s="161"/>
+      <c r="D1420" s="162"/>
+      <c r="E1420" s="162"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17307,9 +17335,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="163"/>
-      <c r="D1437" s="164"/>
-      <c r="E1437" s="164"/>
+      <c r="C1437" s="161"/>
+      <c r="D1437" s="162"/>
+      <c r="E1437" s="162"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17460,9 +17488,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="163"/>
-      <c r="D1454" s="164"/>
-      <c r="E1454" s="164"/>
+      <c r="C1454" s="161"/>
+      <c r="D1454" s="162"/>
+      <c r="E1454" s="162"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17613,9 +17641,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="163"/>
-      <c r="D1471" s="164"/>
-      <c r="E1471" s="164"/>
+      <c r="C1471" s="161"/>
+      <c r="D1471" s="162"/>
+      <c r="E1471" s="162"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17766,9 +17794,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="163"/>
-      <c r="D1488" s="164"/>
-      <c r="E1488" s="164"/>
+      <c r="C1488" s="161"/>
+      <c r="D1488" s="162"/>
+      <c r="E1488" s="162"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17919,9 +17947,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="163"/>
-      <c r="D1505" s="164"/>
-      <c r="E1505" s="164"/>
+      <c r="C1505" s="161"/>
+      <c r="D1505" s="162"/>
+      <c r="E1505" s="162"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18072,9 +18100,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="163"/>
-      <c r="D1522" s="164"/>
-      <c r="E1522" s="164"/>
+      <c r="C1522" s="161"/>
+      <c r="D1522" s="162"/>
+      <c r="E1522" s="162"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18225,9 +18253,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="163"/>
-      <c r="D1539" s="164"/>
-      <c r="E1539" s="164"/>
+      <c r="C1539" s="161"/>
+      <c r="D1539" s="162"/>
+      <c r="E1539" s="162"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18378,9 +18406,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="163"/>
-      <c r="D1556" s="164"/>
-      <c r="E1556" s="164"/>
+      <c r="C1556" s="161"/>
+      <c r="D1556" s="162"/>
+      <c r="E1556" s="162"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18531,9 +18559,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="163"/>
-      <c r="D1573" s="164"/>
-      <c r="E1573" s="164"/>
+      <c r="C1573" s="161"/>
+      <c r="D1573" s="162"/>
+      <c r="E1573" s="162"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18684,9 +18712,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="163"/>
-      <c r="D1590" s="164"/>
-      <c r="E1590" s="164"/>
+      <c r="C1590" s="161"/>
+      <c r="D1590" s="162"/>
+      <c r="E1590" s="162"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18837,9 +18865,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="163"/>
-      <c r="D1607" s="164"/>
-      <c r="E1607" s="164"/>
+      <c r="C1607" s="161"/>
+      <c r="D1607" s="162"/>
+      <c r="E1607" s="162"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18990,9 +19018,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="163"/>
-      <c r="D1624" s="164"/>
-      <c r="E1624" s="164"/>
+      <c r="C1624" s="161"/>
+      <c r="D1624" s="162"/>
+      <c r="E1624" s="162"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19143,18 +19171,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="177"/>
-      <c r="D1641" s="178"/>
-      <c r="E1641" s="178"/>
+      <c r="C1641" s="167"/>
+      <c r="D1641" s="168"/>
+      <c r="E1641" s="168"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="163"/>
-      <c r="D1642" s="164"/>
-      <c r="E1642" s="164"/>
+      <c r="C1642" s="161"/>
+      <c r="D1642" s="162"/>
+      <c r="E1642" s="162"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19305,9 +19333,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="165"/>
-      <c r="D1659" s="166"/>
-      <c r="E1659" s="166"/>
+      <c r="C1659" s="163"/>
+      <c r="D1659" s="164"/>
+      <c r="E1659" s="164"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19458,9 +19486,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="163"/>
-      <c r="D1676" s="164"/>
-      <c r="E1676" s="164"/>
+      <c r="C1676" s="161"/>
+      <c r="D1676" s="162"/>
+      <c r="E1676" s="162"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19611,9 +19639,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="163"/>
-      <c r="D1693" s="164"/>
-      <c r="E1693" s="164"/>
+      <c r="C1693" s="161"/>
+      <c r="D1693" s="162"/>
+      <c r="E1693" s="162"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19764,9 +19792,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="163"/>
-      <c r="D1710" s="164"/>
-      <c r="E1710" s="164"/>
+      <c r="C1710" s="161"/>
+      <c r="D1710" s="162"/>
+      <c r="E1710" s="162"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19917,9 +19945,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="163"/>
-      <c r="D1727" s="164"/>
-      <c r="E1727" s="164"/>
+      <c r="C1727" s="161"/>
+      <c r="D1727" s="162"/>
+      <c r="E1727" s="162"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20070,9 +20098,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="163"/>
-      <c r="D1744" s="164"/>
-      <c r="E1744" s="164"/>
+      <c r="C1744" s="161"/>
+      <c r="D1744" s="162"/>
+      <c r="E1744" s="162"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20223,9 +20251,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="163"/>
-      <c r="D1761" s="164"/>
-      <c r="E1761" s="164"/>
+      <c r="C1761" s="161"/>
+      <c r="D1761" s="162"/>
+      <c r="E1761" s="162"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20376,9 +20404,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="163"/>
-      <c r="D1778" s="164"/>
-      <c r="E1778" s="164"/>
+      <c r="C1778" s="161"/>
+      <c r="D1778" s="162"/>
+      <c r="E1778" s="162"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20529,9 +20557,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="163"/>
-      <c r="D1795" s="164"/>
-      <c r="E1795" s="164"/>
+      <c r="C1795" s="161"/>
+      <c r="D1795" s="162"/>
+      <c r="E1795" s="162"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20682,9 +20710,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="163"/>
-      <c r="D1812" s="164"/>
-      <c r="E1812" s="164"/>
+      <c r="C1812" s="161"/>
+      <c r="D1812" s="162"/>
+      <c r="E1812" s="162"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20835,9 +20863,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="163"/>
-      <c r="D1829" s="164"/>
-      <c r="E1829" s="164"/>
+      <c r="C1829" s="161"/>
+      <c r="D1829" s="162"/>
+      <c r="E1829" s="162"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20988,9 +21016,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="163"/>
-      <c r="D1846" s="164"/>
-      <c r="E1846" s="164"/>
+      <c r="C1846" s="161"/>
+      <c r="D1846" s="162"/>
+      <c r="E1846" s="162"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21141,9 +21169,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="163"/>
-      <c r="D1863" s="164"/>
-      <c r="E1863" s="164"/>
+      <c r="C1863" s="161"/>
+      <c r="D1863" s="162"/>
+      <c r="E1863" s="162"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21294,9 +21322,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="163"/>
-      <c r="D1880" s="164"/>
-      <c r="E1880" s="164"/>
+      <c r="C1880" s="161"/>
+      <c r="D1880" s="162"/>
+      <c r="E1880" s="162"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21447,9 +21475,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="163"/>
-      <c r="D1897" s="164"/>
-      <c r="E1897" s="164"/>
+      <c r="C1897" s="161"/>
+      <c r="D1897" s="162"/>
+      <c r="E1897" s="162"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21600,18 +21628,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="179"/>
-      <c r="D1914" s="180"/>
-      <c r="E1914" s="180"/>
+      <c r="C1914" s="165"/>
+      <c r="D1914" s="166"/>
+      <c r="E1914" s="166"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="163"/>
-      <c r="D1915" s="164"/>
-      <c r="E1915" s="164"/>
+      <c r="C1915" s="161"/>
+      <c r="D1915" s="162"/>
+      <c r="E1915" s="162"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21762,9 +21790,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="165"/>
-      <c r="D1932" s="166"/>
-      <c r="E1932" s="166"/>
+      <c r="C1932" s="163"/>
+      <c r="D1932" s="164"/>
+      <c r="E1932" s="164"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21915,9 +21943,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="163"/>
-      <c r="D1949" s="164"/>
-      <c r="E1949" s="164"/>
+      <c r="C1949" s="161"/>
+      <c r="D1949" s="162"/>
+      <c r="E1949" s="162"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22068,9 +22096,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="163"/>
-      <c r="D1966" s="164"/>
-      <c r="E1966" s="164"/>
+      <c r="C1966" s="161"/>
+      <c r="D1966" s="162"/>
+      <c r="E1966" s="162"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22221,9 +22249,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="163"/>
-      <c r="D1983" s="164"/>
-      <c r="E1983" s="164"/>
+      <c r="C1983" s="161"/>
+      <c r="D1983" s="162"/>
+      <c r="E1983" s="162"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22374,9 +22402,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="163"/>
-      <c r="D2000" s="164"/>
-      <c r="E2000" s="164"/>
+      <c r="C2000" s="161"/>
+      <c r="D2000" s="162"/>
+      <c r="E2000" s="162"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22527,9 +22555,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="163"/>
-      <c r="D2017" s="164"/>
-      <c r="E2017" s="164"/>
+      <c r="C2017" s="161"/>
+      <c r="D2017" s="162"/>
+      <c r="E2017" s="162"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22680,9 +22708,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="163"/>
-      <c r="D2034" s="164"/>
-      <c r="E2034" s="164"/>
+      <c r="C2034" s="161"/>
+      <c r="D2034" s="162"/>
+      <c r="E2034" s="162"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22833,9 +22861,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="163"/>
-      <c r="D2051" s="164"/>
-      <c r="E2051" s="164"/>
+      <c r="C2051" s="161"/>
+      <c r="D2051" s="162"/>
+      <c r="E2051" s="162"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22986,9 +23014,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="163"/>
-      <c r="D2068" s="164"/>
-      <c r="E2068" s="164"/>
+      <c r="C2068" s="161"/>
+      <c r="D2068" s="162"/>
+      <c r="E2068" s="162"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23139,9 +23167,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="163"/>
-      <c r="D2085" s="164"/>
-      <c r="E2085" s="164"/>
+      <c r="C2085" s="161"/>
+      <c r="D2085" s="162"/>
+      <c r="E2085" s="162"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23292,9 +23320,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="163"/>
-      <c r="D2102" s="164"/>
-      <c r="E2102" s="164"/>
+      <c r="C2102" s="161"/>
+      <c r="D2102" s="162"/>
+      <c r="E2102" s="162"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23445,9 +23473,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="163"/>
-      <c r="D2119" s="164"/>
-      <c r="E2119" s="164"/>
+      <c r="C2119" s="161"/>
+      <c r="D2119" s="162"/>
+      <c r="E2119" s="162"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23598,9 +23626,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="163"/>
-      <c r="D2136" s="164"/>
-      <c r="E2136" s="164"/>
+      <c r="C2136" s="161"/>
+      <c r="D2136" s="162"/>
+      <c r="E2136" s="162"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23751,9 +23779,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="163"/>
-      <c r="D2153" s="164"/>
-      <c r="E2153" s="164"/>
+      <c r="C2153" s="161"/>
+      <c r="D2153" s="162"/>
+      <c r="E2153" s="162"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23904,9 +23932,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="163"/>
-      <c r="D2170" s="164"/>
-      <c r="E2170" s="164"/>
+      <c r="C2170" s="161"/>
+      <c r="D2170" s="162"/>
+      <c r="E2170" s="162"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24054,15 +24082,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24075,124 +24210,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24217,51 +24245,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="188" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="187"/>
-      <c r="K1" s="187"/>
-      <c r="L1" s="187"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="185"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="185"/>
-      <c r="J2" s="185"/>
-      <c r="K2" s="185"/>
-      <c r="L2" s="186"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="182" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="183"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="184"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24478,19 +24506,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="181" t="s">
+      <c r="A20" s="182" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="182"/>
-      <c r="C20" s="182"/>
-      <c r="D20" s="182"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="182"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="183"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="183"/>
+      <c r="E20" s="183"/>
+      <c r="F20" s="183"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+      <c r="K20" s="184"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24707,19 +24735,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="182"/>
-      <c r="C37" s="182"/>
-      <c r="D37" s="182"/>
-      <c r="E37" s="182"/>
-      <c r="F37" s="182"/>
-      <c r="G37" s="182"/>
-      <c r="H37" s="182"/>
-      <c r="I37" s="182"/>
-      <c r="J37" s="182"/>
-      <c r="K37" s="183"/>
+      <c r="B37" s="183"/>
+      <c r="C37" s="183"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="183"/>
+      <c r="F37" s="183"/>
+      <c r="G37" s="183"/>
+      <c r="H37" s="183"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="183"/>
+      <c r="K37" s="184"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -24943,7 +24971,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24977,28 +25005,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="188"/>
+      <c r="A3" s="189"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="189"/>
+      <c r="A4" s="190"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="189"/>
+      <c r="A5" s="190"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="189"/>
+      <c r="A6" s="190"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="189"/>
+      <c r="A7" s="190"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="189"/>
+      <c r="A8" s="190"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="189"/>
+      <c r="A9" s="190"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="190"/>
+      <c r="A10" s="191"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25154,7 +25182,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25181,10 +25209,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="191" t="s">
+      <c r="B1" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="192"/>
+      <c r="C1" s="193"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25195,7 +25223,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="193" t="s">
+      <c r="A3" s="194" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25209,7 +25237,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="194"/>
+      <c r="A4" s="195"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25221,7 +25249,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="194"/>
+      <c r="A5" s="195"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25230,7 +25258,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="194"/>
+      <c r="A6" s="195"/>
       <c r="B6" s="139" t="s">
         <v>212</v>
       </c>
@@ -25242,7 +25270,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="194"/>
+      <c r="A7" s="195"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25254,7 +25282,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="194"/>
+      <c r="A8" s="195"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25263,7 +25291,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="195"/>
+      <c r="A9" s="196"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25278,7 +25306,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="194" t="s">
         <v>211</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25292,7 +25320,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="194"/>
+      <c r="A12" s="195"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25304,7 +25332,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="194"/>
+      <c r="A13" s="195"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25313,7 +25341,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="194"/>
+      <c r="A14" s="195"/>
       <c r="B14" s="139" t="s">
         <v>212</v>
       </c>
@@ -25325,7 +25353,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="194"/>
+      <c r="A15" s="195"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25337,7 +25365,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="194"/>
+      <c r="A16" s="195"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25346,7 +25374,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="195"/>
+      <c r="A17" s="196"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25361,7 +25389,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="193" t="s">
+      <c r="A19" s="194" t="s">
         <v>211</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25370,7 +25398,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="194"/>
+      <c r="A20" s="195"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25380,14 +25408,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="194"/>
+      <c r="A21" s="195"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="194"/>
+      <c r="A22" s="195"/>
       <c r="B22" s="139" t="s">
         <v>212</v>
       </c>
@@ -25397,7 +25425,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="194"/>
+      <c r="A23" s="195"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25407,14 +25435,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="194"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="195"/>
+      <c r="A25" s="196"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25427,7 +25455,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25458,17 +25486,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="212" t="s">
+      <c r="A2" s="203" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="213"/>
+      <c r="B2" s="204"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="205" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="213"/>
+      <c r="B3" s="204"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -25484,115 +25512,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="200" t="s">
+      <c r="A7" s="214" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="201"/>
+      <c r="B7" s="215"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="202" t="s">
+      <c r="A9" s="212" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="203"/>
+      <c r="B9" s="213"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="204"/>
-      <c r="B10" s="205"/>
+      <c r="A10" s="199"/>
+      <c r="B10" s="200"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="196" t="s">
+      <c r="A11" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="197"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="196" t="s">
+      <c r="A12" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="197"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="196" t="s">
+      <c r="A13" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="197"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="196" t="s">
+      <c r="A14" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="197"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="197"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="196" t="s">
+      <c r="A16" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="197"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="198" t="s">
+      <c r="A17" s="197" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="199"/>
+      <c r="B17" s="198"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="214" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="201"/>
+      <c r="B19" s="215"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="202" t="s">
+      <c r="A21" s="212" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="203"/>
+      <c r="B21" s="213"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="205"/>
+      <c r="A22" s="199"/>
+      <c r="B22" s="200"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="196" t="s">
+      <c r="A23" s="201" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="197"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="196"/>
-      <c r="B24" s="197"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="196" t="s">
+      <c r="A25" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="197"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="196" t="s">
+      <c r="A26" s="201" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="197"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="198"/>
-      <c r="B27" s="199"/>
+      <c r="A27" s="197"/>
+      <c r="B27" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25603,19 +25644,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Dragon Egg - finished level 2, 398 frames ahead
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="237">
   <si>
     <t>Notes</t>
   </si>
@@ -745,6 +745,21 @@
   <si>
     <t>Screen 2 End</t>
   </si>
+  <si>
+    <t>Checkpoint x = 136</t>
+  </si>
+  <si>
+    <t>Checkpoint x = 24</t>
+  </si>
+  <si>
+    <t>Screen 3 End</t>
+  </si>
+  <si>
+    <t>End Level</t>
+  </si>
+  <si>
+    <t>Dragon appears</t>
+  </si>
 </sst>
 </file>
 
@@ -754,10 +769,24 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1691,34 +1720,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1726,208 +1755,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1937,10 +1966,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1961,18 +1990,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1985,86 +2020,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2072,35 +2107,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2421,8 +2456,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="6" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2438,16 +2473,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="159" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="158" t="s">
+      <c r="B1" s="158"/>
+      <c r="C1" s="160" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="159"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="161"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
@@ -2525,10 +2560,10 @@
       <c r="B5" s="147" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="155" t="s">
+      <c r="C5" s="157" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="155"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2544,10 +2579,10 @@
       <c r="B6" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="156"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2565,7 +2600,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="162" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2585,7 +2620,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="153"/>
+      <c r="A9" s="155"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
@@ -2599,7 +2634,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="153"/>
+      <c r="A10" s="155"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2616,7 +2651,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="153"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2633,7 +2668,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="153"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2650,7 +2685,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="153"/>
+      <c r="A13" s="155"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2661,7 +2696,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2672,7 +2707,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="153"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="148" t="s">
         <v>186</v>
       </c>
@@ -2689,7 +2724,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="153"/>
+      <c r="A16" s="155"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
@@ -2732,7 +2767,7 @@
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="154" t="s">
+      <c r="A19" s="156" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2752,7 +2787,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="153"/>
+      <c r="A20" s="155"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
@@ -2769,7 +2804,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="153"/>
+      <c r="A21" s="155"/>
       <c r="B21" s="148" t="s">
         <v>218</v>
       </c>
@@ -2786,7 +2821,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="153"/>
+      <c r="A22" s="155"/>
       <c r="B22" s="148" t="s">
         <v>219</v>
       </c>
@@ -2809,7 +2844,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="153"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="149" t="s">
         <v>226</v>
       </c>
@@ -2829,7 +2864,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="153"/>
+      <c r="A24" s="155"/>
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
@@ -2846,7 +2881,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="153"/>
+      <c r="A25" s="155"/>
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
@@ -2863,7 +2898,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="153"/>
+      <c r="A26" s="155"/>
       <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
@@ -2883,7 +2918,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="153"/>
+      <c r="A27" s="155"/>
       <c r="B27" s="151" t="s">
         <v>228</v>
       </c>
@@ -2900,7 +2935,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="153"/>
+      <c r="A28" s="155"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2911,7 +2946,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="153"/>
+      <c r="A29" s="155"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2922,7 +2957,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="153"/>
+      <c r="A30" s="155"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2933,7 +2968,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="153"/>
+      <c r="A31" s="155"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2944,7 +2979,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="153"/>
+      <c r="A32" s="155"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2955,7 +2990,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="153"/>
+      <c r="A33" s="155"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
       </c>
@@ -2998,7 +3033,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152" t="s">
+      <c r="A36" s="154" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -3018,7 +3053,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="153"/>
+      <c r="A37" s="155"/>
       <c r="B37" s="98" t="s">
         <v>184</v>
       </c>
@@ -3035,7 +3070,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="153"/>
+      <c r="A38" s="155"/>
       <c r="B38" s="151" t="s">
         <v>229</v>
       </c>
@@ -3052,8 +3087,8 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="153"/>
-      <c r="B39" s="216" t="s">
+      <c r="A39" s="155"/>
+      <c r="B39" s="152" t="s">
         <v>230</v>
       </c>
       <c r="C39" s="101">
@@ -3069,8 +3104,8 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="153"/>
-      <c r="B40" s="216" t="s">
+      <c r="A40" s="155"/>
+      <c r="B40" s="152" t="s">
         <v>231</v>
       </c>
       <c r="C40" s="101">
@@ -3086,51 +3121,75 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="153"/>
-      <c r="B41" s="100"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
+      <c r="A41" s="155"/>
+      <c r="B41" s="153" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="101">
+        <v>8822</v>
+      </c>
+      <c r="D41" s="101">
+        <v>9082</v>
+      </c>
       <c r="E41" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="153"/>
-      <c r="B42" s="100"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
+      <c r="A42" s="155"/>
+      <c r="B42" s="153" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" s="101">
+        <v>9096</v>
+      </c>
+      <c r="D42" s="101">
+        <v>9373</v>
+      </c>
       <c r="E42" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="153"/>
-      <c r="B43" s="100"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="101"/>
+      <c r="A43" s="155"/>
+      <c r="B43" s="153" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="101">
+        <v>9261</v>
+      </c>
+      <c r="D43" s="101">
+        <v>9538</v>
+      </c>
       <c r="E43" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="153"/>
-      <c r="B44" s="100"/>
-      <c r="C44" s="101"/>
-      <c r="D44" s="101"/>
+      <c r="A44" s="155"/>
+      <c r="B44" s="218" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="101">
+        <v>10591</v>
+      </c>
+      <c r="D44" s="101">
+        <v>10989</v>
+      </c>
       <c r="E44" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="153"/>
+      <c r="A45" s="155"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3141,7 +3200,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="153"/>
+      <c r="A46" s="155"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3152,7 +3211,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="153"/>
+      <c r="A47" s="155"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3163,7 +3222,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="153"/>
+      <c r="A48" s="155"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3174,7 +3233,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="153"/>
+      <c r="A49" s="155"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3185,15 +3244,19 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="153"/>
+      <c r="A50" s="155"/>
       <c r="B50" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
+      <c r="C50" s="99">
+        <v>10958</v>
+      </c>
+      <c r="D50" s="99">
+        <v>11356</v>
+      </c>
       <c r="E50" s="125">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="F50" s="104"/>
     </row>
@@ -3206,25 +3269,25 @@
       </c>
       <c r="C51" s="103">
         <f>C50-C37</f>
-        <v>-5414</v>
+        <v>5544</v>
       </c>
       <c r="D51" s="103">
         <f>D50-D37</f>
-        <v>-5454</v>
+        <v>5902</v>
       </c>
       <c r="E51" s="126">
         <f>E50-E37</f>
-        <v>-40</v>
+        <v>358</v>
       </c>
       <c r="F51" s="107"/>
       <c r="G51" s="112">
         <f>E51</f>
-        <v>-40</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="154" t="s">
+    <row r="53" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="156" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3243,32 +3306,42 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="153"/>
+    <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="155"/>
       <c r="B54" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
+      <c r="C54" s="99">
+        <v>10958</v>
+      </c>
+      <c r="D54" s="99">
+        <v>11356</v>
+      </c>
       <c r="E54" s="123">
         <f t="shared" ref="E54:E67" si="4">IF(AND(C54&gt;0,D54&gt;0), D54-C54, 0)</f>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="F54" s="104"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="153"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
+    <row r="55" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="155"/>
+      <c r="B55" s="218" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" s="101">
+        <v>10958</v>
+      </c>
+      <c r="D55" s="101">
+        <v>11356</v>
+      </c>
       <c r="E55" s="124">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="F55" s="105"/>
     </row>
-    <row r="56" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="153"/>
+    <row r="56" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="155"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
@@ -3278,8 +3351,8 @@
       </c>
       <c r="F56" s="105"/>
     </row>
-    <row r="57" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="153"/>
+    <row r="57" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="155"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3289,8 +3362,8 @@
       </c>
       <c r="F57" s="105"/>
     </row>
-    <row r="58" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="153"/>
+    <row r="58" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="155"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3300,8 +3373,8 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="153"/>
+    <row r="59" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="155"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3311,8 +3384,8 @@
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="153"/>
+    <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="155"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3322,8 +3395,8 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="153"/>
+    <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="155"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3333,8 +3406,8 @@
       </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="153"/>
+    <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="155"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3344,8 +3417,8 @@
       </c>
       <c r="F62" s="105"/>
     </row>
-    <row r="63" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="153"/>
+    <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="155"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3355,8 +3428,8 @@
       </c>
       <c r="F63" s="105"/>
     </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="153"/>
+    <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="155"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3366,8 +3439,8 @@
       </c>
       <c r="F64" s="105"/>
     </row>
-    <row r="65" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="153"/>
+    <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="155"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3377,8 +3450,8 @@
       </c>
       <c r="F65" s="105"/>
     </row>
-    <row r="66" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="153"/>
+    <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="155"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3388,8 +3461,8 @@
       </c>
       <c r="F66" s="105"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="153"/>
+    <row r="67" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="155"/>
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
@@ -3401,7 +3474,7 @@
       </c>
       <c r="F67" s="104"/>
     </row>
-    <row r="68" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="117">
         <v>3</v>
       </c>
@@ -3410,25 +3483,25 @@
       </c>
       <c r="C68" s="103">
         <f>C67-C54</f>
-        <v>0</v>
+        <v>-10958</v>
       </c>
       <c r="D68" s="103">
         <f>D67-D54</f>
-        <v>0</v>
+        <v>-11356</v>
       </c>
       <c r="E68" s="126">
         <f>E67-E54</f>
-        <v>0</v>
+        <v>-398</v>
       </c>
       <c r="F68" s="108"/>
       <c r="G68" s="112">
         <f>E68</f>
-        <v>0</v>
+        <v>-398</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="152" t="s">
+      <c r="A70" s="154" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3448,7 +3521,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="153"/>
+      <c r="A71" s="155"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
@@ -3461,7 +3534,7 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="153"/>
+      <c r="A72" s="155"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3472,7 +3545,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="153"/>
+      <c r="A73" s="155"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3483,7 +3556,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="153"/>
+      <c r="A74" s="155"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3494,7 +3567,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="153"/>
+      <c r="A75" s="155"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3505,7 +3578,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="153"/>
+      <c r="A76" s="155"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3516,7 +3589,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="153"/>
+      <c r="A77" s="155"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3527,7 +3600,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="153"/>
+      <c r="A78" s="155"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3538,7 +3611,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="153"/>
+      <c r="A79" s="155"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3549,7 +3622,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="153"/>
+      <c r="A80" s="155"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3560,7 +3633,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="153"/>
+      <c r="A81" s="155"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3571,7 +3644,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="153"/>
+      <c r="A82" s="155"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3582,7 +3655,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="153"/>
+      <c r="A83" s="155"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3593,7 +3666,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="153"/>
+      <c r="A84" s="155"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
@@ -3631,7 +3704,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="154" t="s">
+      <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3651,7 +3724,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="153"/>
+      <c r="A88" s="155"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
@@ -3664,7 +3737,7 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="153"/>
+      <c r="A89" s="155"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3675,7 +3748,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="153"/>
+      <c r="A90" s="155"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -3686,7 +3759,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="153"/>
+      <c r="A91" s="155"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -3697,7 +3770,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="153"/>
+      <c r="A92" s="155"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3708,7 +3781,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="153"/>
+      <c r="A93" s="155"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3719,7 +3792,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="153"/>
+      <c r="A94" s="155"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3730,7 +3803,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="153"/>
+      <c r="A95" s="155"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3741,7 +3814,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="153"/>
+      <c r="A96" s="155"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3752,7 +3825,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="153"/>
+      <c r="A97" s="155"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3763,7 +3836,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="153"/>
+      <c r="A98" s="155"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3774,7 +3847,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="153"/>
+      <c r="A99" s="155"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3785,7 +3858,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="153"/>
+      <c r="A100" s="155"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3796,7 +3869,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="153"/>
+      <c r="A101" s="155"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
       </c>
@@ -3810,7 +3883,7 @@
     </row>
     <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="152" t="s">
+      <c r="A103" s="154" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="113" t="s">
@@ -3830,7 +3903,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="153"/>
+      <c r="A104" s="155"/>
       <c r="B104" s="98" t="s">
         <v>184</v>
       </c>
@@ -3843,7 +3916,7 @@
       <c r="F104" s="104"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="153"/>
+      <c r="A105" s="155"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3854,7 +3927,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="153"/>
+      <c r="A106" s="155"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3865,7 +3938,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="153"/>
+      <c r="A107" s="155"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -3876,7 +3949,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="153"/>
+      <c r="A108" s="155"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -3887,7 +3960,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="153"/>
+      <c r="A109" s="155"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3898,7 +3971,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="153"/>
+      <c r="A110" s="155"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3909,7 +3982,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="153"/>
+      <c r="A111" s="155"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3920,7 +3993,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="153"/>
+      <c r="A112" s="155"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3931,7 +4004,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="153"/>
+      <c r="A113" s="155"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3942,7 +4015,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="153"/>
+      <c r="A114" s="155"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3953,7 +4026,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="153"/>
+      <c r="A115" s="155"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3964,7 +4037,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="153"/>
+      <c r="A116" s="155"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3975,7 +4048,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="153"/>
+      <c r="A117" s="155"/>
       <c r="B117" s="98" t="s">
         <v>187</v>
       </c>
@@ -3989,7 +4062,7 @@
     </row>
     <row r="118" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="119" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="154" t="s">
+      <c r="A119" s="156" t="s">
         <v>175</v>
       </c>
       <c r="B119" s="109" t="s">
@@ -4009,7 +4082,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="153"/>
+      <c r="A120" s="155"/>
       <c r="B120" s="98" t="s">
         <v>184</v>
       </c>
@@ -4022,7 +4095,7 @@
       <c r="F120" s="104"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="153"/>
+      <c r="A121" s="155"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4033,7 +4106,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="153"/>
+      <c r="A122" s="155"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4044,7 +4117,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="153"/>
+      <c r="A123" s="155"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4055,7 +4128,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="153"/>
+      <c r="A124" s="155"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -4066,7 +4139,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="153"/>
+      <c r="A125" s="155"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4077,7 +4150,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="153"/>
+      <c r="A126" s="155"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4088,7 +4161,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="153"/>
+      <c r="A127" s="155"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4099,7 +4172,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="153"/>
+      <c r="A128" s="155"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4110,7 +4183,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="153"/>
+      <c r="A129" s="155"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4121,7 +4194,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="153"/>
+      <c r="A130" s="155"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4132,7 +4205,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="153"/>
+      <c r="A131" s="155"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4143,7 +4216,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="153"/>
+      <c r="A132" s="155"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4154,7 +4227,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="153"/>
+      <c r="A133" s="155"/>
       <c r="B133" s="98" t="s">
         <v>187</v>
       </c>
@@ -4168,7 +4241,7 @@
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A135" s="152" t="s">
+      <c r="A135" s="154" t="s">
         <v>176</v>
       </c>
       <c r="B135" s="113" t="s">
@@ -4188,7 +4261,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="153"/>
+      <c r="A136" s="155"/>
       <c r="B136" s="98" t="s">
         <v>184</v>
       </c>
@@ -4201,7 +4274,7 @@
       <c r="F136" s="104"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="153"/>
+      <c r="A137" s="155"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4212,7 +4285,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A138" s="153"/>
+      <c r="A138" s="155"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4223,7 +4296,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A139" s="153"/>
+      <c r="A139" s="155"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4234,7 +4307,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A140" s="153"/>
+      <c r="A140" s="155"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4245,7 +4318,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A141" s="153"/>
+      <c r="A141" s="155"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4256,7 +4329,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="153"/>
+      <c r="A142" s="155"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4267,7 +4340,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A143" s="153"/>
+      <c r="A143" s="155"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4278,7 +4351,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="153"/>
+      <c r="A144" s="155"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4289,7 +4362,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="153"/>
+      <c r="A145" s="155"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4300,7 +4373,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="153"/>
+      <c r="A146" s="155"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4311,7 +4384,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="153"/>
+      <c r="A147" s="155"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4322,7 +4395,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="153"/>
+      <c r="A148" s="155"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4333,7 +4406,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="153"/>
+      <c r="A149" s="155"/>
       <c r="B149" s="98" t="s">
         <v>187</v>
       </c>
@@ -4392,13 +4465,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4428,18 +4501,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4591,9 +4664,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
+      <c r="C21" s="165"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4744,9 +4817,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="162"/>
-      <c r="E38" s="162"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4897,9 +4970,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="161"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
+      <c r="C55" s="163"/>
+      <c r="D55" s="164"/>
+      <c r="E55" s="164"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5050,9 +5123,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="161"/>
-      <c r="D72" s="162"/>
-      <c r="E72" s="162"/>
+      <c r="C72" s="163"/>
+      <c r="D72" s="164"/>
+      <c r="E72" s="164"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5203,9 +5276,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="161"/>
-      <c r="D89" s="162"/>
-      <c r="E89" s="162"/>
+      <c r="C89" s="163"/>
+      <c r="D89" s="164"/>
+      <c r="E89" s="164"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5356,9 +5429,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="161"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
+      <c r="C106" s="163"/>
+      <c r="D106" s="164"/>
+      <c r="E106" s="164"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5509,9 +5582,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="162"/>
-      <c r="E123" s="162"/>
+      <c r="C123" s="163"/>
+      <c r="D123" s="164"/>
+      <c r="E123" s="164"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5662,9 +5735,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="161"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="162"/>
+      <c r="C140" s="163"/>
+      <c r="D140" s="164"/>
+      <c r="E140" s="164"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5815,9 +5888,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="162"/>
-      <c r="E157" s="162"/>
+      <c r="C157" s="163"/>
+      <c r="D157" s="164"/>
+      <c r="E157" s="164"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5968,9 +6041,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="162"/>
-      <c r="E174" s="162"/>
+      <c r="C174" s="163"/>
+      <c r="D174" s="164"/>
+      <c r="E174" s="164"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6121,9 +6194,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="162"/>
-      <c r="E191" s="162"/>
+      <c r="C191" s="163"/>
+      <c r="D191" s="164"/>
+      <c r="E191" s="164"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6274,9 +6347,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="162"/>
-      <c r="E208" s="162"/>
+      <c r="C208" s="163"/>
+      <c r="D208" s="164"/>
+      <c r="E208" s="164"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6427,9 +6500,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="162"/>
-      <c r="E225" s="162"/>
+      <c r="C225" s="163"/>
+      <c r="D225" s="164"/>
+      <c r="E225" s="164"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6580,9 +6653,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="161"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
+      <c r="C242" s="163"/>
+      <c r="D242" s="164"/>
+      <c r="E242" s="164"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6733,9 +6806,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="161"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
+      <c r="C259" s="163"/>
+      <c r="D259" s="164"/>
+      <c r="E259" s="164"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6886,18 +6959,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="177"/>
-      <c r="D276" s="178"/>
-      <c r="E276" s="178"/>
+      <c r="C276" s="179"/>
+      <c r="D276" s="180"/>
+      <c r="E276" s="180"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="161"/>
-      <c r="D277" s="162"/>
-      <c r="E277" s="162"/>
+      <c r="C277" s="163"/>
+      <c r="D277" s="164"/>
+      <c r="E277" s="164"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7048,9 +7121,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="163"/>
-      <c r="D294" s="164"/>
-      <c r="E294" s="164"/>
+      <c r="C294" s="165"/>
+      <c r="D294" s="166"/>
+      <c r="E294" s="166"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7201,9 +7274,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="161"/>
-      <c r="D311" s="162"/>
-      <c r="E311" s="162"/>
+      <c r="C311" s="163"/>
+      <c r="D311" s="164"/>
+      <c r="E311" s="164"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7354,9 +7427,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="161"/>
-      <c r="D328" s="162"/>
-      <c r="E328" s="162"/>
+      <c r="C328" s="163"/>
+      <c r="D328" s="164"/>
+      <c r="E328" s="164"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7507,9 +7580,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="161"/>
-      <c r="D345" s="162"/>
-      <c r="E345" s="162"/>
+      <c r="C345" s="163"/>
+      <c r="D345" s="164"/>
+      <c r="E345" s="164"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7660,9 +7733,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="161"/>
-      <c r="D362" s="162"/>
-      <c r="E362" s="162"/>
+      <c r="C362" s="163"/>
+      <c r="D362" s="164"/>
+      <c r="E362" s="164"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7813,9 +7886,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="161"/>
-      <c r="D379" s="162"/>
-      <c r="E379" s="162"/>
+      <c r="C379" s="163"/>
+      <c r="D379" s="164"/>
+      <c r="E379" s="164"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7966,9 +8039,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="161"/>
-      <c r="D396" s="162"/>
-      <c r="E396" s="162"/>
+      <c r="C396" s="163"/>
+      <c r="D396" s="164"/>
+      <c r="E396" s="164"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8119,9 +8192,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="161"/>
-      <c r="D413" s="162"/>
-      <c r="E413" s="162"/>
+      <c r="C413" s="163"/>
+      <c r="D413" s="164"/>
+      <c r="E413" s="164"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8272,9 +8345,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="161"/>
-      <c r="D430" s="162"/>
-      <c r="E430" s="162"/>
+      <c r="C430" s="163"/>
+      <c r="D430" s="164"/>
+      <c r="E430" s="164"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8425,9 +8498,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="161"/>
-      <c r="D447" s="162"/>
-      <c r="E447" s="162"/>
+      <c r="C447" s="163"/>
+      <c r="D447" s="164"/>
+      <c r="E447" s="164"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8578,9 +8651,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="161"/>
-      <c r="D464" s="162"/>
-      <c r="E464" s="162"/>
+      <c r="C464" s="163"/>
+      <c r="D464" s="164"/>
+      <c r="E464" s="164"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8731,9 +8804,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="161"/>
-      <c r="D481" s="162"/>
-      <c r="E481" s="162"/>
+      <c r="C481" s="163"/>
+      <c r="D481" s="164"/>
+      <c r="E481" s="164"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8884,9 +8957,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="161"/>
-      <c r="D498" s="162"/>
-      <c r="E498" s="162"/>
+      <c r="C498" s="163"/>
+      <c r="D498" s="164"/>
+      <c r="E498" s="164"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9037,9 +9110,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="161"/>
-      <c r="D515" s="162"/>
-      <c r="E515" s="162"/>
+      <c r="C515" s="163"/>
+      <c r="D515" s="164"/>
+      <c r="E515" s="164"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9190,9 +9263,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="161"/>
-      <c r="D532" s="162"/>
-      <c r="E532" s="162"/>
+      <c r="C532" s="163"/>
+      <c r="D532" s="164"/>
+      <c r="E532" s="164"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9343,18 +9416,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="177"/>
+      <c r="D549" s="178"/>
+      <c r="E549" s="178"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="161"/>
-      <c r="D550" s="162"/>
-      <c r="E550" s="162"/>
+      <c r="C550" s="163"/>
+      <c r="D550" s="164"/>
+      <c r="E550" s="164"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9505,9 +9578,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="163"/>
-      <c r="D567" s="164"/>
-      <c r="E567" s="164"/>
+      <c r="C567" s="165"/>
+      <c r="D567" s="166"/>
+      <c r="E567" s="166"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9658,9 +9731,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="161"/>
-      <c r="D584" s="162"/>
-      <c r="E584" s="162"/>
+      <c r="C584" s="163"/>
+      <c r="D584" s="164"/>
+      <c r="E584" s="164"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9811,9 +9884,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="161"/>
-      <c r="D601" s="162"/>
-      <c r="E601" s="162"/>
+      <c r="C601" s="163"/>
+      <c r="D601" s="164"/>
+      <c r="E601" s="164"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9964,9 +10037,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="161"/>
-      <c r="D618" s="162"/>
-      <c r="E618" s="162"/>
+      <c r="C618" s="163"/>
+      <c r="D618" s="164"/>
+      <c r="E618" s="164"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10117,9 +10190,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="161"/>
-      <c r="D635" s="162"/>
-      <c r="E635" s="162"/>
+      <c r="C635" s="163"/>
+      <c r="D635" s="164"/>
+      <c r="E635" s="164"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10270,9 +10343,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="161"/>
-      <c r="D652" s="162"/>
-      <c r="E652" s="162"/>
+      <c r="C652" s="163"/>
+      <c r="D652" s="164"/>
+      <c r="E652" s="164"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10423,9 +10496,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="161"/>
-      <c r="D669" s="162"/>
-      <c r="E669" s="162"/>
+      <c r="C669" s="163"/>
+      <c r="D669" s="164"/>
+      <c r="E669" s="164"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10576,9 +10649,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="161"/>
-      <c r="D686" s="162"/>
-      <c r="E686" s="162"/>
+      <c r="C686" s="163"/>
+      <c r="D686" s="164"/>
+      <c r="E686" s="164"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10729,9 +10802,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="161"/>
-      <c r="D703" s="162"/>
-      <c r="E703" s="162"/>
+      <c r="C703" s="163"/>
+      <c r="D703" s="164"/>
+      <c r="E703" s="164"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10882,9 +10955,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="161"/>
-      <c r="D720" s="162"/>
-      <c r="E720" s="162"/>
+      <c r="C720" s="163"/>
+      <c r="D720" s="164"/>
+      <c r="E720" s="164"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11035,9 +11108,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="161"/>
-      <c r="D737" s="162"/>
-      <c r="E737" s="162"/>
+      <c r="C737" s="163"/>
+      <c r="D737" s="164"/>
+      <c r="E737" s="164"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11188,9 +11261,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="161"/>
-      <c r="D754" s="162"/>
-      <c r="E754" s="162"/>
+      <c r="C754" s="163"/>
+      <c r="D754" s="164"/>
+      <c r="E754" s="164"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11341,9 +11414,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="161"/>
-      <c r="D771" s="162"/>
-      <c r="E771" s="162"/>
+      <c r="C771" s="163"/>
+      <c r="D771" s="164"/>
+      <c r="E771" s="164"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11494,9 +11567,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="161"/>
-      <c r="D788" s="162"/>
-      <c r="E788" s="162"/>
+      <c r="C788" s="163"/>
+      <c r="D788" s="164"/>
+      <c r="E788" s="164"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11647,9 +11720,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="161"/>
-      <c r="D805" s="162"/>
-      <c r="E805" s="162"/>
+      <c r="C805" s="163"/>
+      <c r="D805" s="164"/>
+      <c r="E805" s="164"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11800,18 +11873,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="173"/>
-      <c r="D822" s="174"/>
-      <c r="E822" s="174"/>
+      <c r="C822" s="175"/>
+      <c r="D822" s="176"/>
+      <c r="E822" s="176"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="161"/>
-      <c r="D823" s="162"/>
-      <c r="E823" s="162"/>
+      <c r="C823" s="163"/>
+      <c r="D823" s="164"/>
+      <c r="E823" s="164"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11962,9 +12035,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="163"/>
-      <c r="D840" s="164"/>
-      <c r="E840" s="164"/>
+      <c r="C840" s="165"/>
+      <c r="D840" s="166"/>
+      <c r="E840" s="166"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12115,9 +12188,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="161"/>
-      <c r="D857" s="162"/>
-      <c r="E857" s="162"/>
+      <c r="C857" s="163"/>
+      <c r="D857" s="164"/>
+      <c r="E857" s="164"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12268,9 +12341,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="161"/>
-      <c r="D874" s="162"/>
-      <c r="E874" s="162"/>
+      <c r="C874" s="163"/>
+      <c r="D874" s="164"/>
+      <c r="E874" s="164"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12421,9 +12494,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="161"/>
-      <c r="D891" s="162"/>
-      <c r="E891" s="162"/>
+      <c r="C891" s="163"/>
+      <c r="D891" s="164"/>
+      <c r="E891" s="164"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12574,9 +12647,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="161"/>
-      <c r="D908" s="162"/>
-      <c r="E908" s="162"/>
+      <c r="C908" s="163"/>
+      <c r="D908" s="164"/>
+      <c r="E908" s="164"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12727,9 +12800,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="161"/>
-      <c r="D925" s="162"/>
-      <c r="E925" s="162"/>
+      <c r="C925" s="163"/>
+      <c r="D925" s="164"/>
+      <c r="E925" s="164"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12880,9 +12953,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="161"/>
-      <c r="D942" s="162"/>
-      <c r="E942" s="162"/>
+      <c r="C942" s="163"/>
+      <c r="D942" s="164"/>
+      <c r="E942" s="164"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13033,9 +13106,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="161"/>
-      <c r="D959" s="162"/>
-      <c r="E959" s="162"/>
+      <c r="C959" s="163"/>
+      <c r="D959" s="164"/>
+      <c r="E959" s="164"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13186,9 +13259,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="161"/>
-      <c r="D976" s="162"/>
-      <c r="E976" s="162"/>
+      <c r="C976" s="163"/>
+      <c r="D976" s="164"/>
+      <c r="E976" s="164"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13339,9 +13412,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="161"/>
-      <c r="D993" s="162"/>
-      <c r="E993" s="162"/>
+      <c r="C993" s="163"/>
+      <c r="D993" s="164"/>
+      <c r="E993" s="164"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13492,9 +13565,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="161"/>
-      <c r="D1010" s="162"/>
-      <c r="E1010" s="162"/>
+      <c r="C1010" s="163"/>
+      <c r="D1010" s="164"/>
+      <c r="E1010" s="164"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13645,9 +13718,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="161"/>
-      <c r="D1027" s="162"/>
-      <c r="E1027" s="162"/>
+      <c r="C1027" s="163"/>
+      <c r="D1027" s="164"/>
+      <c r="E1027" s="164"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13798,9 +13871,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="161"/>
-      <c r="D1044" s="162"/>
-      <c r="E1044" s="162"/>
+      <c r="C1044" s="163"/>
+      <c r="D1044" s="164"/>
+      <c r="E1044" s="164"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13951,9 +14024,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="161"/>
-      <c r="D1061" s="162"/>
-      <c r="E1061" s="162"/>
+      <c r="C1061" s="163"/>
+      <c r="D1061" s="164"/>
+      <c r="E1061" s="164"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14104,9 +14177,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="161"/>
-      <c r="D1078" s="162"/>
-      <c r="E1078" s="162"/>
+      <c r="C1078" s="163"/>
+      <c r="D1078" s="164"/>
+      <c r="E1078" s="164"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14257,18 +14330,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="171"/>
-      <c r="D1095" s="172"/>
-      <c r="E1095" s="172"/>
+      <c r="C1095" s="173"/>
+      <c r="D1095" s="174"/>
+      <c r="E1095" s="174"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="161"/>
-      <c r="D1096" s="162"/>
-      <c r="E1096" s="162"/>
+      <c r="C1096" s="163"/>
+      <c r="D1096" s="164"/>
+      <c r="E1096" s="164"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14419,9 +14492,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="163"/>
-      <c r="D1113" s="164"/>
-      <c r="E1113" s="164"/>
+      <c r="C1113" s="165"/>
+      <c r="D1113" s="166"/>
+      <c r="E1113" s="166"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14572,9 +14645,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="161"/>
-      <c r="D1130" s="162"/>
-      <c r="E1130" s="162"/>
+      <c r="C1130" s="163"/>
+      <c r="D1130" s="164"/>
+      <c r="E1130" s="164"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14725,9 +14798,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="161"/>
-      <c r="D1147" s="162"/>
-      <c r="E1147" s="162"/>
+      <c r="C1147" s="163"/>
+      <c r="D1147" s="164"/>
+      <c r="E1147" s="164"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14878,9 +14951,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="161"/>
-      <c r="D1164" s="162"/>
-      <c r="E1164" s="162"/>
+      <c r="C1164" s="163"/>
+      <c r="D1164" s="164"/>
+      <c r="E1164" s="164"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15031,9 +15104,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="161"/>
-      <c r="D1181" s="162"/>
-      <c r="E1181" s="162"/>
+      <c r="C1181" s="163"/>
+      <c r="D1181" s="164"/>
+      <c r="E1181" s="164"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15184,9 +15257,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="161"/>
-      <c r="D1198" s="162"/>
-      <c r="E1198" s="162"/>
+      <c r="C1198" s="163"/>
+      <c r="D1198" s="164"/>
+      <c r="E1198" s="164"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15337,9 +15410,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="161"/>
-      <c r="D1215" s="162"/>
-      <c r="E1215" s="162"/>
+      <c r="C1215" s="163"/>
+      <c r="D1215" s="164"/>
+      <c r="E1215" s="164"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15490,9 +15563,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="161"/>
-      <c r="D1232" s="162"/>
-      <c r="E1232" s="162"/>
+      <c r="C1232" s="163"/>
+      <c r="D1232" s="164"/>
+      <c r="E1232" s="164"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15643,9 +15716,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="161"/>
-      <c r="D1249" s="162"/>
-      <c r="E1249" s="162"/>
+      <c r="C1249" s="163"/>
+      <c r="D1249" s="164"/>
+      <c r="E1249" s="164"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15796,9 +15869,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="161"/>
-      <c r="D1266" s="162"/>
-      <c r="E1266" s="162"/>
+      <c r="C1266" s="163"/>
+      <c r="D1266" s="164"/>
+      <c r="E1266" s="164"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15949,9 +16022,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="161"/>
-      <c r="D1283" s="162"/>
-      <c r="E1283" s="162"/>
+      <c r="C1283" s="163"/>
+      <c r="D1283" s="164"/>
+      <c r="E1283" s="164"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16102,9 +16175,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="161"/>
-      <c r="D1300" s="162"/>
-      <c r="E1300" s="162"/>
+      <c r="C1300" s="163"/>
+      <c r="D1300" s="164"/>
+      <c r="E1300" s="164"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16255,9 +16328,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="161"/>
-      <c r="D1317" s="162"/>
-      <c r="E1317" s="162"/>
+      <c r="C1317" s="163"/>
+      <c r="D1317" s="164"/>
+      <c r="E1317" s="164"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16408,9 +16481,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="161"/>
-      <c r="D1334" s="162"/>
-      <c r="E1334" s="162"/>
+      <c r="C1334" s="163"/>
+      <c r="D1334" s="164"/>
+      <c r="E1334" s="164"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16561,9 +16634,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="161"/>
-      <c r="D1351" s="162"/>
-      <c r="E1351" s="162"/>
+      <c r="C1351" s="163"/>
+      <c r="D1351" s="164"/>
+      <c r="E1351" s="164"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16714,18 +16787,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="169"/>
-      <c r="D1368" s="170"/>
-      <c r="E1368" s="170"/>
+      <c r="C1368" s="171"/>
+      <c r="D1368" s="172"/>
+      <c r="E1368" s="172"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="161"/>
-      <c r="D1369" s="162"/>
-      <c r="E1369" s="162"/>
+      <c r="C1369" s="163"/>
+      <c r="D1369" s="164"/>
+      <c r="E1369" s="164"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16876,9 +16949,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="163"/>
-      <c r="D1386" s="164"/>
-      <c r="E1386" s="164"/>
+      <c r="C1386" s="165"/>
+      <c r="D1386" s="166"/>
+      <c r="E1386" s="166"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17029,9 +17102,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="161"/>
-      <c r="D1403" s="162"/>
-      <c r="E1403" s="162"/>
+      <c r="C1403" s="163"/>
+      <c r="D1403" s="164"/>
+      <c r="E1403" s="164"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17182,9 +17255,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="161"/>
-      <c r="D1420" s="162"/>
-      <c r="E1420" s="162"/>
+      <c r="C1420" s="163"/>
+      <c r="D1420" s="164"/>
+      <c r="E1420" s="164"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17335,9 +17408,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="161"/>
-      <c r="D1437" s="162"/>
-      <c r="E1437" s="162"/>
+      <c r="C1437" s="163"/>
+      <c r="D1437" s="164"/>
+      <c r="E1437" s="164"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17488,9 +17561,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="161"/>
-      <c r="D1454" s="162"/>
-      <c r="E1454" s="162"/>
+      <c r="C1454" s="163"/>
+      <c r="D1454" s="164"/>
+      <c r="E1454" s="164"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17641,9 +17714,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="161"/>
-      <c r="D1471" s="162"/>
-      <c r="E1471" s="162"/>
+      <c r="C1471" s="163"/>
+      <c r="D1471" s="164"/>
+      <c r="E1471" s="164"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17794,9 +17867,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="161"/>
-      <c r="D1488" s="162"/>
-      <c r="E1488" s="162"/>
+      <c r="C1488" s="163"/>
+      <c r="D1488" s="164"/>
+      <c r="E1488" s="164"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17947,9 +18020,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="161"/>
-      <c r="D1505" s="162"/>
-      <c r="E1505" s="162"/>
+      <c r="C1505" s="163"/>
+      <c r="D1505" s="164"/>
+      <c r="E1505" s="164"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18100,9 +18173,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="161"/>
-      <c r="D1522" s="162"/>
-      <c r="E1522" s="162"/>
+      <c r="C1522" s="163"/>
+      <c r="D1522" s="164"/>
+      <c r="E1522" s="164"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18253,9 +18326,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="161"/>
-      <c r="D1539" s="162"/>
-      <c r="E1539" s="162"/>
+      <c r="C1539" s="163"/>
+      <c r="D1539" s="164"/>
+      <c r="E1539" s="164"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18406,9 +18479,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="161"/>
-      <c r="D1556" s="162"/>
-      <c r="E1556" s="162"/>
+      <c r="C1556" s="163"/>
+      <c r="D1556" s="164"/>
+      <c r="E1556" s="164"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18559,9 +18632,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="161"/>
-      <c r="D1573" s="162"/>
-      <c r="E1573" s="162"/>
+      <c r="C1573" s="163"/>
+      <c r="D1573" s="164"/>
+      <c r="E1573" s="164"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18712,9 +18785,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="161"/>
-      <c r="D1590" s="162"/>
-      <c r="E1590" s="162"/>
+      <c r="C1590" s="163"/>
+      <c r="D1590" s="164"/>
+      <c r="E1590" s="164"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18865,9 +18938,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="161"/>
-      <c r="D1607" s="162"/>
-      <c r="E1607" s="162"/>
+      <c r="C1607" s="163"/>
+      <c r="D1607" s="164"/>
+      <c r="E1607" s="164"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19018,9 +19091,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="161"/>
-      <c r="D1624" s="162"/>
-      <c r="E1624" s="162"/>
+      <c r="C1624" s="163"/>
+      <c r="D1624" s="164"/>
+      <c r="E1624" s="164"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19171,18 +19244,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="167"/>
-      <c r="D1641" s="168"/>
-      <c r="E1641" s="168"/>
+      <c r="C1641" s="169"/>
+      <c r="D1641" s="170"/>
+      <c r="E1641" s="170"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="161"/>
-      <c r="D1642" s="162"/>
-      <c r="E1642" s="162"/>
+      <c r="C1642" s="163"/>
+      <c r="D1642" s="164"/>
+      <c r="E1642" s="164"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19333,9 +19406,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="163"/>
-      <c r="D1659" s="164"/>
-      <c r="E1659" s="164"/>
+      <c r="C1659" s="165"/>
+      <c r="D1659" s="166"/>
+      <c r="E1659" s="166"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19486,9 +19559,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="161"/>
-      <c r="D1676" s="162"/>
-      <c r="E1676" s="162"/>
+      <c r="C1676" s="163"/>
+      <c r="D1676" s="164"/>
+      <c r="E1676" s="164"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19639,9 +19712,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="161"/>
-      <c r="D1693" s="162"/>
-      <c r="E1693" s="162"/>
+      <c r="C1693" s="163"/>
+      <c r="D1693" s="164"/>
+      <c r="E1693" s="164"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19792,9 +19865,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="161"/>
-      <c r="D1710" s="162"/>
-      <c r="E1710" s="162"/>
+      <c r="C1710" s="163"/>
+      <c r="D1710" s="164"/>
+      <c r="E1710" s="164"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19945,9 +20018,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="161"/>
-      <c r="D1727" s="162"/>
-      <c r="E1727" s="162"/>
+      <c r="C1727" s="163"/>
+      <c r="D1727" s="164"/>
+      <c r="E1727" s="164"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20098,9 +20171,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="161"/>
-      <c r="D1744" s="162"/>
-      <c r="E1744" s="162"/>
+      <c r="C1744" s="163"/>
+      <c r="D1744" s="164"/>
+      <c r="E1744" s="164"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20251,9 +20324,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="161"/>
-      <c r="D1761" s="162"/>
-      <c r="E1761" s="162"/>
+      <c r="C1761" s="163"/>
+      <c r="D1761" s="164"/>
+      <c r="E1761" s="164"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20404,9 +20477,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="161"/>
-      <c r="D1778" s="162"/>
-      <c r="E1778" s="162"/>
+      <c r="C1778" s="163"/>
+      <c r="D1778" s="164"/>
+      <c r="E1778" s="164"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20557,9 +20630,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="161"/>
-      <c r="D1795" s="162"/>
-      <c r="E1795" s="162"/>
+      <c r="C1795" s="163"/>
+      <c r="D1795" s="164"/>
+      <c r="E1795" s="164"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20710,9 +20783,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="161"/>
-      <c r="D1812" s="162"/>
-      <c r="E1812" s="162"/>
+      <c r="C1812" s="163"/>
+      <c r="D1812" s="164"/>
+      <c r="E1812" s="164"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20863,9 +20936,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="161"/>
-      <c r="D1829" s="162"/>
-      <c r="E1829" s="162"/>
+      <c r="C1829" s="163"/>
+      <c r="D1829" s="164"/>
+      <c r="E1829" s="164"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21016,9 +21089,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="161"/>
-      <c r="D1846" s="162"/>
-      <c r="E1846" s="162"/>
+      <c r="C1846" s="163"/>
+      <c r="D1846" s="164"/>
+      <c r="E1846" s="164"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21169,9 +21242,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="161"/>
-      <c r="D1863" s="162"/>
-      <c r="E1863" s="162"/>
+      <c r="C1863" s="163"/>
+      <c r="D1863" s="164"/>
+      <c r="E1863" s="164"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21322,9 +21395,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="161"/>
-      <c r="D1880" s="162"/>
-      <c r="E1880" s="162"/>
+      <c r="C1880" s="163"/>
+      <c r="D1880" s="164"/>
+      <c r="E1880" s="164"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21475,9 +21548,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="161"/>
-      <c r="D1897" s="162"/>
-      <c r="E1897" s="162"/>
+      <c r="C1897" s="163"/>
+      <c r="D1897" s="164"/>
+      <c r="E1897" s="164"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21628,18 +21701,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="165"/>
-      <c r="D1914" s="166"/>
-      <c r="E1914" s="166"/>
+      <c r="C1914" s="167"/>
+      <c r="D1914" s="168"/>
+      <c r="E1914" s="168"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="161"/>
-      <c r="D1915" s="162"/>
-      <c r="E1915" s="162"/>
+      <c r="C1915" s="163"/>
+      <c r="D1915" s="164"/>
+      <c r="E1915" s="164"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21790,9 +21863,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="163"/>
-      <c r="D1932" s="164"/>
-      <c r="E1932" s="164"/>
+      <c r="C1932" s="165"/>
+      <c r="D1932" s="166"/>
+      <c r="E1932" s="166"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21943,9 +22016,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="161"/>
-      <c r="D1949" s="162"/>
-      <c r="E1949" s="162"/>
+      <c r="C1949" s="163"/>
+      <c r="D1949" s="164"/>
+      <c r="E1949" s="164"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22096,9 +22169,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="161"/>
-      <c r="D1966" s="162"/>
-      <c r="E1966" s="162"/>
+      <c r="C1966" s="163"/>
+      <c r="D1966" s="164"/>
+      <c r="E1966" s="164"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22249,9 +22322,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="161"/>
-      <c r="D1983" s="162"/>
-      <c r="E1983" s="162"/>
+      <c r="C1983" s="163"/>
+      <c r="D1983" s="164"/>
+      <c r="E1983" s="164"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22402,9 +22475,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="161"/>
-      <c r="D2000" s="162"/>
-      <c r="E2000" s="162"/>
+      <c r="C2000" s="163"/>
+      <c r="D2000" s="164"/>
+      <c r="E2000" s="164"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22555,9 +22628,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="161"/>
-      <c r="D2017" s="162"/>
-      <c r="E2017" s="162"/>
+      <c r="C2017" s="163"/>
+      <c r="D2017" s="164"/>
+      <c r="E2017" s="164"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22708,9 +22781,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="161"/>
-      <c r="D2034" s="162"/>
-      <c r="E2034" s="162"/>
+      <c r="C2034" s="163"/>
+      <c r="D2034" s="164"/>
+      <c r="E2034" s="164"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22861,9 +22934,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="161"/>
-      <c r="D2051" s="162"/>
-      <c r="E2051" s="162"/>
+      <c r="C2051" s="163"/>
+      <c r="D2051" s="164"/>
+      <c r="E2051" s="164"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23014,9 +23087,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="161"/>
-      <c r="D2068" s="162"/>
-      <c r="E2068" s="162"/>
+      <c r="C2068" s="163"/>
+      <c r="D2068" s="164"/>
+      <c r="E2068" s="164"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23167,9 +23240,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="161"/>
-      <c r="D2085" s="162"/>
-      <c r="E2085" s="162"/>
+      <c r="C2085" s="163"/>
+      <c r="D2085" s="164"/>
+      <c r="E2085" s="164"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23320,9 +23393,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="161"/>
-      <c r="D2102" s="162"/>
-      <c r="E2102" s="162"/>
+      <c r="C2102" s="163"/>
+      <c r="D2102" s="164"/>
+      <c r="E2102" s="164"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23473,9 +23546,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="161"/>
-      <c r="D2119" s="162"/>
-      <c r="E2119" s="162"/>
+      <c r="C2119" s="163"/>
+      <c r="D2119" s="164"/>
+      <c r="E2119" s="164"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23626,9 +23699,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="161"/>
-      <c r="D2136" s="162"/>
-      <c r="E2136" s="162"/>
+      <c r="C2136" s="163"/>
+      <c r="D2136" s="164"/>
+      <c r="E2136" s="164"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23779,9 +23852,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="161"/>
-      <c r="D2153" s="162"/>
-      <c r="E2153" s="162"/>
+      <c r="C2153" s="163"/>
+      <c r="D2153" s="164"/>
+      <c r="E2153" s="164"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23932,9 +24005,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="161"/>
-      <c r="D2170" s="162"/>
-      <c r="E2170" s="162"/>
+      <c r="C2170" s="163"/>
+      <c r="D2170" s="164"/>
+      <c r="E2170" s="164"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24220,7 +24293,7 @@
     <mergeCell ref="C2136:E2136"/>
     <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24245,51 +24318,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
+      <c r="I1" s="190"/>
+      <c r="J1" s="190"/>
+      <c r="K1" s="190"/>
+      <c r="L1" s="190"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
-      <c r="J2" s="186"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="187"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
+      <c r="K2" s="188"/>
+      <c r="L2" s="189"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="184" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="183"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="184"/>
+      <c r="B3" s="185"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="186"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24506,19 +24579,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="184" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="183"/>
-      <c r="E20" s="183"/>
-      <c r="F20" s="183"/>
-      <c r="G20" s="183"/>
-      <c r="H20" s="183"/>
-      <c r="I20" s="183"/>
-      <c r="J20" s="183"/>
-      <c r="K20" s="184"/>
+      <c r="B20" s="185"/>
+      <c r="C20" s="185"/>
+      <c r="D20" s="185"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="185"/>
+      <c r="G20" s="185"/>
+      <c r="H20" s="185"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="185"/>
+      <c r="K20" s="186"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24735,19 +24808,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="182" t="s">
+      <c r="A37" s="184" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="183"/>
-      <c r="C37" s="183"/>
-      <c r="D37" s="183"/>
-      <c r="E37" s="183"/>
-      <c r="F37" s="183"/>
-      <c r="G37" s="183"/>
-      <c r="H37" s="183"/>
-      <c r="I37" s="183"/>
-      <c r="J37" s="183"/>
-      <c r="K37" s="184"/>
+      <c r="B37" s="185"/>
+      <c r="C37" s="185"/>
+      <c r="D37" s="185"/>
+      <c r="E37" s="185"/>
+      <c r="F37" s="185"/>
+      <c r="G37" s="185"/>
+      <c r="H37" s="185"/>
+      <c r="I37" s="185"/>
+      <c r="J37" s="185"/>
+      <c r="K37" s="186"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -24971,7 +25044,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25005,28 +25078,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="189"/>
+      <c r="A3" s="191"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="190"/>
+      <c r="A4" s="192"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="190"/>
+      <c r="A5" s="192"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="190"/>
+      <c r="A6" s="192"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="190"/>
+      <c r="A7" s="192"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="190"/>
+      <c r="A8" s="192"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="190"/>
+      <c r="A9" s="192"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="191"/>
+      <c r="A10" s="193"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25182,7 +25255,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25209,10 +25282,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="192" t="s">
+      <c r="B1" s="194" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="193"/>
+      <c r="C1" s="195"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25223,7 +25296,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="196" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25237,7 +25310,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="195"/>
+      <c r="A4" s="197"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25249,7 +25322,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="195"/>
+      <c r="A5" s="197"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25258,7 +25331,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="195"/>
+      <c r="A6" s="197"/>
       <c r="B6" s="139" t="s">
         <v>212</v>
       </c>
@@ -25270,7 +25343,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="195"/>
+      <c r="A7" s="197"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25282,7 +25355,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="195"/>
+      <c r="A8" s="197"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25291,7 +25364,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="196"/>
+      <c r="A9" s="198"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25306,7 +25379,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="194" t="s">
+      <c r="A11" s="196" t="s">
         <v>211</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25320,7 +25393,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="195"/>
+      <c r="A12" s="197"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25332,7 +25405,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="195"/>
+      <c r="A13" s="197"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25341,7 +25414,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="195"/>
+      <c r="A14" s="197"/>
       <c r="B14" s="139" t="s">
         <v>212</v>
       </c>
@@ -25353,7 +25426,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="195"/>
+      <c r="A15" s="197"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25365,7 +25438,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="195"/>
+      <c r="A16" s="197"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25374,7 +25447,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="196"/>
+      <c r="A17" s="198"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25389,7 +25462,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="194" t="s">
+      <c r="A19" s="196" t="s">
         <v>211</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25398,7 +25471,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="195"/>
+      <c r="A20" s="197"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25408,14 +25481,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="195"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="195"/>
+      <c r="A22" s="197"/>
       <c r="B22" s="139" t="s">
         <v>212</v>
       </c>
@@ -25425,7 +25498,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="195"/>
+      <c r="A23" s="197"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25435,14 +25508,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="195"/>
+      <c r="A24" s="197"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="196"/>
+      <c r="A25" s="198"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25455,7 +25528,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25477,147 +25550,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="208" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="207"/>
+      <c r="B1" s="209"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="205" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="204"/>
+      <c r="B2" s="206"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="207" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="204"/>
+      <c r="B3" s="206"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="210"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="212"/>
+      <c r="B4" s="213"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="208" t="s">
+      <c r="A5" s="210" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="209"/>
+      <c r="B5" s="211"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="214" t="s">
+      <c r="A7" s="216" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="215"/>
+      <c r="B7" s="217"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="214" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="213"/>
+      <c r="B9" s="215"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200"/>
+      <c r="A10" s="201"/>
+      <c r="B10" s="202"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="203" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="204"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="203" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="204"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="203" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="204"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="203" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="204"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="203" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="204"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="203" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="204"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="199" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="214" t="s">
+      <c r="A19" s="216" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="215"/>
+      <c r="B19" s="217"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="214" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="213"/>
+      <c r="B21" s="215"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="199"/>
-      <c r="B22" s="200"/>
+      <c r="A22" s="201"/>
+      <c r="B22" s="202"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="203" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="204"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="203"/>
+      <c r="B24" s="204"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="203" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="204"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="203" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="204"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Level 4 done, 1137 frames ahead.  692 saved in with a radical new strategy that eliminates the need to stay on the log auto-scroller style
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="247">
   <si>
     <t>Notes</t>
   </si>
@@ -759,6 +759,36 @@
   </si>
   <si>
     <t>Dragon appears</t>
+  </si>
+  <si>
+    <t>End Screen 1</t>
+  </si>
+  <si>
+    <t>Door #2</t>
+  </si>
+  <si>
+    <t>Door #1</t>
+  </si>
+  <si>
+    <t>Door #3</t>
+  </si>
+  <si>
+    <t>Door #4</t>
+  </si>
+  <si>
+    <t>Door #5</t>
+  </si>
+  <si>
+    <t>Door #6</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Dragon Appears</t>
+  </si>
+  <si>
+    <t>Down Water Fall</t>
   </si>
 </sst>
 </file>
@@ -2456,8 +2486,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="6" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2486,7 +2516,7 @@
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="I1" s="141" t="s">
         <v>204</v>
@@ -2508,7 +2538,7 @@
       <c r="G2" s="140"/>
       <c r="H2" s="144">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>0</v>
+        <v>18.95</v>
       </c>
       <c r="I2" s="141" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -3342,100 +3372,154 @@
     </row>
     <row r="56" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="155"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
+      <c r="B56" s="218" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="101">
+        <v>11545</v>
+      </c>
+      <c r="D56" s="101">
+        <v>11953</v>
+      </c>
       <c r="E56" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="155"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="101"/>
+      <c r="B57" s="218" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="101">
+        <v>11841</v>
+      </c>
+      <c r="D57" s="101">
+        <v>12249</v>
+      </c>
       <c r="E57" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="155"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="101"/>
+      <c r="B58" s="218" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="101">
+        <v>12142</v>
+      </c>
+      <c r="D58" s="101">
+        <v>12548</v>
+      </c>
       <c r="E58" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>406</v>
       </c>
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="155"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="101"/>
-      <c r="D59" s="101"/>
+      <c r="B59" s="218" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" s="101">
+        <v>12270</v>
+      </c>
+      <c r="D59" s="101">
+        <v>12672</v>
+      </c>
       <c r="E59" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>402</v>
       </c>
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="155"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="101"/>
+      <c r="B60" s="218" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="101">
+        <v>12574</v>
+      </c>
+      <c r="D60" s="101">
+        <v>12985</v>
+      </c>
       <c r="E60" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="155"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="101"/>
+      <c r="B61" s="218" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" s="101">
+        <v>12704</v>
+      </c>
+      <c r="D61" s="101">
+        <v>13117</v>
+      </c>
       <c r="E61" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="155"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="101"/>
+      <c r="B62" s="218" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" s="101">
+        <v>12860</v>
+      </c>
+      <c r="D62" s="101">
+        <v>13271</v>
+      </c>
       <c r="E62" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="155"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="101"/>
-      <c r="D63" s="101"/>
+      <c r="B63" s="218" t="s">
+        <v>244</v>
+      </c>
+      <c r="C63" s="101">
+        <v>13072</v>
+      </c>
+      <c r="D63" s="101">
+        <v>13490</v>
+      </c>
       <c r="E63" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>418</v>
       </c>
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="155"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="101"/>
-      <c r="D64" s="101"/>
+      <c r="B64" s="218" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64" s="101">
+        <v>14445</v>
+      </c>
+      <c r="D64" s="101">
+        <v>14889</v>
+      </c>
       <c r="E64" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="F64" s="105"/>
     </row>
@@ -3466,11 +3550,15 @@
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
+      <c r="C67" s="99">
+        <v>14824</v>
+      </c>
+      <c r="D67" s="99">
+        <v>15269</v>
+      </c>
       <c r="E67" s="125">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="F67" s="104"/>
     </row>
@@ -3483,24 +3571,24 @@
       </c>
       <c r="C68" s="103">
         <f>C67-C54</f>
-        <v>-10958</v>
+        <v>3866</v>
       </c>
       <c r="D68" s="103">
         <f>D67-D54</f>
-        <v>-11356</v>
+        <v>3913</v>
       </c>
       <c r="E68" s="126">
         <f>E67-E54</f>
-        <v>-398</v>
+        <v>47</v>
       </c>
       <c r="F68" s="108"/>
       <c r="G68" s="112">
         <f>E68</f>
-        <v>-398</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="154" t="s">
         <v>172</v>
       </c>
@@ -3520,53 +3608,75 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="155"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="99"/>
-      <c r="D71" s="99"/>
+      <c r="C71" s="99">
+        <v>14824</v>
+      </c>
+      <c r="D71" s="99">
+        <v>15269</v>
+      </c>
       <c r="E71" s="123">
         <f t="shared" ref="E71:E84" si="5">IF(AND(C71&gt;0,D71&gt;0), D71-C71, 0)</f>
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="F71" s="104"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A72" s="155"/>
-      <c r="B72" s="100"/>
-      <c r="C72" s="101"/>
-      <c r="D72" s="101"/>
+      <c r="B72" s="218" t="s">
+        <v>245</v>
+      </c>
+      <c r="C72" s="101">
+        <v>14824</v>
+      </c>
+      <c r="D72" s="101">
+        <v>15269</v>
+      </c>
       <c r="E72" s="124">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="F72" s="105"/>
     </row>
-    <row r="73" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="155"/>
-      <c r="B73" s="100"/>
-      <c r="C73" s="101"/>
-      <c r="D73" s="101"/>
+      <c r="B73" s="218" t="s">
+        <v>246</v>
+      </c>
+      <c r="C73" s="101">
+        <v>16243</v>
+      </c>
+      <c r="D73" s="101">
+        <v>17380</v>
+      </c>
       <c r="E73" s="123">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="F73" s="105"/>
     </row>
-    <row r="74" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="155"/>
-      <c r="B74" s="100"/>
-      <c r="C74" s="101"/>
-      <c r="D74" s="101"/>
+      <c r="B74" s="218" t="s">
+        <v>235</v>
+      </c>
+      <c r="C74" s="101">
+        <v>17446</v>
+      </c>
+      <c r="D74" s="101">
+        <v>18583</v>
+      </c>
       <c r="E74" s="123">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="F74" s="105"/>
     </row>
-    <row r="75" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="155"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
@@ -3577,7 +3687,7 @@
       </c>
       <c r="F75" s="105"/>
     </row>
-    <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="155"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
@@ -3588,7 +3698,7 @@
       </c>
       <c r="F76" s="105"/>
     </row>
-    <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="155"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
@@ -3599,7 +3709,7 @@
       </c>
       <c r="F77" s="105"/>
     </row>
-    <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="155"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
@@ -3610,7 +3720,7 @@
       </c>
       <c r="F78" s="105"/>
     </row>
-    <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="155"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
@@ -3621,7 +3731,7 @@
       </c>
       <c r="F79" s="105"/>
     </row>
-    <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="155"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
@@ -3632,7 +3742,7 @@
       </c>
       <c r="F80" s="105"/>
     </row>
-    <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="155"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
@@ -3643,7 +3753,7 @@
       </c>
       <c r="F81" s="105"/>
     </row>
-    <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="155"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
@@ -3654,7 +3764,7 @@
       </c>
       <c r="F82" s="105"/>
     </row>
-    <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="155"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
@@ -3665,20 +3775,24 @@
       </c>
       <c r="F83" s="105"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="155"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C84" s="99"/>
-      <c r="D84" s="99"/>
+      <c r="C84" s="99">
+        <v>17818</v>
+      </c>
+      <c r="D84" s="99">
+        <v>18955</v>
+      </c>
       <c r="E84" s="125">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="F84" s="104"/>
     </row>
-    <row r="85" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="116">
         <v>4</v>
       </c>
@@ -3687,23 +3801,24 @@
       </c>
       <c r="C85" s="103">
         <f>C84-C71</f>
-        <v>0</v>
+        <v>2994</v>
       </c>
       <c r="D85" s="103">
         <f>D84-D71</f>
-        <v>0</v>
+        <v>3686</v>
       </c>
       <c r="E85" s="126">
         <f>E84-E71</f>
-        <v>0</v>
+        <v>692</v>
       </c>
       <c r="F85" s="107"/>
       <c r="G85" s="112">
         <f>E85</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="156" t="s">
         <v>173</v>
       </c>
@@ -3723,31 +3838,41 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="155"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C88" s="99"/>
-      <c r="D88" s="99"/>
+      <c r="C88" s="99">
+        <v>17818</v>
+      </c>
+      <c r="D88" s="99">
+        <v>18955</v>
+      </c>
       <c r="E88" s="123">
         <f t="shared" ref="E88:E101" si="6">IF(AND(C88&gt;0,D88&gt;0), D88-C88, 0)</f>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="F88" s="104"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A89" s="155"/>
-      <c r="B89" s="100"/>
-      <c r="C89" s="101"/>
-      <c r="D89" s="101"/>
+      <c r="B89" s="218" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" s="101">
+        <v>17818</v>
+      </c>
+      <c r="D89" s="101">
+        <v>18955</v>
+      </c>
       <c r="E89" s="124">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="F89" s="105"/>
     </row>
-    <row r="90" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="155"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
@@ -3758,7 +3883,7 @@
       </c>
       <c r="F90" s="105"/>
     </row>
-    <row r="91" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="155"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
@@ -3769,7 +3894,7 @@
       </c>
       <c r="F91" s="105"/>
     </row>
-    <row r="92" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="155"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
@@ -3780,7 +3905,7 @@
       </c>
       <c r="F92" s="105"/>
     </row>
-    <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="155"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
@@ -3791,7 +3916,7 @@
       </c>
       <c r="F93" s="105"/>
     </row>
-    <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="155"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
@@ -3802,7 +3927,7 @@
       </c>
       <c r="F94" s="105"/>
     </row>
-    <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="155"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
@@ -3813,7 +3938,7 @@
       </c>
       <c r="F95" s="105"/>
     </row>
-    <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="155"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
@@ -3824,7 +3949,7 @@
       </c>
       <c r="F96" s="105"/>
     </row>
-    <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="155"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
@@ -3835,7 +3960,7 @@
       </c>
       <c r="F97" s="105"/>
     </row>
-    <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="155"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
@@ -3846,7 +3971,7 @@
       </c>
       <c r="F98" s="105"/>
     </row>
-    <row r="99" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="155"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
@@ -3857,7 +3982,7 @@
       </c>
       <c r="F99" s="105"/>
     </row>
-    <row r="100" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="155"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
@@ -3868,7 +3993,7 @@
       </c>
       <c r="F100" s="105"/>
     </row>
-    <row r="101" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="155"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
@@ -3881,7 +4006,7 @@
       </c>
       <c r="F101" s="104"/>
     </row>
-    <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="102" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="154" t="s">
         <v>174</v>
@@ -25337,7 +25462,7 @@
       </c>
       <c r="C6" s="134">
         <f>FrameCounts!H2</f>
-        <v>0</v>
+        <v>18.95</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -25349,7 +25474,7 @@
       </c>
       <c r="C7" s="135">
         <f>C6/60</f>
-        <v>0</v>
+        <v>0.3158333333333333</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>

</xml_diff>

<commit_message>
Dragon Egg - more progress, almost done
</commit_message>
<xml_diff>
--- a/DragonEgg/DEgg.xlsx
+++ b/DragonEgg/DEgg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="252">
   <si>
     <t>Notes</t>
   </si>
@@ -790,6 +790,21 @@
   <si>
     <t>Down Water Fall</t>
   </si>
+  <si>
+    <t>Begin Elevator</t>
+  </si>
+  <si>
+    <t>Start Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Elevator</t>
+  </si>
 </sst>
 </file>
 
@@ -799,10 +814,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1750,34 +1772,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1785,208 +1807,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1996,10 +2018,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2020,18 +2042,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2050,124 +2075,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2486,8 +2514,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <pane ySplit="6" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2503,16 +2531,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="159"/>
+      <c r="C1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65531)</f>
@@ -2528,7 +2556,7 @@
       <c r="A2" s="142" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="142">
+      <c r="B2" s="220">
         <v>2</v>
       </c>
       <c r="C2" s="143"/>
@@ -2536,9 +2564,8 @@
       <c r="E2" s="143"/>
       <c r="F2" s="143"/>
       <c r="G2" s="140"/>
-      <c r="H2" s="144">
-        <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>18.95</v>
+      <c r="H2" s="144" t="s">
+        <v>249</v>
       </c>
       <c r="I2" s="141" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
@@ -2590,10 +2617,10 @@
       <c r="B5" s="147" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2609,10 +2636,10 @@
       <c r="B6" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2630,7 +2657,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2650,7 +2677,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="155"/>
+      <c r="A9" s="156"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
@@ -2664,7 +2691,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
+      <c r="A10" s="156"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2681,7 +2708,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
+      <c r="A11" s="156"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2698,7 +2725,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
+      <c r="A12" s="156"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2715,7 +2742,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
+      <c r="A13" s="156"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2726,7 +2753,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
+      <c r="A14" s="156"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2737,7 +2764,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
+      <c r="A15" s="156"/>
       <c r="B15" s="148" t="s">
         <v>186</v>
       </c>
@@ -2754,7 +2781,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="155"/>
+      <c r="A16" s="156"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
@@ -2797,7 +2824,7 @@
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:10" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="157" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2817,7 +2844,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="155"/>
+      <c r="A20" s="156"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
@@ -2834,7 +2861,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
+      <c r="A21" s="156"/>
       <c r="B21" s="148" t="s">
         <v>218</v>
       </c>
@@ -2851,7 +2878,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
+      <c r="A22" s="156"/>
       <c r="B22" s="148" t="s">
         <v>219</v>
       </c>
@@ -2874,7 +2901,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
+      <c r="A23" s="156"/>
       <c r="B23" s="149" t="s">
         <v>226</v>
       </c>
@@ -2894,7 +2921,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
+      <c r="A24" s="156"/>
       <c r="B24" s="148" t="s">
         <v>223</v>
       </c>
@@ -2911,7 +2938,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
+      <c r="A25" s="156"/>
       <c r="B25" s="148" t="s">
         <v>225</v>
       </c>
@@ -2928,7 +2955,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="155"/>
+      <c r="A26" s="156"/>
       <c r="B26" s="150" t="s">
         <v>227</v>
       </c>
@@ -2948,7 +2975,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
+      <c r="A27" s="156"/>
       <c r="B27" s="151" t="s">
         <v>228</v>
       </c>
@@ -2965,7 +2992,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="155"/>
+      <c r="A28" s="156"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2976,7 +3003,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="155"/>
+      <c r="A29" s="156"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2987,7 +3014,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="155"/>
+      <c r="A30" s="156"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2998,7 +3025,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="155"/>
+      <c r="A31" s="156"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -3009,7 +3036,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:10" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="155"/>
+      <c r="A32" s="156"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -3020,7 +3047,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="155"/>
+      <c r="A33" s="156"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
       </c>
@@ -3063,7 +3090,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="154" t="s">
+      <c r="A36" s="155" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -3083,7 +3110,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="155"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="98" t="s">
         <v>184</v>
       </c>
@@ -3100,7 +3127,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="155"/>
+      <c r="A38" s="156"/>
       <c r="B38" s="151" t="s">
         <v>229</v>
       </c>
@@ -3117,7 +3144,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="155"/>
+      <c r="A39" s="156"/>
       <c r="B39" s="152" t="s">
         <v>230</v>
       </c>
@@ -3134,7 +3161,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="155"/>
+      <c r="A40" s="156"/>
       <c r="B40" s="152" t="s">
         <v>231</v>
       </c>
@@ -3151,7 +3178,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="155"/>
+      <c r="A41" s="156"/>
       <c r="B41" s="153" t="s">
         <v>232</v>
       </c>
@@ -3168,7 +3195,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="155"/>
+      <c r="A42" s="156"/>
       <c r="B42" s="153" t="s">
         <v>233</v>
       </c>
@@ -3185,7 +3212,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="155"/>
+      <c r="A43" s="156"/>
       <c r="B43" s="153" t="s">
         <v>234</v>
       </c>
@@ -3202,8 +3229,8 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="155"/>
-      <c r="B44" s="218" t="s">
+      <c r="A44" s="156"/>
+      <c r="B44" s="154" t="s">
         <v>235</v>
       </c>
       <c r="C44" s="101">
@@ -3219,7 +3246,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="155"/>
+      <c r="A45" s="156"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3230,7 +3257,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="155"/>
+      <c r="A46" s="156"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3241,7 +3268,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="155"/>
+      <c r="A47" s="156"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3252,7 +3279,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="155"/>
+      <c r="A48" s="156"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3263,7 +3290,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="155"/>
+      <c r="A49" s="156"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3274,7 +3301,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="155"/>
+      <c r="A50" s="156"/>
       <c r="B50" s="98" t="s">
         <v>187</v>
       </c>
@@ -3317,7 +3344,7 @@
     </row>
     <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="157" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="109" t="s">
@@ -3337,7 +3364,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="155"/>
+      <c r="A54" s="156"/>
       <c r="B54" s="98" t="s">
         <v>184</v>
       </c>
@@ -3354,8 +3381,8 @@
       <c r="F54" s="104"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="155"/>
-      <c r="B55" s="218" t="s">
+      <c r="A55" s="156"/>
+      <c r="B55" s="154" t="s">
         <v>236</v>
       </c>
       <c r="C55" s="101">
@@ -3371,8 +3398,8 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="155"/>
-      <c r="B56" s="218" t="s">
+      <c r="A56" s="156"/>
+      <c r="B56" s="154" t="s">
         <v>237</v>
       </c>
       <c r="C56" s="101">
@@ -3388,8 +3415,8 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="155"/>
-      <c r="B57" s="218" t="s">
+      <c r="A57" s="156"/>
+      <c r="B57" s="154" t="s">
         <v>239</v>
       </c>
       <c r="C57" s="101">
@@ -3405,8 +3432,8 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="155"/>
-      <c r="B58" s="218" t="s">
+      <c r="A58" s="156"/>
+      <c r="B58" s="154" t="s">
         <v>238</v>
       </c>
       <c r="C58" s="101">
@@ -3422,8 +3449,8 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="155"/>
-      <c r="B59" s="218" t="s">
+      <c r="A59" s="156"/>
+      <c r="B59" s="154" t="s">
         <v>240</v>
       </c>
       <c r="C59" s="101">
@@ -3439,8 +3466,8 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="155"/>
-      <c r="B60" s="218" t="s">
+      <c r="A60" s="156"/>
+      <c r="B60" s="154" t="s">
         <v>241</v>
       </c>
       <c r="C60" s="101">
@@ -3456,8 +3483,8 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="155"/>
-      <c r="B61" s="218" t="s">
+      <c r="A61" s="156"/>
+      <c r="B61" s="154" t="s">
         <v>242</v>
       </c>
       <c r="C61" s="101">
@@ -3473,8 +3500,8 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="155"/>
-      <c r="B62" s="218" t="s">
+      <c r="A62" s="156"/>
+      <c r="B62" s="154" t="s">
         <v>243</v>
       </c>
       <c r="C62" s="101">
@@ -3490,8 +3517,8 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="155"/>
-      <c r="B63" s="218" t="s">
+      <c r="A63" s="156"/>
+      <c r="B63" s="154" t="s">
         <v>244</v>
       </c>
       <c r="C63" s="101">
@@ -3507,8 +3534,8 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="155"/>
-      <c r="B64" s="218" t="s">
+      <c r="A64" s="156"/>
+      <c r="B64" s="154" t="s">
         <v>235</v>
       </c>
       <c r="C64" s="101">
@@ -3524,7 +3551,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="155"/>
+      <c r="A65" s="156"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3535,7 +3562,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="155"/>
+      <c r="A66" s="156"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3546,7 +3573,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="155"/>
+      <c r="A67" s="156"/>
       <c r="B67" s="98" t="s">
         <v>187</v>
       </c>
@@ -3589,7 +3616,7 @@
     </row>
     <row r="69" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="154" t="s">
+      <c r="A70" s="155" t="s">
         <v>172</v>
       </c>
       <c r="B70" s="113" t="s">
@@ -3609,7 +3636,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="155"/>
+      <c r="A71" s="156"/>
       <c r="B71" s="98" t="s">
         <v>184</v>
       </c>
@@ -3626,8 +3653,8 @@
       <c r="F71" s="104"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="155"/>
-      <c r="B72" s="218" t="s">
+      <c r="A72" s="156"/>
+      <c r="B72" s="154" t="s">
         <v>245</v>
       </c>
       <c r="C72" s="101">
@@ -3643,8 +3670,8 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="155"/>
-      <c r="B73" s="218" t="s">
+      <c r="A73" s="156"/>
+      <c r="B73" s="154" t="s">
         <v>246</v>
       </c>
       <c r="C73" s="101">
@@ -3660,8 +3687,8 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="155"/>
-      <c r="B74" s="218" t="s">
+      <c r="A74" s="156"/>
+      <c r="B74" s="154" t="s">
         <v>235</v>
       </c>
       <c r="C74" s="101">
@@ -3677,7 +3704,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="155"/>
+      <c r="A75" s="156"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3688,7 +3715,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="155"/>
+      <c r="A76" s="156"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3699,7 +3726,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="155"/>
+      <c r="A77" s="156"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3710,7 +3737,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="155"/>
+      <c r="A78" s="156"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3721,7 +3748,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="155"/>
+      <c r="A79" s="156"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3732,7 +3759,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="155"/>
+      <c r="A80" s="156"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3743,7 +3770,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="155"/>
+      <c r="A81" s="156"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3754,7 +3781,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="155"/>
+      <c r="A82" s="156"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3765,7 +3792,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="155"/>
+      <c r="A83" s="156"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3776,7 +3803,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="155"/>
+      <c r="A84" s="156"/>
       <c r="B84" s="98" t="s">
         <v>187</v>
       </c>
@@ -3819,7 +3846,7 @@
     </row>
     <row r="86" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="157" t="s">
         <v>173</v>
       </c>
       <c r="B87" s="109" t="s">
@@ -3839,7 +3866,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="155"/>
+      <c r="A88" s="156"/>
       <c r="B88" s="98" t="s">
         <v>184</v>
       </c>
@@ -3856,8 +3883,8 @@
       <c r="F88" s="104"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="155"/>
-      <c r="B89" s="218" t="s">
+      <c r="A89" s="156"/>
+      <c r="B89" s="154" t="s">
         <v>245</v>
       </c>
       <c r="C89" s="101">
@@ -3873,29 +3900,41 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="155"/>
-      <c r="B90" s="100"/>
-      <c r="C90" s="101"/>
-      <c r="D90" s="101"/>
+      <c r="A90" s="156"/>
+      <c r="B90" s="219" t="s">
+        <v>237</v>
+      </c>
+      <c r="C90" s="101">
+        <v>19397</v>
+      </c>
+      <c r="D90" s="101">
+        <v>20538</v>
+      </c>
       <c r="E90" s="123">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1141</v>
       </c>
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="155"/>
-      <c r="B91" s="100"/>
-      <c r="C91" s="101"/>
-      <c r="D91" s="101"/>
+      <c r="A91" s="156"/>
+      <c r="B91" s="219" t="s">
+        <v>235</v>
+      </c>
+      <c r="C91" s="101">
+        <v>20883</v>
+      </c>
+      <c r="D91" s="101">
+        <v>22044</v>
+      </c>
       <c r="E91" s="123">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1161</v>
       </c>
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="155"/>
+      <c r="A92" s="156"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3906,7 +3945,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="155"/>
+      <c r="A93" s="156"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3917,7 +3956,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="155"/>
+      <c r="A94" s="156"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3928,7 +3967,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="155"/>
+      <c r="A95" s="156"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3939,7 +3978,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="155"/>
+      <c r="A96" s="156"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3950,7 +3989,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="155"/>
+      <c r="A97" s="156"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3961,7 +4000,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="155"/>
+      <c r="A98" s="156"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3972,7 +4011,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="155"/>
+      <c r="A99" s="156"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3983,7 +4022,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="155"/>
+      <c r="A100" s="156"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3994,21 +4033,25 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="155"/>
+      <c r="A101" s="156"/>
       <c r="B101" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="C101" s="99"/>
-      <c r="D101" s="99"/>
+      <c r="C101" s="99">
+        <v>21266</v>
+      </c>
+      <c r="D101" s="99">
+        <v>22427</v>
+      </c>
       <c r="E101" s="125">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1161</v>
       </c>
       <c r="F101" s="104"/>
     </row>
-    <row r="102" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="103" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="154" t="s">
+    <row r="102" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="155" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="113" t="s">
@@ -4027,87 +4070,125 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="155"/>
+    <row r="104" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="156"/>
       <c r="B104" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C104" s="99"/>
-      <c r="D104" s="99"/>
+      <c r="C104" s="99">
+        <v>21266</v>
+      </c>
+      <c r="D104" s="99">
+        <v>22427</v>
+      </c>
       <c r="E104" s="123">
         <f t="shared" ref="E104:E117" si="7">IF(AND(C104&gt;0,D104&gt;0), D104-C104, 0)</f>
-        <v>0</v>
+        <v>1161</v>
       </c>
       <c r="F104" s="104"/>
     </row>
-    <row r="105" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="155"/>
-      <c r="B105" s="100"/>
-      <c r="C105" s="101"/>
-      <c r="D105" s="101"/>
+    <row r="105" spans="1:6" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="156"/>
+      <c r="B105" s="219" t="s">
+        <v>245</v>
+      </c>
+      <c r="C105" s="101">
+        <v>21266</v>
+      </c>
+      <c r="D105" s="101">
+        <v>22427</v>
+      </c>
       <c r="E105" s="124">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1161</v>
       </c>
       <c r="F105" s="105"/>
     </row>
-    <row r="106" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="155"/>
-      <c r="B106" s="100"/>
-      <c r="C106" s="101"/>
-      <c r="D106" s="101"/>
+    <row r="106" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="156"/>
+      <c r="B106" s="219" t="s">
+        <v>247</v>
+      </c>
+      <c r="C106" s="101">
+        <v>22842</v>
+      </c>
+      <c r="D106" s="101">
+        <v>24009</v>
+      </c>
       <c r="E106" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1167</v>
       </c>
       <c r="F106" s="105"/>
     </row>
-    <row r="107" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="155"/>
-      <c r="B107" s="100"/>
-      <c r="C107" s="101"/>
-      <c r="D107" s="101"/>
+    <row r="107" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="156"/>
+      <c r="B107" s="219" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" s="101">
+        <v>23185</v>
+      </c>
+      <c r="D107" s="101">
+        <v>24353</v>
+      </c>
       <c r="E107" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1168</v>
       </c>
       <c r="F107" s="105"/>
     </row>
-    <row r="108" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="155"/>
-      <c r="B108" s="100"/>
-      <c r="C108" s="101"/>
-      <c r="D108" s="101"/>
+    <row r="108" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="156"/>
+      <c r="B108" s="219" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="101">
+        <v>23259</v>
+      </c>
+      <c r="D108" s="101">
+        <v>24427</v>
+      </c>
       <c r="E108" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1168</v>
       </c>
       <c r="F108" s="105"/>
     </row>
-    <row r="109" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="155"/>
-      <c r="B109" s="100"/>
-      <c r="C109" s="101"/>
-      <c r="D109" s="101"/>
+    <row r="109" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="156"/>
+      <c r="B109" s="219" t="s">
+        <v>250</v>
+      </c>
+      <c r="C109" s="101">
+        <v>23684</v>
+      </c>
+      <c r="D109" s="101">
+        <v>24851</v>
+      </c>
       <c r="E109" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1167</v>
       </c>
       <c r="F109" s="105"/>
     </row>
-    <row r="110" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="155"/>
-      <c r="B110" s="100"/>
+    <row r="110" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="156"/>
+      <c r="B110" s="219" t="s">
+        <v>251</v>
+      </c>
       <c r="C110" s="101"/>
-      <c r="D110" s="101"/>
+      <c r="D110" s="101">
+        <v>25089</v>
+      </c>
       <c r="E110" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F110" s="105"/>
     </row>
-    <row r="111" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="155"/>
+    <row r="111" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="156"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -4117,8 +4198,8 @@
       </c>
       <c r="F111" s="105"/>
     </row>
-    <row r="112" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="155"/>
+    <row r="112" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="156"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -4128,8 +4209,8 @@
       </c>
       <c r="F112" s="105"/>
     </row>
-    <row r="113" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="155"/>
+    <row r="113" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="156"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -4139,8 +4220,8 @@
       </c>
       <c r="F113" s="105"/>
     </row>
-    <row r="114" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="155"/>
+    <row r="114" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="156"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -4150,8 +4231,8 @@
       </c>
       <c r="F114" s="105"/>
     </row>
-    <row r="115" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="155"/>
+    <row r="115" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="156"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4161,8 +4242,8 @@
       </c>
       <c r="F115" s="105"/>
     </row>
-    <row r="116" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="155"/>
+    <row r="116" spans="1:6" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="156"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4172,8 +4253,8 @@
       </c>
       <c r="F116" s="105"/>
     </row>
-    <row r="117" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="155"/>
+    <row r="117" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="156"/>
       <c r="B117" s="98" t="s">
         <v>187</v>
       </c>
@@ -4185,9 +4266,9 @@
       </c>
       <c r="F117" s="104"/>
     </row>
-    <row r="118" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="118" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="119" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="156" t="s">
+      <c r="A119" s="157" t="s">
         <v>175</v>
       </c>
       <c r="B119" s="109" t="s">
@@ -4207,7 +4288,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="155"/>
+      <c r="A120" s="156"/>
       <c r="B120" s="98" t="s">
         <v>184</v>
       </c>
@@ -4220,7 +4301,7 @@
       <c r="F120" s="104"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="155"/>
+      <c r="A121" s="156"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4231,7 +4312,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="155"/>
+      <c r="A122" s="156"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4242,7 +4323,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="155"/>
+      <c r="A123" s="156"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4253,7 +4334,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="155"/>
+      <c r="A124" s="156"/>
       <c r="B124" s="100"/>
       <c r="C124" s="101"/>
       <c r="D124" s="101"/>
@@ -4264,7 +4345,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="155"/>
+      <c r="A125" s="156"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4275,7 +4356,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="155"/>
+      <c r="A126" s="156"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4286,7 +4367,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="155"/>
+      <c r="A127" s="156"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4297,7 +4378,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="155"/>
+      <c r="A128" s="156"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4308,7 +4389,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="155"/>
+      <c r="A129" s="156"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4319,7 +4400,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="155"/>
+      <c r="A130" s="156"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4330,7 +4411,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="155"/>
+      <c r="A131" s="156"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4341,7 +4422,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="155"/>
+      <c r="A132" s="156"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4352,7 +4433,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:6" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="155"/>
+      <c r="A133" s="156"/>
       <c r="B133" s="98" t="s">
         <v>187</v>
       </c>
@@ -4366,7 +4447,7 @@
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A135" s="154" t="s">
+      <c r="A135" s="155" t="s">
         <v>176</v>
       </c>
       <c r="B135" s="113" t="s">
@@ -4386,7 +4467,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="155"/>
+      <c r="A136" s="156"/>
       <c r="B136" s="98" t="s">
         <v>184</v>
       </c>
@@ -4399,7 +4480,7 @@
       <c r="F136" s="104"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="155"/>
+      <c r="A137" s="156"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4410,7 +4491,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A138" s="155"/>
+      <c r="A138" s="156"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4421,7 +4502,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A139" s="155"/>
+      <c r="A139" s="156"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4432,7 +4513,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A140" s="155"/>
+      <c r="A140" s="156"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4443,7 +4524,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A141" s="155"/>
+      <c r="A141" s="156"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4454,7 +4535,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="155"/>
+      <c r="A142" s="156"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4465,7 +4546,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A143" s="155"/>
+      <c r="A143" s="156"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4476,7 +4557,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="155"/>
+      <c r="A144" s="156"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4487,7 +4568,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="155"/>
+      <c r="A145" s="156"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4498,7 +4579,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="155"/>
+      <c r="A146" s="156"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4509,7 +4590,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="155"/>
+      <c r="A147" s="156"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4520,7 +4601,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:6" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="155"/>
+      <c r="A148" s="156"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4531,7 +4612,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="155"/>
+      <c r="A149" s="156"/>
       <c r="B149" s="98" t="s">
         <v>187</v>
       </c>
@@ -4546,6 +4627,11 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4554,11 +4640,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4590,13 +4671,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4626,18 +4707,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4789,9 +4870,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="165"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="166"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4942,9 +5023,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="168"/>
+      <c r="E38" s="168"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5095,9 +5176,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="163"/>
-      <c r="D55" s="164"/>
-      <c r="E55" s="164"/>
+      <c r="C55" s="167"/>
+      <c r="D55" s="168"/>
+      <c r="E55" s="168"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5248,9 +5329,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="163"/>
-      <c r="D72" s="164"/>
-      <c r="E72" s="164"/>
+      <c r="C72" s="167"/>
+      <c r="D72" s="168"/>
+      <c r="E72" s="168"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5401,9 +5482,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="163"/>
-      <c r="D89" s="164"/>
-      <c r="E89" s="164"/>
+      <c r="C89" s="167"/>
+      <c r="D89" s="168"/>
+      <c r="E89" s="168"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5554,9 +5635,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="163"/>
-      <c r="D106" s="164"/>
-      <c r="E106" s="164"/>
+      <c r="C106" s="167"/>
+      <c r="D106" s="168"/>
+      <c r="E106" s="168"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5707,9 +5788,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="163"/>
-      <c r="D123" s="164"/>
-      <c r="E123" s="164"/>
+      <c r="C123" s="167"/>
+      <c r="D123" s="168"/>
+      <c r="E123" s="168"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5860,9 +5941,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="163"/>
-      <c r="D140" s="164"/>
-      <c r="E140" s="164"/>
+      <c r="C140" s="167"/>
+      <c r="D140" s="168"/>
+      <c r="E140" s="168"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -6013,9 +6094,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="163"/>
-      <c r="D157" s="164"/>
-      <c r="E157" s="164"/>
+      <c r="C157" s="167"/>
+      <c r="D157" s="168"/>
+      <c r="E157" s="168"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6166,9 +6247,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="163"/>
-      <c r="D174" s="164"/>
-      <c r="E174" s="164"/>
+      <c r="C174" s="167"/>
+      <c r="D174" s="168"/>
+      <c r="E174" s="168"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6319,9 +6400,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="163"/>
-      <c r="D191" s="164"/>
-      <c r="E191" s="164"/>
+      <c r="C191" s="167"/>
+      <c r="D191" s="168"/>
+      <c r="E191" s="168"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6472,9 +6553,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="163"/>
-      <c r="D208" s="164"/>
-      <c r="E208" s="164"/>
+      <c r="C208" s="167"/>
+      <c r="D208" s="168"/>
+      <c r="E208" s="168"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6625,9 +6706,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="163"/>
-      <c r="D225" s="164"/>
-      <c r="E225" s="164"/>
+      <c r="C225" s="167"/>
+      <c r="D225" s="168"/>
+      <c r="E225" s="168"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6778,9 +6859,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="163"/>
-      <c r="D242" s="164"/>
-      <c r="E242" s="164"/>
+      <c r="C242" s="167"/>
+      <c r="D242" s="168"/>
+      <c r="E242" s="168"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6931,9 +7012,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="163"/>
-      <c r="D259" s="164"/>
-      <c r="E259" s="164"/>
+      <c r="C259" s="167"/>
+      <c r="D259" s="168"/>
+      <c r="E259" s="168"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7084,18 +7165,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="179"/>
-      <c r="D276" s="180"/>
-      <c r="E276" s="180"/>
+      <c r="C276" s="171"/>
+      <c r="D276" s="172"/>
+      <c r="E276" s="172"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="163"/>
-      <c r="D277" s="164"/>
-      <c r="E277" s="164"/>
+      <c r="C277" s="167"/>
+      <c r="D277" s="168"/>
+      <c r="E277" s="168"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7246,9 +7327,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="165"/>
-      <c r="D294" s="166"/>
-      <c r="E294" s="166"/>
+      <c r="C294" s="169"/>
+      <c r="D294" s="170"/>
+      <c r="E294" s="170"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7399,9 +7480,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="163"/>
-      <c r="D311" s="164"/>
-      <c r="E311" s="164"/>
+      <c r="C311" s="167"/>
+      <c r="D311" s="168"/>
+      <c r="E311" s="168"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7552,9 +7633,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="163"/>
-      <c r="D328" s="164"/>
-      <c r="E328" s="164"/>
+      <c r="C328" s="167"/>
+      <c r="D328" s="168"/>
+      <c r="E328" s="168"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7705,9 +7786,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="163"/>
-      <c r="D345" s="164"/>
-      <c r="E345" s="164"/>
+      <c r="C345" s="167"/>
+      <c r="D345" s="168"/>
+      <c r="E345" s="168"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7858,9 +7939,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="163"/>
-      <c r="D362" s="164"/>
-      <c r="E362" s="164"/>
+      <c r="C362" s="167"/>
+      <c r="D362" s="168"/>
+      <c r="E362" s="168"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -8011,9 +8092,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="163"/>
-      <c r="D379" s="164"/>
-      <c r="E379" s="164"/>
+      <c r="C379" s="167"/>
+      <c r="D379" s="168"/>
+      <c r="E379" s="168"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8164,9 +8245,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="163"/>
-      <c r="D396" s="164"/>
-      <c r="E396" s="164"/>
+      <c r="C396" s="167"/>
+      <c r="D396" s="168"/>
+      <c r="E396" s="168"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8317,9 +8398,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="163"/>
-      <c r="D413" s="164"/>
-      <c r="E413" s="164"/>
+      <c r="C413" s="167"/>
+      <c r="D413" s="168"/>
+      <c r="E413" s="168"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8470,9 +8551,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="163"/>
-      <c r="D430" s="164"/>
-      <c r="E430" s="164"/>
+      <c r="C430" s="167"/>
+      <c r="D430" s="168"/>
+      <c r="E430" s="168"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8623,9 +8704,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="163"/>
-      <c r="D447" s="164"/>
-      <c r="E447" s="164"/>
+      <c r="C447" s="167"/>
+      <c r="D447" s="168"/>
+      <c r="E447" s="168"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8776,9 +8857,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="163"/>
-      <c r="D464" s="164"/>
-      <c r="E464" s="164"/>
+      <c r="C464" s="167"/>
+      <c r="D464" s="168"/>
+      <c r="E464" s="168"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8929,9 +9010,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="163"/>
-      <c r="D481" s="164"/>
-      <c r="E481" s="164"/>
+      <c r="C481" s="167"/>
+      <c r="D481" s="168"/>
+      <c r="E481" s="168"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9082,9 +9163,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="163"/>
-      <c r="D498" s="164"/>
-      <c r="E498" s="164"/>
+      <c r="C498" s="167"/>
+      <c r="D498" s="168"/>
+      <c r="E498" s="168"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9235,9 +9316,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="163"/>
-      <c r="D515" s="164"/>
-      <c r="E515" s="164"/>
+      <c r="C515" s="167"/>
+      <c r="D515" s="168"/>
+      <c r="E515" s="168"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9388,9 +9469,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="163"/>
-      <c r="D532" s="164"/>
-      <c r="E532" s="164"/>
+      <c r="C532" s="167"/>
+      <c r="D532" s="168"/>
+      <c r="E532" s="168"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9541,18 +9622,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="177"/>
-      <c r="D549" s="178"/>
-      <c r="E549" s="178"/>
+      <c r="C549" s="173"/>
+      <c r="D549" s="174"/>
+      <c r="E549" s="174"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="163"/>
-      <c r="D550" s="164"/>
-      <c r="E550" s="164"/>
+      <c r="C550" s="167"/>
+      <c r="D550" s="168"/>
+      <c r="E550" s="168"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9703,9 +9784,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="165"/>
-      <c r="D567" s="166"/>
-      <c r="E567" s="166"/>
+      <c r="C567" s="169"/>
+      <c r="D567" s="170"/>
+      <c r="E567" s="170"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9856,9 +9937,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="163"/>
-      <c r="D584" s="164"/>
-      <c r="E584" s="164"/>
+      <c r="C584" s="167"/>
+      <c r="D584" s="168"/>
+      <c r="E584" s="168"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -10009,9 +10090,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="163"/>
-      <c r="D601" s="164"/>
-      <c r="E601" s="164"/>
+      <c r="C601" s="167"/>
+      <c r="D601" s="168"/>
+      <c r="E601" s="168"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10162,9 +10243,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="163"/>
-      <c r="D618" s="164"/>
-      <c r="E618" s="164"/>
+      <c r="C618" s="167"/>
+      <c r="D618" s="168"/>
+      <c r="E618" s="168"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10315,9 +10396,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="163"/>
-      <c r="D635" s="164"/>
-      <c r="E635" s="164"/>
+      <c r="C635" s="167"/>
+      <c r="D635" s="168"/>
+      <c r="E635" s="168"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10468,9 +10549,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="163"/>
-      <c r="D652" s="164"/>
-      <c r="E652" s="164"/>
+      <c r="C652" s="167"/>
+      <c r="D652" s="168"/>
+      <c r="E652" s="168"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10621,9 +10702,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="163"/>
-      <c r="D669" s="164"/>
-      <c r="E669" s="164"/>
+      <c r="C669" s="167"/>
+      <c r="D669" s="168"/>
+      <c r="E669" s="168"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10774,9 +10855,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="163"/>
-      <c r="D686" s="164"/>
-      <c r="E686" s="164"/>
+      <c r="C686" s="167"/>
+      <c r="D686" s="168"/>
+      <c r="E686" s="168"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10927,9 +11008,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="163"/>
-      <c r="D703" s="164"/>
-      <c r="E703" s="164"/>
+      <c r="C703" s="167"/>
+      <c r="D703" s="168"/>
+      <c r="E703" s="168"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11080,9 +11161,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="163"/>
-      <c r="D720" s="164"/>
-      <c r="E720" s="164"/>
+      <c r="C720" s="167"/>
+      <c r="D720" s="168"/>
+      <c r="E720" s="168"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11233,9 +11314,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="163"/>
-      <c r="D737" s="164"/>
-      <c r="E737" s="164"/>
+      <c r="C737" s="167"/>
+      <c r="D737" s="168"/>
+      <c r="E737" s="168"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11386,9 +11467,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="163"/>
-      <c r="D754" s="164"/>
-      <c r="E754" s="164"/>
+      <c r="C754" s="167"/>
+      <c r="D754" s="168"/>
+      <c r="E754" s="168"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11539,9 +11620,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="163"/>
-      <c r="D771" s="164"/>
-      <c r="E771" s="164"/>
+      <c r="C771" s="167"/>
+      <c r="D771" s="168"/>
+      <c r="E771" s="168"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11692,9 +11773,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="163"/>
-      <c r="D788" s="164"/>
-      <c r="E788" s="164"/>
+      <c r="C788" s="167"/>
+      <c r="D788" s="168"/>
+      <c r="E788" s="168"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11845,9 +11926,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="163"/>
-      <c r="D805" s="164"/>
-      <c r="E805" s="164"/>
+      <c r="C805" s="167"/>
+      <c r="D805" s="168"/>
+      <c r="E805" s="168"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -12007,9 +12088,9 @@
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="163"/>
-      <c r="D823" s="164"/>
-      <c r="E823" s="164"/>
+      <c r="C823" s="167"/>
+      <c r="D823" s="168"/>
+      <c r="E823" s="168"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12160,9 +12241,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="165"/>
-      <c r="D840" s="166"/>
-      <c r="E840" s="166"/>
+      <c r="C840" s="169"/>
+      <c r="D840" s="170"/>
+      <c r="E840" s="170"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12313,9 +12394,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="163"/>
-      <c r="D857" s="164"/>
-      <c r="E857" s="164"/>
+      <c r="C857" s="167"/>
+      <c r="D857" s="168"/>
+      <c r="E857" s="168"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12466,9 +12547,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="163"/>
-      <c r="D874" s="164"/>
-      <c r="E874" s="164"/>
+      <c r="C874" s="167"/>
+      <c r="D874" s="168"/>
+      <c r="E874" s="168"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12619,9 +12700,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="163"/>
-      <c r="D891" s="164"/>
-      <c r="E891" s="164"/>
+      <c r="C891" s="167"/>
+      <c r="D891" s="168"/>
+      <c r="E891" s="168"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12772,9 +12853,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="163"/>
-      <c r="D908" s="164"/>
-      <c r="E908" s="164"/>
+      <c r="C908" s="167"/>
+      <c r="D908" s="168"/>
+      <c r="E908" s="168"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12925,9 +13006,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="163"/>
-      <c r="D925" s="164"/>
-      <c r="E925" s="164"/>
+      <c r="C925" s="167"/>
+      <c r="D925" s="168"/>
+      <c r="E925" s="168"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13078,9 +13159,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="163"/>
-      <c r="D942" s="164"/>
-      <c r="E942" s="164"/>
+      <c r="C942" s="167"/>
+      <c r="D942" s="168"/>
+      <c r="E942" s="168"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13231,9 +13312,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="163"/>
-      <c r="D959" s="164"/>
-      <c r="E959" s="164"/>
+      <c r="C959" s="167"/>
+      <c r="D959" s="168"/>
+      <c r="E959" s="168"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13384,9 +13465,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="163"/>
-      <c r="D976" s="164"/>
-      <c r="E976" s="164"/>
+      <c r="C976" s="167"/>
+      <c r="D976" s="168"/>
+      <c r="E976" s="168"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13537,9 +13618,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="163"/>
-      <c r="D993" s="164"/>
-      <c r="E993" s="164"/>
+      <c r="C993" s="167"/>
+      <c r="D993" s="168"/>
+      <c r="E993" s="168"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13690,9 +13771,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="163"/>
-      <c r="D1010" s="164"/>
-      <c r="E1010" s="164"/>
+      <c r="C1010" s="167"/>
+      <c r="D1010" s="168"/>
+      <c r="E1010" s="168"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13843,9 +13924,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="163"/>
-      <c r="D1027" s="164"/>
-      <c r="E1027" s="164"/>
+      <c r="C1027" s="167"/>
+      <c r="D1027" s="168"/>
+      <c r="E1027" s="168"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13996,9 +14077,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="163"/>
-      <c r="D1044" s="164"/>
-      <c r="E1044" s="164"/>
+      <c r="C1044" s="167"/>
+      <c r="D1044" s="168"/>
+      <c r="E1044" s="168"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14149,9 +14230,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="163"/>
-      <c r="D1061" s="164"/>
-      <c r="E1061" s="164"/>
+      <c r="C1061" s="167"/>
+      <c r="D1061" s="168"/>
+      <c r="E1061" s="168"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14302,9 +14383,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="163"/>
-      <c r="D1078" s="164"/>
-      <c r="E1078" s="164"/>
+      <c r="C1078" s="167"/>
+      <c r="D1078" s="168"/>
+      <c r="E1078" s="168"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14455,18 +14536,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="173"/>
-      <c r="D1095" s="174"/>
-      <c r="E1095" s="174"/>
+      <c r="C1095" s="177"/>
+      <c r="D1095" s="178"/>
+      <c r="E1095" s="178"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="163"/>
-      <c r="D1096" s="164"/>
-      <c r="E1096" s="164"/>
+      <c r="C1096" s="167"/>
+      <c r="D1096" s="168"/>
+      <c r="E1096" s="168"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14617,9 +14698,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="165"/>
-      <c r="D1113" s="166"/>
-      <c r="E1113" s="166"/>
+      <c r="C1113" s="169"/>
+      <c r="D1113" s="170"/>
+      <c r="E1113" s="170"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14770,9 +14851,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="163"/>
-      <c r="D1130" s="164"/>
-      <c r="E1130" s="164"/>
+      <c r="C1130" s="167"/>
+      <c r="D1130" s="168"/>
+      <c r="E1130" s="168"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14923,9 +15004,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="163"/>
-      <c r="D1147" s="164"/>
-      <c r="E1147" s="164"/>
+      <c r="C1147" s="167"/>
+      <c r="D1147" s="168"/>
+      <c r="E1147" s="168"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15076,9 +15157,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="163"/>
-      <c r="D1164" s="164"/>
-      <c r="E1164" s="164"/>
+      <c r="C1164" s="167"/>
+      <c r="D1164" s="168"/>
+      <c r="E1164" s="168"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15229,9 +15310,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="163"/>
-      <c r="D1181" s="164"/>
-      <c r="E1181" s="164"/>
+      <c r="C1181" s="167"/>
+      <c r="D1181" s="168"/>
+      <c r="E1181" s="168"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15382,9 +15463,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="163"/>
-      <c r="D1198" s="164"/>
-      <c r="E1198" s="164"/>
+      <c r="C1198" s="167"/>
+      <c r="D1198" s="168"/>
+      <c r="E1198" s="168"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15535,9 +15616,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="163"/>
-      <c r="D1215" s="164"/>
-      <c r="E1215" s="164"/>
+      <c r="C1215" s="167"/>
+      <c r="D1215" s="168"/>
+      <c r="E1215" s="168"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15688,9 +15769,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="163"/>
-      <c r="D1232" s="164"/>
-      <c r="E1232" s="164"/>
+      <c r="C1232" s="167"/>
+      <c r="D1232" s="168"/>
+      <c r="E1232" s="168"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15841,9 +15922,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="163"/>
-      <c r="D1249" s="164"/>
-      <c r="E1249" s="164"/>
+      <c r="C1249" s="167"/>
+      <c r="D1249" s="168"/>
+      <c r="E1249" s="168"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15994,9 +16075,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="163"/>
-      <c r="D1266" s="164"/>
-      <c r="E1266" s="164"/>
+      <c r="C1266" s="167"/>
+      <c r="D1266" s="168"/>
+      <c r="E1266" s="168"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16147,9 +16228,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="163"/>
-      <c r="D1283" s="164"/>
-      <c r="E1283" s="164"/>
+      <c r="C1283" s="167"/>
+      <c r="D1283" s="168"/>
+      <c r="E1283" s="168"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16300,9 +16381,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="163"/>
-      <c r="D1300" s="164"/>
-      <c r="E1300" s="164"/>
+      <c r="C1300" s="167"/>
+      <c r="D1300" s="168"/>
+      <c r="E1300" s="168"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16453,9 +16534,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="163"/>
-      <c r="D1317" s="164"/>
-      <c r="E1317" s="164"/>
+      <c r="C1317" s="167"/>
+      <c r="D1317" s="168"/>
+      <c r="E1317" s="168"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16606,9 +16687,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="163"/>
-      <c r="D1334" s="164"/>
-      <c r="E1334" s="164"/>
+      <c r="C1334" s="167"/>
+      <c r="D1334" s="168"/>
+      <c r="E1334" s="168"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16759,9 +16840,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="163"/>
-      <c r="D1351" s="164"/>
-      <c r="E1351" s="164"/>
+      <c r="C1351" s="167"/>
+      <c r="D1351" s="168"/>
+      <c r="E1351" s="168"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16912,18 +16993,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="171"/>
-      <c r="D1368" s="172"/>
-      <c r="E1368" s="172"/>
+      <c r="C1368" s="179"/>
+      <c r="D1368" s="180"/>
+      <c r="E1368" s="180"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="163"/>
-      <c r="D1369" s="164"/>
-      <c r="E1369" s="164"/>
+      <c r="C1369" s="167"/>
+      <c r="D1369" s="168"/>
+      <c r="E1369" s="168"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17074,9 +17155,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="165"/>
-      <c r="D1386" s="166"/>
-      <c r="E1386" s="166"/>
+      <c r="C1386" s="169"/>
+      <c r="D1386" s="170"/>
+      <c r="E1386" s="170"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17227,9 +17308,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="163"/>
-      <c r="D1403" s="164"/>
-      <c r="E1403" s="164"/>
+      <c r="C1403" s="167"/>
+      <c r="D1403" s="168"/>
+      <c r="E1403" s="168"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17380,9 +17461,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="163"/>
-      <c r="D1420" s="164"/>
-      <c r="E1420" s="164"/>
+      <c r="C1420" s="167"/>
+      <c r="D1420" s="168"/>
+      <c r="E1420" s="168"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17533,9 +17614,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="163"/>
-      <c r="D1437" s="164"/>
-      <c r="E1437" s="164"/>
+      <c r="C1437" s="167"/>
+      <c r="D1437" s="168"/>
+      <c r="E1437" s="168"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17686,9 +17767,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="163"/>
-      <c r="D1454" s="164"/>
-      <c r="E1454" s="164"/>
+      <c r="C1454" s="167"/>
+      <c r="D1454" s="168"/>
+      <c r="E1454" s="168"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17839,9 +17920,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="163"/>
-      <c r="D1471" s="164"/>
-      <c r="E1471" s="164"/>
+      <c r="C1471" s="167"/>
+      <c r="D1471" s="168"/>
+      <c r="E1471" s="168"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17992,9 +18073,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="163"/>
-      <c r="D1488" s="164"/>
-      <c r="E1488" s="164"/>
+      <c r="C1488" s="167"/>
+      <c r="D1488" s="168"/>
+      <c r="E1488" s="168"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18145,9 +18226,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="163"/>
-      <c r="D1505" s="164"/>
-      <c r="E1505" s="164"/>
+      <c r="C1505" s="167"/>
+      <c r="D1505" s="168"/>
+      <c r="E1505" s="168"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18298,9 +18379,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="163"/>
-      <c r="D1522" s="164"/>
-      <c r="E1522" s="164"/>
+      <c r="C1522" s="167"/>
+      <c r="D1522" s="168"/>
+      <c r="E1522" s="168"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18451,9 +18532,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="163"/>
-      <c r="D1539" s="164"/>
-      <c r="E1539" s="164"/>
+      <c r="C1539" s="167"/>
+      <c r="D1539" s="168"/>
+      <c r="E1539" s="168"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18604,9 +18685,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="163"/>
-      <c r="D1556" s="164"/>
-      <c r="E1556" s="164"/>
+      <c r="C1556" s="167"/>
+      <c r="D1556" s="168"/>
+      <c r="E1556" s="168"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18757,9 +18838,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="163"/>
-      <c r="D1573" s="164"/>
-      <c r="E1573" s="164"/>
+      <c r="C1573" s="167"/>
+      <c r="D1573" s="168"/>
+      <c r="E1573" s="168"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18910,9 +18991,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="163"/>
-      <c r="D1590" s="164"/>
-      <c r="E1590" s="164"/>
+      <c r="C1590" s="167"/>
+      <c r="D1590" s="168"/>
+      <c r="E1590" s="168"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19063,9 +19144,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="163"/>
-      <c r="D1607" s="164"/>
-      <c r="E1607" s="164"/>
+      <c r="C1607" s="167"/>
+      <c r="D1607" s="168"/>
+      <c r="E1607" s="168"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19216,9 +19297,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="163"/>
-      <c r="D1624" s="164"/>
-      <c r="E1624" s="164"/>
+      <c r="C1624" s="167"/>
+      <c r="D1624" s="168"/>
+      <c r="E1624" s="168"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19369,18 +19450,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="169"/>
-      <c r="D1641" s="170"/>
-      <c r="E1641" s="170"/>
+      <c r="C1641" s="181"/>
+      <c r="D1641" s="182"/>
+      <c r="E1641" s="182"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="163"/>
-      <c r="D1642" s="164"/>
-      <c r="E1642" s="164"/>
+      <c r="C1642" s="167"/>
+      <c r="D1642" s="168"/>
+      <c r="E1642" s="168"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19531,9 +19612,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="165"/>
-      <c r="D1659" s="166"/>
-      <c r="E1659" s="166"/>
+      <c r="C1659" s="169"/>
+      <c r="D1659" s="170"/>
+      <c r="E1659" s="170"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19684,9 +19765,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="163"/>
-      <c r="D1676" s="164"/>
-      <c r="E1676" s="164"/>
+      <c r="C1676" s="167"/>
+      <c r="D1676" s="168"/>
+      <c r="E1676" s="168"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19837,9 +19918,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="163"/>
-      <c r="D1693" s="164"/>
-      <c r="E1693" s="164"/>
+      <c r="C1693" s="167"/>
+      <c r="D1693" s="168"/>
+      <c r="E1693" s="168"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19990,9 +20071,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="163"/>
-      <c r="D1710" s="164"/>
-      <c r="E1710" s="164"/>
+      <c r="C1710" s="167"/>
+      <c r="D1710" s="168"/>
+      <c r="E1710" s="168"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20143,9 +20224,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="163"/>
-      <c r="D1727" s="164"/>
-      <c r="E1727" s="164"/>
+      <c r="C1727" s="167"/>
+      <c r="D1727" s="168"/>
+      <c r="E1727" s="168"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20296,9 +20377,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="163"/>
-      <c r="D1744" s="164"/>
-      <c r="E1744" s="164"/>
+      <c r="C1744" s="167"/>
+      <c r="D1744" s="168"/>
+      <c r="E1744" s="168"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20449,9 +20530,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="163"/>
-      <c r="D1761" s="164"/>
-      <c r="E1761" s="164"/>
+      <c r="C1761" s="167"/>
+      <c r="D1761" s="168"/>
+      <c r="E1761" s="168"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20602,9 +20683,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="163"/>
-      <c r="D1778" s="164"/>
-      <c r="E1778" s="164"/>
+      <c r="C1778" s="167"/>
+      <c r="D1778" s="168"/>
+      <c r="E1778" s="168"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20755,9 +20836,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="163"/>
-      <c r="D1795" s="164"/>
-      <c r="E1795" s="164"/>
+      <c r="C1795" s="167"/>
+      <c r="D1795" s="168"/>
+      <c r="E1795" s="168"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20908,9 +20989,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="163"/>
-      <c r="D1812" s="164"/>
-      <c r="E1812" s="164"/>
+      <c r="C1812" s="167"/>
+      <c r="D1812" s="168"/>
+      <c r="E1812" s="168"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21061,9 +21142,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="163"/>
-      <c r="D1829" s="164"/>
-      <c r="E1829" s="164"/>
+      <c r="C1829" s="167"/>
+      <c r="D1829" s="168"/>
+      <c r="E1829" s="168"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21214,9 +21295,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="163"/>
-      <c r="D1846" s="164"/>
-      <c r="E1846" s="164"/>
+      <c r="C1846" s="167"/>
+      <c r="D1846" s="168"/>
+      <c r="E1846" s="168"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21367,9 +21448,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="163"/>
-      <c r="D1863" s="164"/>
-      <c r="E1863" s="164"/>
+      <c r="C1863" s="167"/>
+      <c r="D1863" s="168"/>
+      <c r="E1863" s="168"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21520,9 +21601,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="163"/>
-      <c r="D1880" s="164"/>
-      <c r="E1880" s="164"/>
+      <c r="C1880" s="167"/>
+      <c r="D1880" s="168"/>
+      <c r="E1880" s="168"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21673,9 +21754,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="163"/>
-      <c r="D1897" s="164"/>
-      <c r="E1897" s="164"/>
+      <c r="C1897" s="167"/>
+      <c r="D1897" s="168"/>
+      <c r="E1897" s="168"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21826,18 +21907,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="167"/>
-      <c r="D1914" s="168"/>
-      <c r="E1914" s="168"/>
+      <c r="C1914" s="183"/>
+      <c r="D1914" s="184"/>
+      <c r="E1914" s="184"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="163"/>
-      <c r="D1915" s="164"/>
-      <c r="E1915" s="164"/>
+      <c r="C1915" s="167"/>
+      <c r="D1915" s="168"/>
+      <c r="E1915" s="168"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21988,9 +22069,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="165"/>
-      <c r="D1932" s="166"/>
-      <c r="E1932" s="166"/>
+      <c r="C1932" s="169"/>
+      <c r="D1932" s="170"/>
+      <c r="E1932" s="170"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22141,9 +22222,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="163"/>
-      <c r="D1949" s="164"/>
-      <c r="E1949" s="164"/>
+      <c r="C1949" s="167"/>
+      <c r="D1949" s="168"/>
+      <c r="E1949" s="168"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22294,9 +22375,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="163"/>
-      <c r="D1966" s="164"/>
-      <c r="E1966" s="164"/>
+      <c r="C1966" s="167"/>
+      <c r="D1966" s="168"/>
+      <c r="E1966" s="168"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22447,9 +22528,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="163"/>
-      <c r="D1983" s="164"/>
-      <c r="E1983" s="164"/>
+      <c r="C1983" s="167"/>
+      <c r="D1983" s="168"/>
+      <c r="E1983" s="168"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22600,9 +22681,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="163"/>
-      <c r="D2000" s="164"/>
-      <c r="E2000" s="164"/>
+      <c r="C2000" s="167"/>
+      <c r="D2000" s="168"/>
+      <c r="E2000" s="168"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22753,9 +22834,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="163"/>
-      <c r="D2017" s="164"/>
-      <c r="E2017" s="164"/>
+      <c r="C2017" s="167"/>
+      <c r="D2017" s="168"/>
+      <c r="E2017" s="168"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22906,9 +22987,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="163"/>
-      <c r="D2034" s="164"/>
-      <c r="E2034" s="164"/>
+      <c r="C2034" s="167"/>
+      <c r="D2034" s="168"/>
+      <c r="E2034" s="168"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23059,9 +23140,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="163"/>
-      <c r="D2051" s="164"/>
-      <c r="E2051" s="164"/>
+      <c r="C2051" s="167"/>
+      <c r="D2051" s="168"/>
+      <c r="E2051" s="168"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23212,9 +23293,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="163"/>
-      <c r="D2068" s="164"/>
-      <c r="E2068" s="164"/>
+      <c r="C2068" s="167"/>
+      <c r="D2068" s="168"/>
+      <c r="E2068" s="168"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23365,9 +23446,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="163"/>
-      <c r="D2085" s="164"/>
-      <c r="E2085" s="164"/>
+      <c r="C2085" s="167"/>
+      <c r="D2085" s="168"/>
+      <c r="E2085" s="168"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23518,9 +23599,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="163"/>
-      <c r="D2102" s="164"/>
-      <c r="E2102" s="164"/>
+      <c r="C2102" s="167"/>
+      <c r="D2102" s="168"/>
+      <c r="E2102" s="168"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23671,9 +23752,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="163"/>
-      <c r="D2119" s="164"/>
-      <c r="E2119" s="164"/>
+      <c r="C2119" s="167"/>
+      <c r="D2119" s="168"/>
+      <c r="E2119" s="168"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23824,9 +23905,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="163"/>
-      <c r="D2136" s="164"/>
-      <c r="E2136" s="164"/>
+      <c r="C2136" s="167"/>
+      <c r="D2136" s="168"/>
+      <c r="E2136" s="168"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23977,9 +24058,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="163"/>
-      <c r="D2153" s="164"/>
-      <c r="E2153" s="164"/>
+      <c r="C2153" s="167"/>
+      <c r="D2153" s="168"/>
+      <c r="E2153" s="168"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24130,9 +24211,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="163"/>
-      <c r="D2170" s="164"/>
-      <c r="E2170" s="164"/>
+      <c r="C2170" s="167"/>
+      <c r="D2170" s="168"/>
+      <c r="E2170" s="168"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24280,26 +24361,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24312,113 +24478,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24443,51 +24524,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="191" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
-      <c r="K1" s="190"/>
-      <c r="L1" s="190"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="188" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="188"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
-      <c r="K2" s="188"/>
-      <c r="L2" s="189"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
+      <c r="L2" s="190"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="185"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="186"/>
+      <c r="F3" s="186"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="186"/>
+      <c r="K3" s="187"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24704,19 +24785,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="184" t="s">
+      <c r="A20" s="185" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="185"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="185"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="185"/>
-      <c r="G20" s="185"/>
-      <c r="H20" s="185"/>
-      <c r="I20" s="185"/>
-      <c r="J20" s="185"/>
-      <c r="K20" s="186"/>
+      <c r="B20" s="186"/>
+      <c r="C20" s="186"/>
+      <c r="D20" s="186"/>
+      <c r="E20" s="186"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="186"/>
+      <c r="K20" s="187"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24933,19 +25014,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="184" t="s">
+      <c r="A37" s="185" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="185"/>
-      <c r="C37" s="185"/>
-      <c r="D37" s="185"/>
-      <c r="E37" s="185"/>
-      <c r="F37" s="185"/>
-      <c r="G37" s="185"/>
-      <c r="H37" s="185"/>
-      <c r="I37" s="185"/>
-      <c r="J37" s="185"/>
-      <c r="K37" s="186"/>
+      <c r="B37" s="186"/>
+      <c r="C37" s="186"/>
+      <c r="D37" s="186"/>
+      <c r="E37" s="186"/>
+      <c r="F37" s="186"/>
+      <c r="G37" s="186"/>
+      <c r="H37" s="186"/>
+      <c r="I37" s="186"/>
+      <c r="J37" s="186"/>
+      <c r="K37" s="187"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -25169,7 +25250,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25203,28 +25284,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="191"/>
+      <c r="A3" s="192"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="192"/>
+      <c r="A4" s="193"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="192"/>
+      <c r="A5" s="193"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="192"/>
+      <c r="A6" s="193"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="192"/>
+      <c r="A7" s="193"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="192"/>
+      <c r="A8" s="193"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="192"/>
+      <c r="A9" s="193"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="193"/>
+      <c r="A10" s="194"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25380,7 +25461,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25407,10 +25488,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="194" t="s">
+      <c r="B1" s="195" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="195"/>
+      <c r="C1" s="196"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25421,7 +25502,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="197" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25435,7 +25516,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="197"/>
+      <c r="A4" s="198"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25447,7 +25528,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="197"/>
+      <c r="A5" s="198"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25456,31 +25537,31 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="197"/>
+      <c r="A6" s="198"/>
       <c r="B6" s="139" t="s">
         <v>212</v>
       </c>
-      <c r="C6" s="134">
+      <c r="C6" s="134" t="str">
         <f>FrameCounts!H2</f>
-        <v>18.95</v>
+        <v xml:space="preserve">  </v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="197"/>
+      <c r="A7" s="198"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="135">
+      <c r="C7" s="135" t="e">
         <f>C6/60</f>
-        <v>0.3158333333333333</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="197"/>
+      <c r="A8" s="198"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25489,7 +25570,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="198"/>
+      <c r="A9" s="199"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25504,7 +25585,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="196" t="s">
+      <c r="A11" s="197" t="s">
         <v>211</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25518,7 +25599,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="197"/>
+      <c r="A12" s="198"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25530,7 +25611,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="197"/>
+      <c r="A13" s="198"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25539,7 +25620,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="197"/>
+      <c r="A14" s="198"/>
       <c r="B14" s="139" t="s">
         <v>212</v>
       </c>
@@ -25551,7 +25632,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="197"/>
+      <c r="A15" s="198"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25563,7 +25644,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="197"/>
+      <c r="A16" s="198"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25572,7 +25653,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="198"/>
+      <c r="A17" s="199"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25587,7 +25668,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="196" t="s">
+      <c r="A19" s="197" t="s">
         <v>211</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25596,7 +25677,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="197"/>
+      <c r="A20" s="198"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25606,14 +25687,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="197"/>
+      <c r="A21" s="198"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="197"/>
+      <c r="A22" s="198"/>
       <c r="B22" s="139" t="s">
         <v>212</v>
       </c>
@@ -25623,7 +25704,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="197"/>
+      <c r="A23" s="198"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25633,14 +25714,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="197"/>
+      <c r="A24" s="198"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="198"/>
+      <c r="A25" s="199"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25653,7 +25734,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25675,163 +25756,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="210" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="209"/>
+      <c r="B1" s="211"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="205" t="s">
+      <c r="A2" s="216" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="206"/>
+      <c r="B2" s="217"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="218" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="206"/>
+      <c r="B3" s="217"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="212"/>
-      <c r="B4" s="213"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="215"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="210" t="s">
+      <c r="A5" s="212" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="211"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="204" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="217"/>
+      <c r="B7" s="205"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="214" t="s">
+      <c r="A9" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="215"/>
+      <c r="B9" s="207"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202"/>
+      <c r="A10" s="208"/>
+      <c r="B10" s="209"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="203" t="s">
+      <c r="A11" s="200" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="204"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="203" t="s">
+      <c r="A12" s="200" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="204"/>
+      <c r="B12" s="201"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="203" t="s">
+      <c r="A13" s="200" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="204"/>
+      <c r="B13" s="201"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="203" t="s">
+      <c r="A14" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="204"/>
+      <c r="B14" s="201"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="204"/>
+      <c r="B15" s="201"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="203" t="s">
+      <c r="A16" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="204"/>
+      <c r="B16" s="201"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="202" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="200"/>
+      <c r="B17" s="203"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="216" t="s">
+      <c r="A19" s="204" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="217"/>
+      <c r="B19" s="205"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="214" t="s">
+      <c r="A21" s="206" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="215"/>
+      <c r="B21" s="207"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="201"/>
-      <c r="B22" s="202"/>
+      <c r="A22" s="208"/>
+      <c r="B22" s="209"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="203" t="s">
+      <c r="A23" s="200" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="204"/>
+      <c r="B23" s="201"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="203"/>
-      <c r="B24" s="204"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="200" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="204"/>
+      <c r="B25" s="201"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="203" t="s">
+      <c r="A26" s="200" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="204"/>
+      <c r="B26" s="201"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25842,6 +25910,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>